<commit_message>
Update 'convert' notebook with sessions/assignment pages, generate pages
</commit_message>
<xml_diff>
--- a/book.xlsx
+++ b/book.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sjgar\Documents\RPI\clubs and activities\Metallography\course-intro-ml-app\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B924A501-0F8C-49D1-B0AC-D389062D66B8}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16429FD4-3C85-4D66-8D85-21AD94A93178}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12696" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12696" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Configuration" sheetId="1" r:id="rId1"/>
@@ -24,8 +24,8 @@
     <sheet name="schedule_md" sheetId="3" state="hidden" r:id="rId9"/>
     <sheet name="readings_md" sheetId="20" state="hidden" r:id="rId10"/>
     <sheet name="notebooks_md" sheetId="12" state="hidden" r:id="rId11"/>
-    <sheet name="assignments_md" sheetId="13" state="hidden" r:id="rId12"/>
-    <sheet name="session_md" sheetId="4" r:id="rId13"/>
+    <sheet name="assignments_md" sheetId="13" r:id="rId12"/>
+    <sheet name="session_md" sheetId="4" state="hidden" r:id="rId13"/>
     <sheet name="assign_md" sheetId="23" r:id="rId14"/>
     <sheet name="grading_md" sheetId="15" state="hidden" r:id="rId15"/>
     <sheet name="AcademicCalendar" sheetId="5" state="hidden" r:id="rId16"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4076" uniqueCount="875">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4105" uniqueCount="875">
   <si>
     <t>MGMT6560-fa19</t>
   </si>
@@ -3209,6 +3209,8 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -3234,8 +3236,6 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -3672,23 +3672,23 @@
       <c r="A14" s="24" t="s">
         <v>696</v>
       </c>
-      <c r="B14" s="89" t="s">
+      <c r="B14" s="91" t="s">
         <v>698</v>
       </c>
-      <c r="C14" s="89"/>
-      <c r="D14" s="89"/>
-      <c r="E14" s="89"/>
+      <c r="C14" s="91"/>
+      <c r="D14" s="91"/>
+      <c r="E14" s="91"/>
     </row>
     <row r="15" spans="1:5" s="4" customFormat="1" ht="99" customHeight="1">
       <c r="A15" s="24" t="s">
         <v>706</v>
       </c>
-      <c r="B15" s="89" t="s">
+      <c r="B15" s="91" t="s">
         <v>707</v>
       </c>
-      <c r="C15" s="89"/>
-      <c r="D15" s="89"/>
-      <c r="E15" s="89"/>
+      <c r="C15" s="91"/>
+      <c r="D15" s="91"/>
+      <c r="E15" s="91"/>
     </row>
     <row r="16" spans="1:5" s="4" customFormat="1" ht="15" customHeight="1">
       <c r="A16" s="1"/>
@@ -4456,7 +4456,7 @@
   <dimension ref="A1:A36"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="15.6"/>
@@ -4494,7 +4494,7 @@
     <row r="6" spans="1:1">
       <c r="A6" s="40" t="str">
         <f>IF(ISBLANK(Schedule!H5),"",CONCATENATE("| ",Schedule!H5," | [",Schedule!B5,"](",Configuration!B$20,Configuration!B$19,"/sessions/session",Schedule!B5,"/) | ",TEXT(Schedule!D5+Configuration!$B$6, "mm/dd")," | ",Schedule!I5," | ",IF(ISBLANK(Schedule!K5),"*None*",Schedule!R5)," |"))</f>
-        <v>| 1 | [2](https://rpi-data.github.io/course-intro-ml-app/sessions/session2/) | 09/17 | This introductory assignment introduces the basics of loading files from a variety of formats.  | [Link](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/02-intro-python/hm-01/hm01.ipynb) |</v>
+        <v>| 1 | [2](https://rpi-data.github.io/course-intro-ml-app/sessions/session2/) | 09/17 | This introductory assignment introduces the basics of loading files from a variety of formats.  | [Assignment 1](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/02-intro-python/hm-01/hm01.ipynb) |</v>
       </c>
     </row>
     <row r="7" spans="1:1">
@@ -4512,7 +4512,7 @@
     <row r="9" spans="1:1">
       <c r="A9" s="40" t="str">
         <f>IF(ISBLANK(Schedule!H8),"",CONCATENATE("| ",Schedule!H8," | [",Schedule!B8,"](",Configuration!B$20,Configuration!B$19,"/sessions/session",Schedule!B8,"/) | ",TEXT(Schedule!D8+Configuration!$B$6, "mm/dd")," | ",Schedule!I8," | ",IF(ISBLANK(Schedule!K8),"*None*",Schedule!R8)," |"))</f>
-        <v>| 2 | [5](https://rpi-data.github.io/course-intro-ml-app/sessions/session5/) | 09/26 |  | [Link](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/03-python/hm-02/hm02.ipynb) |</v>
+        <v>| 2 | [5](https://rpi-data.github.io/course-intro-ml-app/sessions/session5/) | 09/26 |  | [Assignment 2](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/03-python/hm-02/hm02.ipynb) |</v>
       </c>
     </row>
     <row r="10" spans="1:1">
@@ -4524,7 +4524,7 @@
     <row r="11" spans="1:1">
       <c r="A11" s="40" t="str">
         <f>IF(ISBLANK(Schedule!H10),"",CONCATENATE("| ",Schedule!H10," | [",Schedule!B10,"](",Configuration!B$20,Configuration!B$19,"/sessions/session",Schedule!B10,"/) | ",TEXT(Schedule!D10+Configuration!$B$6, "mm/dd")," | ",Schedule!I10," | ",IF(ISBLANK(Schedule!K10),"*None*",Schedule!R10)," |"))</f>
-        <v>| 3 | [7](https://rpi-data.github.io/course-intro-ml-app/sessions/session7/) | 10/03 |  | [Link](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/04-viz-api-scraper/hm-03/hm03.ipynb) |</v>
+        <v>| 3 | [7](https://rpi-data.github.io/course-intro-ml-app/sessions/session7/) | 10/03 |  | [Assignment 3](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/04-viz-api-scraper/hm-03/hm03.ipynb) |</v>
       </c>
     </row>
     <row r="12" spans="1:1">
@@ -4687,35 +4687,40 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:G33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.09765625" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="45" style="3" customWidth="1"/>
-    <col min="2" max="2" width="8" style="3" customWidth="1"/>
-    <col min="3" max="4" width="45" style="3" customWidth="1"/>
-    <col min="5" max="16384" width="11.09765625" style="3"/>
+    <col min="1" max="1" width="11.09765625" style="42"/>
+    <col min="2" max="2" width="45" style="3" customWidth="1"/>
+    <col min="3" max="3" width="8" style="3" customWidth="1"/>
+    <col min="4" max="5" width="45" style="3" customWidth="1"/>
+    <col min="6" max="16384" width="11.09765625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.6">
-      <c r="A1" s="11"/>
-      <c r="B1" s="11" t="s">
+    <row r="1" spans="1:7" ht="15.6">
+      <c r="B1" s="11"/>
+      <c r="C1" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="C1" s="11" t="s">
+      <c r="D1" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="D1" s="11" t="s">
+      <c r="E1" s="11" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="120" customHeight="1">
-      <c r="A2" s="21" t="str">
-        <f>CONCATENATE(C2,D2)</f>
+    <row r="2" spans="1:7" ht="15" customHeight="1">
+      <c r="A2" s="42" t="str">
+        <f>IF(ISBLANK(Schedule!B3),"",CONCATENATE("session",Schedule!B3))</f>
+        <v>session1</v>
+      </c>
+      <c r="B2" s="21" t="str">
+        <f>CONCATENATE(D2,E2)</f>
         <v>&lt;h1 style="font-family: Verdana, Geneva, sans-serif; text-align:center"&gt;Course Overview &amp; Introduction to the Data Science Lifecycle&lt;/h1&gt;
 ---
 ### Description
@@ -4728,16 +4733,16 @@
 ### Notebooks
 [Check here](https://rpi-data.github.io/course-intro-ml-app/sessions/assignments/)</v>
       </c>
-      <c r="B2" s="12" t="s">
+      <c r="C2" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="C2" s="3" t="str">
+      <c r="D2" s="3" t="str">
         <f>CONCATENATE("&lt;h1 style="&amp;CHAR(34)&amp;"font-family: Verdana, Geneva, sans-serif; text-align:center"&amp;CHAR(34)&amp;"&gt;",Schedule!E3,"&lt;/h1&gt;
 ---")</f>
         <v>&lt;h1 style="font-family: Verdana, Geneva, sans-serif; text-align:center"&gt;Course Overview &amp; Introduction to the Data Science Lifecycle&lt;/h1&gt;
 ---</v>
       </c>
-      <c r="D2" s="11" t="str">
+      <c r="E2" s="11" t="str">
         <f>CONCATENATE("
 ### Description
 ",IF(ISBLANK(Schedule!F3),"*None*",Schedule!F3),"
@@ -4758,11 +4763,15 @@
 ### Notebooks
 [Check here](https://rpi-data.github.io/course-intro-ml-app/sessions/assignments/)</v>
       </c>
-      <c r="F2" s="41"/>
-    </row>
-    <row r="3" spans="1:6" ht="120" customHeight="1">
-      <c r="A3" s="21" t="str">
-        <f>CONCATENATE(C3,D3)</f>
+      <c r="G2" s="41"/>
+    </row>
+    <row r="3" spans="1:7" ht="15" customHeight="1">
+      <c r="A3" s="42" t="str">
+        <f>IF(ISBLANK(Schedule!B4),"",CONCATENATE("session",Schedule!B4))</f>
+        <v/>
+      </c>
+      <c r="B3" s="21" t="str">
+        <f t="shared" ref="B3:B5" si="0">CONCATENATE(D3,E3)</f>
         <v>&lt;h1 style="font-family: Verdana, Geneva, sans-serif; text-align:center"&gt;Labor Day - no classes (Tuesday follows Monday schedule)&lt;/h1&gt;
 ---
 ### Description
@@ -4774,16 +4783,16 @@
 ### Notebooks
 *None*</v>
       </c>
-      <c r="B3" s="12" t="s">
+      <c r="C3" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="C3" s="42" t="str">
+      <c r="D3" s="42" t="str">
         <f>CONCATENATE("&lt;h1 style="&amp;CHAR(34)&amp;"font-family: Verdana, Geneva, sans-serif; text-align:center"&amp;CHAR(34)&amp;"&gt;",Schedule!E4,"&lt;/h1&gt;
 ---")</f>
         <v>&lt;h1 style="font-family: Verdana, Geneva, sans-serif; text-align:center"&gt;Labor Day - no classes (Tuesday follows Monday schedule)&lt;/h1&gt;
 ---</v>
       </c>
-      <c r="D3" s="11" t="str">
+      <c r="E3" s="11" t="str">
         <f>CONCATENATE("
 ### Description
 ",IF(ISBLANK(Schedule!F4),"*None*",Schedule!F4),"
@@ -4804,9 +4813,13 @@
 *None*</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="120" customHeight="1">
-      <c r="A4" s="21" t="str">
-        <f>CONCATENATE(C4,D4)</f>
+    <row r="4" spans="1:7" ht="15" customHeight="1">
+      <c r="A4" s="42" t="str">
+        <f>IF(ISBLANK(Schedule!B5),"",CONCATENATE("session",Schedule!B5))</f>
+        <v>session2</v>
+      </c>
+      <c r="B4" s="21" t="str">
+        <f t="shared" si="0"/>
         <v>&lt;h1 style="font-family: Verdana, Geneva, sans-serif; text-align:center"&gt;Python Basics&lt;/h1&gt;
 ---
 ### Description
@@ -4820,16 +4833,16 @@
 ### Notebooks
 [Check here](https://rpi-data.github.io/course-intro-ml-app/sessions/assignments/)</v>
       </c>
-      <c r="B4" s="12" t="s">
+      <c r="C4" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="C4" s="42" t="str">
+      <c r="D4" s="42" t="str">
         <f>CONCATENATE("&lt;h1 style="&amp;CHAR(34)&amp;"font-family: Verdana, Geneva, sans-serif; text-align:center"&amp;CHAR(34)&amp;"&gt;",Schedule!E5,"&lt;/h1&gt;
 ---")</f>
         <v>&lt;h1 style="font-family: Verdana, Geneva, sans-serif; text-align:center"&gt;Python Basics&lt;/h1&gt;
 ---</v>
       </c>
-      <c r="D4" s="11" t="str">
+      <c r="E4" s="11" t="str">
         <f>CONCATENATE("
 ### Description
 ",IF(ISBLANK(Schedule!F5),"*None*",Schedule!F5),"
@@ -4851,7 +4864,1399 @@
 ### Notebooks
 [Check here](https://rpi-data.github.io/course-intro-ml-app/sessions/assignments/)</v>
       </c>
-      <c r="E4" s="42"/>
+      <c r="F4" s="42"/>
+    </row>
+    <row r="5" spans="1:7" ht="15" customHeight="1">
+      <c r="A5" s="42" t="str">
+        <f>IF(ISBLANK(Schedule!B6),"",CONCATENATE("session",Schedule!B6))</f>
+        <v>session3</v>
+      </c>
+      <c r="B5" s="21" t="str">
+        <f t="shared" si="0"/>
+        <v>&lt;h1 style="font-family: Verdana, Geneva, sans-serif; text-align:center"&gt;Python Basics&lt;/h1&gt;
+---
+### Description
+Lab/homework
+### Learning Objectives
+*None*
+### Readings
+*None*
+### Notebooks
+*None*</v>
+      </c>
+      <c r="C5" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="D5" s="42" t="str">
+        <f>CONCATENATE("&lt;h1 style="&amp;CHAR(34)&amp;"font-family: Verdana, Geneva, sans-serif; text-align:center"&amp;CHAR(34)&amp;"&gt;",Schedule!E6,"&lt;/h1&gt;
+---")</f>
+        <v>&lt;h1 style="font-family: Verdana, Geneva, sans-serif; text-align:center"&gt;Python Basics&lt;/h1&gt;
+---</v>
+      </c>
+      <c r="E5" s="11" t="str">
+        <f>CONCATENATE("
+### Description
+",IF(ISBLANK(Schedule!F6),"*None*",Schedule!F6),"
+### Learning Objectives
+",IF(ISBLANK(Schedule!G6),"*None*",Schedule!G6),"
+### Readings
+",IF(Schedule!L6,CONCATENATE("[Check here](",Configuration!B$20,Configuration!B$19,"/sessions/notebooks/)"),"*None*"),"
+### Notebooks
+",IF(Schedule!M6,CONCATENATE("[Check here](",Configuration!B$20,Configuration!B$19,"/sessions/assignments/)"),"*None*"))</f>
+        <v xml:space="preserve">
+### Description
+Lab/homework
+### Learning Objectives
+*None*
+### Readings
+*None*
+### Notebooks
+*None*</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="15" customHeight="1">
+      <c r="A6" s="42" t="str">
+        <f>IF(ISBLANK(Schedule!B7),"",CONCATENATE("session",Schedule!B7))</f>
+        <v>session4</v>
+      </c>
+      <c r="B6" s="21" t="str">
+        <f t="shared" ref="B6:B33" si="1">CONCATENATE(D6,E6)</f>
+        <v>&lt;h1 style="font-family: Verdana, Geneva, sans-serif; text-align:center"&gt;Python conditionals, loops, functions, aggregating. &lt;/h1&gt;
+---
+### Description
+This lecture discusses the general strategic impact of data, open data, data encoding, data provenance, data wrangling, includeing merging, aggregation, filtering. Continued introduction to coding includes conditionals, loops, functions, missing values, filtering, group-by.  We will also introduce a basic Kaggle model for the Titantic dataset. 
+### Learning Objectives
+*None*
+### Readings
+[Check here](https://rpi-data.github.io/course-intro-ml-app/sessions/notebooks/)
+### Notebooks
+[Check here](https://rpi-data.github.io/course-intro-ml-app/sessions/assignments/)</v>
+      </c>
+      <c r="C6" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="D6" s="42" t="str">
+        <f>CONCATENATE("&lt;h1 style="&amp;CHAR(34)&amp;"font-family: Verdana, Geneva, sans-serif; text-align:center"&amp;CHAR(34)&amp;"&gt;",Schedule!E7,"&lt;/h1&gt;
+---")</f>
+        <v>&lt;h1 style="font-family: Verdana, Geneva, sans-serif; text-align:center"&gt;Python conditionals, loops, functions, aggregating. &lt;/h1&gt;
+---</v>
+      </c>
+      <c r="E6" s="11" t="str">
+        <f>CONCATENATE("
+### Description
+",IF(ISBLANK(Schedule!F7),"*None*",Schedule!F7),"
+### Learning Objectives
+",IF(ISBLANK(Schedule!G7),"*None*",Schedule!G7),"
+### Readings
+",IF(Schedule!L7,CONCATENATE("[Check here](",Configuration!B$20,Configuration!B$19,"/sessions/notebooks/)"),"*None*"),"
+### Notebooks
+",IF(Schedule!M7,CONCATENATE("[Check here](",Configuration!B$20,Configuration!B$19,"/sessions/assignments/)"),"*None*"))</f>
+        <v xml:space="preserve">
+### Description
+This lecture discusses the general strategic impact of data, open data, data encoding, data provenance, data wrangling, includeing merging, aggregation, filtering. Continued introduction to coding includes conditionals, loops, functions, missing values, filtering, group-by.  We will also introduce a basic Kaggle model for the Titantic dataset. 
+### Learning Objectives
+*None*
+### Readings
+[Check here](https://rpi-data.github.io/course-intro-ml-app/sessions/notebooks/)
+### Notebooks
+[Check here](https://rpi-data.github.io/course-intro-ml-app/sessions/assignments/)</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="15" customHeight="1">
+      <c r="A7" s="42" t="str">
+        <f>IF(ISBLANK(Schedule!B8),"",CONCATENATE("session",Schedule!B8))</f>
+        <v>session5</v>
+      </c>
+      <c r="B7" s="21" t="str">
+        <f t="shared" si="1"/>
+        <v>&lt;h1 style="font-family: Verdana, Geneva, sans-serif; text-align:center"&gt;Python conditionals, loops, functions, aggregating (continued) &lt;/h1&gt;
+---
+### Description
+Lab/homework
+### Learning Objectives
+*None*
+### Readings
+*None*
+### Notebooks
+*None*</v>
+      </c>
+      <c r="C7" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="D7" s="42" t="str">
+        <f>CONCATENATE("&lt;h1 style="&amp;CHAR(34)&amp;"font-family: Verdana, Geneva, sans-serif; text-align:center"&amp;CHAR(34)&amp;"&gt;",Schedule!E8,"&lt;/h1&gt;
+---")</f>
+        <v>&lt;h1 style="font-family: Verdana, Geneva, sans-serif; text-align:center"&gt;Python conditionals, loops, functions, aggregating (continued) &lt;/h1&gt;
+---</v>
+      </c>
+      <c r="E7" s="11" t="str">
+        <f>CONCATENATE("
+### Description
+",IF(ISBLANK(Schedule!F8),"*None*",Schedule!F8),"
+### Learning Objectives
+",IF(ISBLANK(Schedule!G8),"*None*",Schedule!G8),"
+### Readings
+",IF(Schedule!L8,CONCATENATE("[Check here](",Configuration!B$20,Configuration!B$19,"/sessions/notebooks/)"),"*None*"),"
+### Notebooks
+",IF(Schedule!M8,CONCATENATE("[Check here](",Configuration!B$20,Configuration!B$19,"/sessions/assignments/)"),"*None*"))</f>
+        <v xml:space="preserve">
+### Description
+Lab/homework
+### Learning Objectives
+*None*
+### Readings
+*None*
+### Notebooks
+*None*</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="15" customHeight="1">
+      <c r="A8" s="42" t="str">
+        <f>IF(ISBLANK(Schedule!B9),"",CONCATENATE("session",Schedule!B9))</f>
+        <v>session6</v>
+      </c>
+      <c r="B8" s="21" t="str">
+        <f t="shared" si="1"/>
+        <v>&lt;h1 style="font-family: Verdana, Geneva, sans-serif; text-align:center"&gt;Python visualization, data manipulation , and feature creation.&lt;/h1&gt;
+---
+### Description
+Introduction to APIs, web scraping feature creation, and feature creation/extraction.  The genaral goal is to get students to the point where they are able to start to do some data manipulation and utilize code they haven't created (packages, functions)
+### Learning Objectives
+*None*
+### Readings
+[Check here](https://rpi-data.github.io/course-intro-ml-app/sessions/notebooks/)
+### Notebooks
+[Check here](https://rpi-data.github.io/course-intro-ml-app/sessions/assignments/)</v>
+      </c>
+      <c r="C8" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="D8" s="42" t="str">
+        <f>CONCATENATE("&lt;h1 style="&amp;CHAR(34)&amp;"font-family: Verdana, Geneva, sans-serif; text-align:center"&amp;CHAR(34)&amp;"&gt;",Schedule!E9,"&lt;/h1&gt;
+---")</f>
+        <v>&lt;h1 style="font-family: Verdana, Geneva, sans-serif; text-align:center"&gt;Python visualization, data manipulation , and feature creation.&lt;/h1&gt;
+---</v>
+      </c>
+      <c r="E8" s="11" t="str">
+        <f>CONCATENATE("
+### Description
+",IF(ISBLANK(Schedule!F9),"*None*",Schedule!F9),"
+### Learning Objectives
+",IF(ISBLANK(Schedule!G9),"*None*",Schedule!G9),"
+### Readings
+",IF(Schedule!L9,CONCATENATE("[Check here](",Configuration!B$20,Configuration!B$19,"/sessions/notebooks/)"),"*None*"),"
+### Notebooks
+",IF(Schedule!M9,CONCATENATE("[Check here](",Configuration!B$20,Configuration!B$19,"/sessions/assignments/)"),"*None*"))</f>
+        <v xml:space="preserve">
+### Description
+Introduction to APIs, web scraping feature creation, and feature creation/extraction.  The genaral goal is to get students to the point where they are able to start to do some data manipulation and utilize code they haven't created (packages, functions)
+### Learning Objectives
+*None*
+### Readings
+[Check here](https://rpi-data.github.io/course-intro-ml-app/sessions/notebooks/)
+### Notebooks
+[Check here](https://rpi-data.github.io/course-intro-ml-app/sessions/assignments/)</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="15" customHeight="1">
+      <c r="A9" s="42" t="str">
+        <f>IF(ISBLANK(Schedule!B10),"",CONCATENATE("session",Schedule!B10))</f>
+        <v>session7</v>
+      </c>
+      <c r="B9" s="21" t="str">
+        <f t="shared" si="1"/>
+        <v>&lt;h1 style="font-family: Verdana, Geneva, sans-serif; text-align:center"&gt;Python visualization, data manipulation , and feature creation (continued)&lt;/h1&gt;
+---
+### Description
+Lab/homework
+### Learning Objectives
+*None*
+### Readings
+*None*
+### Notebooks
+*None*</v>
+      </c>
+      <c r="C9" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="D9" s="42" t="str">
+        <f>CONCATENATE("&lt;h1 style="&amp;CHAR(34)&amp;"font-family: Verdana, Geneva, sans-serif; text-align:center"&amp;CHAR(34)&amp;"&gt;",Schedule!E10,"&lt;/h1&gt;
+---")</f>
+        <v>&lt;h1 style="font-family: Verdana, Geneva, sans-serif; text-align:center"&gt;Python visualization, data manipulation , and feature creation (continued)&lt;/h1&gt;
+---</v>
+      </c>
+      <c r="E9" s="11" t="str">
+        <f>CONCATENATE("
+### Description
+",IF(ISBLANK(Schedule!F10),"*None*",Schedule!F10),"
+### Learning Objectives
+",IF(ISBLANK(Schedule!G10),"*None*",Schedule!G10),"
+### Readings
+",IF(Schedule!L10,CONCATENATE("[Check here](",Configuration!B$20,Configuration!B$19,"/sessions/notebooks/)"),"*None*"),"
+### Notebooks
+",IF(Schedule!M10,CONCATENATE("[Check here](",Configuration!B$20,Configuration!B$19,"/sessions/assignments/)"),"*None*"))</f>
+        <v xml:space="preserve">
+### Description
+Lab/homework
+### Learning Objectives
+*None*
+### Readings
+*None*
+### Notebooks
+*None*</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="15" customHeight="1">
+      <c r="A10" s="42" t="str">
+        <f>IF(ISBLANK(Schedule!B11),"",CONCATENATE("session",Schedule!B11))</f>
+        <v>session8</v>
+      </c>
+      <c r="B10" s="21" t="str">
+        <f t="shared" si="1"/>
+        <v>&lt;h1 style="font-family: Verdana, Geneva, sans-serif; text-align:center"&gt;Visualization with Tableau&lt;/h1&gt;
+---
+### Description
+Visualization is an important component of data understanding. 
+### Learning Objectives
+*None*
+### Readings
+[Check here](https://rpi-data.github.io/course-intro-ml-app/sessions/notebooks/)
+### Notebooks
+*None*</v>
+      </c>
+      <c r="C10" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="D10" s="42" t="str">
+        <f>CONCATENATE("&lt;h1 style="&amp;CHAR(34)&amp;"font-family: Verdana, Geneva, sans-serif; text-align:center"&amp;CHAR(34)&amp;"&gt;",Schedule!E11,"&lt;/h1&gt;
+---")</f>
+        <v>&lt;h1 style="font-family: Verdana, Geneva, sans-serif; text-align:center"&gt;Visualization with Tableau&lt;/h1&gt;
+---</v>
+      </c>
+      <c r="E10" s="11" t="str">
+        <f>CONCATENATE("
+### Description
+",IF(ISBLANK(Schedule!F11),"*None*",Schedule!F11),"
+### Learning Objectives
+",IF(ISBLANK(Schedule!G11),"*None*",Schedule!G11),"
+### Readings
+",IF(Schedule!L11,CONCATENATE("[Check here](",Configuration!B$20,Configuration!B$19,"/sessions/notebooks/)"),"*None*"),"
+### Notebooks
+",IF(Schedule!M11,CONCATENATE("[Check here](",Configuration!B$20,Configuration!B$19,"/sessions/assignments/)"),"*None*"))</f>
+        <v xml:space="preserve">
+### Description
+Visualization is an important component of data understanding. 
+### Learning Objectives
+*None*
+### Readings
+[Check here](https://rpi-data.github.io/course-intro-ml-app/sessions/notebooks/)
+### Notebooks
+*None*</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="15" customHeight="1">
+      <c r="A11" s="42" t="str">
+        <f>IF(ISBLANK(Schedule!B12),"",CONCATENATE("session",Schedule!B12))</f>
+        <v>session9</v>
+      </c>
+      <c r="B11" s="21" t="str">
+        <f t="shared" si="1"/>
+        <v>&lt;h1 style="font-family: Verdana, Geneva, sans-serif; text-align:center"&gt;Visualization with Tableau&lt;/h1&gt;
+---
+### Description
+Lab/homework
+### Learning Objectives
+*None*
+### Readings
+*None*
+### Notebooks
+[Check here](https://rpi-data.github.io/course-intro-ml-app/sessions/assignments/)</v>
+      </c>
+      <c r="C11" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="D11" s="42" t="str">
+        <f>CONCATENATE("&lt;h1 style="&amp;CHAR(34)&amp;"font-family: Verdana, Geneva, sans-serif; text-align:center"&amp;CHAR(34)&amp;"&gt;",Schedule!E12,"&lt;/h1&gt;
+---")</f>
+        <v>&lt;h1 style="font-family: Verdana, Geneva, sans-serif; text-align:center"&gt;Visualization with Tableau&lt;/h1&gt;
+---</v>
+      </c>
+      <c r="E11" s="11" t="str">
+        <f>CONCATENATE("
+### Description
+",IF(ISBLANK(Schedule!F12),"*None*",Schedule!F12),"
+### Learning Objectives
+",IF(ISBLANK(Schedule!G12),"*None*",Schedule!G12),"
+### Readings
+",IF(Schedule!L12,CONCATENATE("[Check here](",Configuration!B$20,Configuration!B$19,"/sessions/notebooks/)"),"*None*"),"
+### Notebooks
+",IF(Schedule!M12,CONCATENATE("[Check here](",Configuration!B$20,Configuration!B$19,"/sessions/assignments/)"),"*None*"))</f>
+        <v xml:space="preserve">
+### Description
+Lab/homework
+### Learning Objectives
+*None*
+### Readings
+*None*
+### Notebooks
+[Check here](https://rpi-data.github.io/course-intro-ml-app/sessions/assignments/)</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="15" customHeight="1">
+      <c r="A12" s="42" t="str">
+        <f>IF(ISBLANK(Schedule!B13),"",CONCATENATE("session",Schedule!B13))</f>
+        <v>session10</v>
+      </c>
+      <c r="B12" s="21" t="str">
+        <f t="shared" si="1"/>
+        <v>&lt;h1 style="font-family: Verdana, Geneva, sans-serif; text-align:center"&gt;Introduction to R&lt;/h1&gt;
+---
+### Description
+The goal of this class is to get you familiar to using R. While we will be Jupyter notebooks, we will also examine using RStudio. Now that you have already started with Python, many of the concepts will map.
+### Learning Objectives
+*None*
+### Readings
+[Check here](https://rpi-data.github.io/course-intro-ml-app/sessions/notebooks/)
+### Notebooks
+*None*</v>
+      </c>
+      <c r="C12" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="D12" s="42" t="str">
+        <f>CONCATENATE("&lt;h1 style="&amp;CHAR(34)&amp;"font-family: Verdana, Geneva, sans-serif; text-align:center"&amp;CHAR(34)&amp;"&gt;",Schedule!E13,"&lt;/h1&gt;
+---")</f>
+        <v>&lt;h1 style="font-family: Verdana, Geneva, sans-serif; text-align:center"&gt;Introduction to R&lt;/h1&gt;
+---</v>
+      </c>
+      <c r="E12" s="11" t="str">
+        <f>CONCATENATE("
+### Description
+",IF(ISBLANK(Schedule!F13),"*None*",Schedule!F13),"
+### Learning Objectives
+",IF(ISBLANK(Schedule!G13),"*None*",Schedule!G13),"
+### Readings
+",IF(Schedule!L13,CONCATENATE("[Check here](",Configuration!B$20,Configuration!B$19,"/sessions/notebooks/)"),"*None*"),"
+### Notebooks
+",IF(Schedule!M13,CONCATENATE("[Check here](",Configuration!B$20,Configuration!B$19,"/sessions/assignments/)"),"*None*"))</f>
+        <v xml:space="preserve">
+### Description
+The goal of this class is to get you familiar to using R. While we will be Jupyter notebooks, we will also examine using RStudio. Now that you have already started with Python, many of the concepts will map.
+### Learning Objectives
+*None*
+### Readings
+[Check here](https://rpi-data.github.io/course-intro-ml-app/sessions/notebooks/)
+### Notebooks
+*None*</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="15" customHeight="1">
+      <c r="A13" s="42" t="str">
+        <f>IF(ISBLANK(Schedule!B14),"",CONCATENATE("session",Schedule!B14))</f>
+        <v>session11</v>
+      </c>
+      <c r="B13" s="21" t="str">
+        <f t="shared" si="1"/>
+        <v>&lt;h1 style="font-family: Verdana, Geneva, sans-serif; text-align:center"&gt;Introduction to R&lt;/h1&gt;
+---
+### Description
+Lab/homework
+### Learning Objectives
+*None*
+### Readings
+*None*
+### Notebooks
+*None*</v>
+      </c>
+      <c r="C13" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="D13" s="42" t="str">
+        <f>CONCATENATE("&lt;h1 style="&amp;CHAR(34)&amp;"font-family: Verdana, Geneva, sans-serif; text-align:center"&amp;CHAR(34)&amp;"&gt;",Schedule!E14,"&lt;/h1&gt;
+---")</f>
+        <v>&lt;h1 style="font-family: Verdana, Geneva, sans-serif; text-align:center"&gt;Introduction to R&lt;/h1&gt;
+---</v>
+      </c>
+      <c r="E13" s="11" t="str">
+        <f>CONCATENATE("
+### Description
+",IF(ISBLANK(Schedule!F14),"*None*",Schedule!F14),"
+### Learning Objectives
+",IF(ISBLANK(Schedule!G14),"*None*",Schedule!G14),"
+### Readings
+",IF(Schedule!L14,CONCATENATE("[Check here](",Configuration!B$20,Configuration!B$19,"/sessions/notebooks/)"),"*None*"),"
+### Notebooks
+",IF(Schedule!M14,CONCATENATE("[Check here](",Configuration!B$20,Configuration!B$19,"/sessions/assignments/)"),"*None*"))</f>
+        <v xml:space="preserve">
+### Description
+Lab/homework
+### Learning Objectives
+*None*
+### Readings
+*None*
+### Notebooks
+*None*</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="15" customHeight="1">
+      <c r="A14" s="42" t="str">
+        <f>IF(ISBLANK(Schedule!B15),"",CONCATENATE("session",Schedule!B15))</f>
+        <v>session12</v>
+      </c>
+      <c r="B14" s="21" t="str">
+        <f t="shared" si="1"/>
+        <v>&lt;h1 style="font-family: Verdana, Geneva, sans-serif; text-align:center"&gt;Overview of Modeling&lt;/h1&gt;
+---
+### Description
+We examine the basics of classess of supervised, unsupervised, reenforcement learning. Also examine overfitting and how cross validation is used for overfitting and how hypterparameters are used to optimize models. 
+### Learning Objectives
+*None*
+### Readings
+[Check here](https://rpi-data.github.io/course-intro-ml-app/sessions/notebooks/)
+### Notebooks
+*None*</v>
+      </c>
+      <c r="C14" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="D14" s="42" t="str">
+        <f>CONCATENATE("&lt;h1 style="&amp;CHAR(34)&amp;"font-family: Verdana, Geneva, sans-serif; text-align:center"&amp;CHAR(34)&amp;"&gt;",Schedule!E15,"&lt;/h1&gt;
+---")</f>
+        <v>&lt;h1 style="font-family: Verdana, Geneva, sans-serif; text-align:center"&gt;Overview of Modeling&lt;/h1&gt;
+---</v>
+      </c>
+      <c r="E14" s="11" t="str">
+        <f>CONCATENATE("
+### Description
+",IF(ISBLANK(Schedule!F15),"*None*",Schedule!F15),"
+### Learning Objectives
+",IF(ISBLANK(Schedule!G15),"*None*",Schedule!G15),"
+### Readings
+",IF(Schedule!L15,CONCATENATE("[Check here](",Configuration!B$20,Configuration!B$19,"/sessions/notebooks/)"),"*None*"),"
+### Notebooks
+",IF(Schedule!M15,CONCATENATE("[Check here](",Configuration!B$20,Configuration!B$19,"/sessions/assignments/)"),"*None*"))</f>
+        <v xml:space="preserve">
+### Description
+We examine the basics of classess of supervised, unsupervised, reenforcement learning. Also examine overfitting and how cross validation is used for overfitting and how hypterparameters are used to optimize models. 
+### Learning Objectives
+*None*
+### Readings
+[Check here](https://rpi-data.github.io/course-intro-ml-app/sessions/notebooks/)
+### Notebooks
+*None*</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="15" customHeight="1">
+      <c r="A15" s="42" t="str">
+        <f>IF(ISBLANK(Schedule!B16),"",CONCATENATE("session",Schedule!B16))</f>
+        <v>session13</v>
+      </c>
+      <c r="B15" s="21" t="str">
+        <f t="shared" si="1"/>
+        <v>&lt;h1 style="font-family: Verdana, Geneva, sans-serif; text-align:center"&gt;Overview of Modeling&lt;/h1&gt;
+---
+### Description
+Lab/homework
+### Learning Objectives
+*None*
+### Readings
+*None*
+### Notebooks
+[Check here](https://rpi-data.github.io/course-intro-ml-app/sessions/assignments/)</v>
+      </c>
+      <c r="C15" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="D15" s="42" t="str">
+        <f>CONCATENATE("&lt;h1 style="&amp;CHAR(34)&amp;"font-family: Verdana, Geneva, sans-serif; text-align:center"&amp;CHAR(34)&amp;"&gt;",Schedule!E16,"&lt;/h1&gt;
+---")</f>
+        <v>&lt;h1 style="font-family: Verdana, Geneva, sans-serif; text-align:center"&gt;Overview of Modeling&lt;/h1&gt;
+---</v>
+      </c>
+      <c r="E15" s="11" t="str">
+        <f>CONCATENATE("
+### Description
+",IF(ISBLANK(Schedule!F16),"*None*",Schedule!F16),"
+### Learning Objectives
+",IF(ISBLANK(Schedule!G16),"*None*",Schedule!G16),"
+### Readings
+",IF(Schedule!L16,CONCATENATE("[Check here](",Configuration!B$20,Configuration!B$19,"/sessions/notebooks/)"),"*None*"),"
+### Notebooks
+",IF(Schedule!M16,CONCATENATE("[Check here](",Configuration!B$20,Configuration!B$19,"/sessions/assignments/)"),"*None*"))</f>
+        <v xml:space="preserve">
+### Description
+Lab/homework
+### Learning Objectives
+*None*
+### Readings
+*None*
+### Notebooks
+[Check here](https://rpi-data.github.io/course-intro-ml-app/sessions/assignments/)</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="15" customHeight="1">
+      <c r="A16" s="42" t="str">
+        <f>IF(ISBLANK(Schedule!B17),"",CONCATENATE("session",Schedule!B17))</f>
+        <v>session14</v>
+      </c>
+      <c r="B16" s="21" t="str">
+        <f t="shared" si="1"/>
+        <v>&lt;h1 style="font-family: Verdana, Geneva, sans-serif; text-align:center"&gt;Review/Kaggle Project Introduction &lt;/h1&gt;
+---
+### Description
+*None*
+### Learning Objectives
+*None*
+### Readings
+*None*
+### Notebooks
+*None*</v>
+      </c>
+      <c r="C16" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="D16" s="42" t="str">
+        <f>CONCATENATE("&lt;h1 style="&amp;CHAR(34)&amp;"font-family: Verdana, Geneva, sans-serif; text-align:center"&amp;CHAR(34)&amp;"&gt;",Schedule!E17,"&lt;/h1&gt;
+---")</f>
+        <v>&lt;h1 style="font-family: Verdana, Geneva, sans-serif; text-align:center"&gt;Review/Kaggle Project Introduction &lt;/h1&gt;
+---</v>
+      </c>
+      <c r="E16" s="11" t="str">
+        <f>CONCATENATE("
+### Description
+",IF(ISBLANK(Schedule!F17),"*None*",Schedule!F17),"
+### Learning Objectives
+",IF(ISBLANK(Schedule!G17),"*None*",Schedule!G17),"
+### Readings
+",IF(Schedule!L17,CONCATENATE("[Check here](",Configuration!B$20,Configuration!B$19,"/sessions/notebooks/)"),"*None*"),"
+### Notebooks
+",IF(Schedule!M17,CONCATENATE("[Check here](",Configuration!B$20,Configuration!B$19,"/sessions/assignments/)"),"*None*"))</f>
+        <v xml:space="preserve">
+### Description
+*None*
+### Learning Objectives
+*None*
+### Readings
+*None*
+### Notebooks
+*None*</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="15" customHeight="1">
+      <c r="A17" s="42" t="str">
+        <f>IF(ISBLANK(Schedule!B18),"",CONCATENATE("session",Schedule!B18))</f>
+        <v>session15</v>
+      </c>
+      <c r="B17" s="21" t="str">
+        <f t="shared" si="1"/>
+        <v>&lt;h1 style="font-family: Verdana, Geneva, sans-serif; text-align:center"&gt;Midterm &lt;/h1&gt;
+---
+### Description
+*None*
+### Learning Objectives
+*None*
+### Readings
+*None*
+### Notebooks
+[Check here](https://rpi-data.github.io/course-intro-ml-app/sessions/assignments/)</v>
+      </c>
+      <c r="C17" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="D17" s="42" t="str">
+        <f>CONCATENATE("&lt;h1 style="&amp;CHAR(34)&amp;"font-family: Verdana, Geneva, sans-serif; text-align:center"&amp;CHAR(34)&amp;"&gt;",Schedule!E18,"&lt;/h1&gt;
+---")</f>
+        <v>&lt;h1 style="font-family: Verdana, Geneva, sans-serif; text-align:center"&gt;Midterm &lt;/h1&gt;
+---</v>
+      </c>
+      <c r="E17" s="11" t="str">
+        <f>CONCATENATE("
+### Description
+",IF(ISBLANK(Schedule!F18),"*None*",Schedule!F18),"
+### Learning Objectives
+",IF(ISBLANK(Schedule!G18),"*None*",Schedule!G18),"
+### Readings
+",IF(Schedule!L18,CONCATENATE("[Check here](",Configuration!B$20,Configuration!B$19,"/sessions/notebooks/)"),"*None*"),"
+### Notebooks
+",IF(Schedule!M18,CONCATENATE("[Check here](",Configuration!B$20,Configuration!B$19,"/sessions/assignments/)"),"*None*"))</f>
+        <v xml:space="preserve">
+### Description
+*None*
+### Learning Objectives
+*None*
+### Readings
+*None*
+### Notebooks
+[Check here](https://rpi-data.github.io/course-intro-ml-app/sessions/assignments/)</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="15" customHeight="1">
+      <c r="A18" s="42" t="str">
+        <f>IF(ISBLANK(Schedule!B19),"",CONCATENATE("session",Schedule!B19))</f>
+        <v>session16</v>
+      </c>
+      <c r="B18" s="21" t="str">
+        <f t="shared" si="1"/>
+        <v>&lt;h1 style="font-family: Verdana, Geneva, sans-serif; text-align:center"&gt;Classification&lt;/h1&gt;
+---
+### Description
+Classifcation is one of the critical machine learning applications.  In this class we review a variety of different approaches. 
+### Learning Objectives
+*None*
+### Readings
+*None*
+### Notebooks
+*None*</v>
+      </c>
+      <c r="C18" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="D18" s="42" t="str">
+        <f>CONCATENATE("&lt;h1 style="&amp;CHAR(34)&amp;"font-family: Verdana, Geneva, sans-serif; text-align:center"&amp;CHAR(34)&amp;"&gt;",Schedule!E19,"&lt;/h1&gt;
+---")</f>
+        <v>&lt;h1 style="font-family: Verdana, Geneva, sans-serif; text-align:center"&gt;Classification&lt;/h1&gt;
+---</v>
+      </c>
+      <c r="E18" s="11" t="str">
+        <f>CONCATENATE("
+### Description
+",IF(ISBLANK(Schedule!F19),"*None*",Schedule!F19),"
+### Learning Objectives
+",IF(ISBLANK(Schedule!G19),"*None*",Schedule!G19),"
+### Readings
+",IF(Schedule!L19,CONCATENATE("[Check here](",Configuration!B$20,Configuration!B$19,"/sessions/notebooks/)"),"*None*"),"
+### Notebooks
+",IF(Schedule!M19,CONCATENATE("[Check here](",Configuration!B$20,Configuration!B$19,"/sessions/assignments/)"),"*None*"))</f>
+        <v xml:space="preserve">
+### Description
+Classifcation is one of the critical machine learning applications.  In this class we review a variety of different approaches. 
+### Learning Objectives
+*None*
+### Readings
+*None*
+### Notebooks
+*None*</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="15" customHeight="1">
+      <c r="A19" s="42" t="str">
+        <f>IF(ISBLANK(Schedule!B20),"",CONCATENATE("session",Schedule!B20))</f>
+        <v>session17</v>
+      </c>
+      <c r="B19" s="21" t="str">
+        <f t="shared" si="1"/>
+        <v>&lt;h1 style="font-family: Verdana, Geneva, sans-serif; text-align:center"&gt;Classification&lt;/h1&gt;
+---
+### Description
+Lab/homework
+### Learning Objectives
+*None*
+### Readings
+*None*
+### Notebooks
+*None*</v>
+      </c>
+      <c r="C19" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="D19" s="42" t="str">
+        <f>CONCATENATE("&lt;h1 style="&amp;CHAR(34)&amp;"font-family: Verdana, Geneva, sans-serif; text-align:center"&amp;CHAR(34)&amp;"&gt;",Schedule!E20,"&lt;/h1&gt;
+---")</f>
+        <v>&lt;h1 style="font-family: Verdana, Geneva, sans-serif; text-align:center"&gt;Classification&lt;/h1&gt;
+---</v>
+      </c>
+      <c r="E19" s="11" t="str">
+        <f>CONCATENATE("
+### Description
+",IF(ISBLANK(Schedule!F20),"*None*",Schedule!F20),"
+### Learning Objectives
+",IF(ISBLANK(Schedule!G20),"*None*",Schedule!G20),"
+### Readings
+",IF(Schedule!L20,CONCATENATE("[Check here](",Configuration!B$20,Configuration!B$19,"/sessions/notebooks/)"),"*None*"),"
+### Notebooks
+",IF(Schedule!M20,CONCATENATE("[Check here](",Configuration!B$20,Configuration!B$19,"/sessions/assignments/)"),"*None*"))</f>
+        <v xml:space="preserve">
+### Description
+Lab/homework
+### Learning Objectives
+*None*
+### Readings
+*None*
+### Notebooks
+*None*</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="15" customHeight="1">
+      <c r="A20" s="42" t="str">
+        <f>IF(ISBLANK(Schedule!B21),"",CONCATENATE("session",Schedule!B21))</f>
+        <v>session18</v>
+      </c>
+      <c r="B20" s="21" t="str">
+        <f t="shared" si="1"/>
+        <v>&lt;h1 style="font-family: Verdana, Geneva, sans-serif; text-align:center"&gt;Regression&lt;/h1&gt;
+---
+### Description
+Regression models similarly a a major type of machine learning application.  In this 
+### Learning Objectives
+*None*
+### Readings
+*None*
+### Notebooks
+*None*</v>
+      </c>
+      <c r="C20" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="D20" s="42" t="str">
+        <f>CONCATENATE("&lt;h1 style="&amp;CHAR(34)&amp;"font-family: Verdana, Geneva, sans-serif; text-align:center"&amp;CHAR(34)&amp;"&gt;",Schedule!E21,"&lt;/h1&gt;
+---")</f>
+        <v>&lt;h1 style="font-family: Verdana, Geneva, sans-serif; text-align:center"&gt;Regression&lt;/h1&gt;
+---</v>
+      </c>
+      <c r="E20" s="11" t="str">
+        <f>CONCATENATE("
+### Description
+",IF(ISBLANK(Schedule!F21),"*None*",Schedule!F21),"
+### Learning Objectives
+",IF(ISBLANK(Schedule!G21),"*None*",Schedule!G21),"
+### Readings
+",IF(Schedule!L21,CONCATENATE("[Check here](",Configuration!B$20,Configuration!B$19,"/sessions/notebooks/)"),"*None*"),"
+### Notebooks
+",IF(Schedule!M21,CONCATENATE("[Check here](",Configuration!B$20,Configuration!B$19,"/sessions/assignments/)"),"*None*"))</f>
+        <v xml:space="preserve">
+### Description
+Regression models similarly a a major type of machine learning application.  In this 
+### Learning Objectives
+*None*
+### Readings
+*None*
+### Notebooks
+*None*</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="15" customHeight="1">
+      <c r="A21" s="42" t="str">
+        <f>IF(ISBLANK(Schedule!B22),"",CONCATENATE("session",Schedule!B22))</f>
+        <v>session19</v>
+      </c>
+      <c r="B21" s="21" t="str">
+        <f t="shared" si="1"/>
+        <v>&lt;h1 style="font-family: Verdana, Geneva, sans-serif; text-align:center"&gt;Regression&lt;/h1&gt;
+---
+### Description
+Lab/homework
+### Learning Objectives
+*None*
+### Readings
+*None*
+### Notebooks
+*None*</v>
+      </c>
+      <c r="C21" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="D21" s="42" t="str">
+        <f>CONCATENATE("&lt;h1 style="&amp;CHAR(34)&amp;"font-family: Verdana, Geneva, sans-serif; text-align:center"&amp;CHAR(34)&amp;"&gt;",Schedule!E22,"&lt;/h1&gt;
+---")</f>
+        <v>&lt;h1 style="font-family: Verdana, Geneva, sans-serif; text-align:center"&gt;Regression&lt;/h1&gt;
+---</v>
+      </c>
+      <c r="E21" s="11" t="str">
+        <f>CONCATENATE("
+### Description
+",IF(ISBLANK(Schedule!F22),"*None*",Schedule!F22),"
+### Learning Objectives
+",IF(ISBLANK(Schedule!G22),"*None*",Schedule!G22),"
+### Readings
+",IF(Schedule!L22,CONCATENATE("[Check here](",Configuration!B$20,Configuration!B$19,"/sessions/notebooks/)"),"*None*"),"
+### Notebooks
+",IF(Schedule!M22,CONCATENATE("[Check here](",Configuration!B$20,Configuration!B$19,"/sessions/assignments/)"),"*None*"))</f>
+        <v xml:space="preserve">
+### Description
+Lab/homework
+### Learning Objectives
+*None*
+### Readings
+*None*
+### Notebooks
+*None*</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="15" customHeight="1">
+      <c r="A22" s="42" t="str">
+        <f>IF(ISBLANK(Schedule!B23),"",CONCATENATE("session",Schedule!B23))</f>
+        <v>session20</v>
+      </c>
+      <c r="B22" s="21" t="str">
+        <f t="shared" si="1"/>
+        <v>&lt;h1 style="font-family: Verdana, Geneva, sans-serif; text-align:center"&gt;Text and NLP&lt;/h1&gt;
+---
+### Description
+The goal of this class is to investigate basic concepts surrounding text mining.
+### Learning Objectives
+*None*
+### Readings
+[Check here](https://rpi-data.github.io/course-intro-ml-app/sessions/notebooks/)
+### Notebooks
+*None*</v>
+      </c>
+      <c r="C22" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="D22" s="42" t="str">
+        <f>CONCATENATE("&lt;h1 style="&amp;CHAR(34)&amp;"font-family: Verdana, Geneva, sans-serif; text-align:center"&amp;CHAR(34)&amp;"&gt;",Schedule!E23,"&lt;/h1&gt;
+---")</f>
+        <v>&lt;h1 style="font-family: Verdana, Geneva, sans-serif; text-align:center"&gt;Text and NLP&lt;/h1&gt;
+---</v>
+      </c>
+      <c r="E22" s="11" t="str">
+        <f>CONCATENATE("
+### Description
+",IF(ISBLANK(Schedule!F23),"*None*",Schedule!F23),"
+### Learning Objectives
+",IF(ISBLANK(Schedule!G23),"*None*",Schedule!G23),"
+### Readings
+",IF(Schedule!L23,CONCATENATE("[Check here](",Configuration!B$20,Configuration!B$19,"/sessions/notebooks/)"),"*None*"),"
+### Notebooks
+",IF(Schedule!M23,CONCATENATE("[Check here](",Configuration!B$20,Configuration!B$19,"/sessions/assignments/)"),"*None*"))</f>
+        <v xml:space="preserve">
+### Description
+The goal of this class is to investigate basic concepts surrounding text mining.
+### Learning Objectives
+*None*
+### Readings
+[Check here](https://rpi-data.github.io/course-intro-ml-app/sessions/notebooks/)
+### Notebooks
+*None*</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="15" customHeight="1">
+      <c r="A23" s="42" t="str">
+        <f>IF(ISBLANK(Schedule!B24),"",CONCATENATE("session",Schedule!B24))</f>
+        <v>session21</v>
+      </c>
+      <c r="B23" s="21" t="str">
+        <f t="shared" si="1"/>
+        <v>&lt;h1 style="font-family: Verdana, Geneva, sans-serif; text-align:center"&gt;Text and NLP&lt;/h1&gt;
+---
+### Description
+Lab/homework
+### Learning Objectives
+*None*
+### Readings
+*None*
+### Notebooks
+*None*</v>
+      </c>
+      <c r="C23" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="D23" s="42" t="str">
+        <f>CONCATENATE("&lt;h1 style="&amp;CHAR(34)&amp;"font-family: Verdana, Geneva, sans-serif; text-align:center"&amp;CHAR(34)&amp;"&gt;",Schedule!E24,"&lt;/h1&gt;
+---")</f>
+        <v>&lt;h1 style="font-family: Verdana, Geneva, sans-serif; text-align:center"&gt;Text and NLP&lt;/h1&gt;
+---</v>
+      </c>
+      <c r="E23" s="11" t="str">
+        <f>CONCATENATE("
+### Description
+",IF(ISBLANK(Schedule!F24),"*None*",Schedule!F24),"
+### Learning Objectives
+",IF(ISBLANK(Schedule!G24),"*None*",Schedule!G24),"
+### Readings
+",IF(Schedule!L24,CONCATENATE("[Check here](",Configuration!B$20,Configuration!B$19,"/sessions/notebooks/)"),"*None*"),"
+### Notebooks
+",IF(Schedule!M24,CONCATENATE("[Check here](",Configuration!B$20,Configuration!B$19,"/sessions/assignments/)"),"*None*"))</f>
+        <v xml:space="preserve">
+### Description
+Lab/homework
+### Learning Objectives
+*None*
+### Readings
+*None*
+### Notebooks
+*None*</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="15" customHeight="1">
+      <c r="A24" s="42" t="str">
+        <f>IF(ISBLANK(Schedule!B25),"",CONCATENATE("session",Schedule!B25))</f>
+        <v>session22</v>
+      </c>
+      <c r="B24" s="21" t="str">
+        <f t="shared" si="1"/>
+        <v>&lt;h1 style="font-family: Verdana, Geneva, sans-serif; text-align:center"&gt;Introduction to Big Data &lt;/h1&gt;
+---
+### Description
+The goal here is to provide an overview of how data processes can be scaled with Spark.
+### Learning Objectives
+*None*
+### Readings
+*None*
+### Notebooks
+*None*</v>
+      </c>
+      <c r="C24" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="D24" s="42" t="str">
+        <f>CONCATENATE("&lt;h1 style="&amp;CHAR(34)&amp;"font-family: Verdana, Geneva, sans-serif; text-align:center"&amp;CHAR(34)&amp;"&gt;",Schedule!E25,"&lt;/h1&gt;
+---")</f>
+        <v>&lt;h1 style="font-family: Verdana, Geneva, sans-serif; text-align:center"&gt;Introduction to Big Data &lt;/h1&gt;
+---</v>
+      </c>
+      <c r="E24" s="11" t="str">
+        <f>CONCATENATE("
+### Description
+",IF(ISBLANK(Schedule!F25),"*None*",Schedule!F25),"
+### Learning Objectives
+",IF(ISBLANK(Schedule!G25),"*None*",Schedule!G25),"
+### Readings
+",IF(Schedule!L25,CONCATENATE("[Check here](",Configuration!B$20,Configuration!B$19,"/sessions/notebooks/)"),"*None*"),"
+### Notebooks
+",IF(Schedule!M25,CONCATENATE("[Check here](",Configuration!B$20,Configuration!B$19,"/sessions/assignments/)"),"*None*"))</f>
+        <v xml:space="preserve">
+### Description
+The goal here is to provide an overview of how data processes can be scaled with Spark.
+### Learning Objectives
+*None*
+### Readings
+*None*
+### Notebooks
+*None*</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="15" customHeight="1">
+      <c r="A25" s="42" t="str">
+        <f>IF(ISBLANK(Schedule!B26),"",CONCATENATE("session",Schedule!B26))</f>
+        <v>session23</v>
+      </c>
+      <c r="B25" s="21" t="str">
+        <f t="shared" si="1"/>
+        <v>&lt;h1 style="font-family: Verdana, Geneva, sans-serif; text-align:center"&gt;Time Series Analysis&lt;/h1&gt;
+---
+### Description
+Time series and panel data is a bit different and requires a different approach.  Here we cover some of the basics. 
+### Learning Objectives
+*None*
+### Readings
+[Check here](https://rpi-data.github.io/course-intro-ml-app/sessions/notebooks/)
+### Notebooks
+*None*</v>
+      </c>
+      <c r="C25" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="D25" s="42" t="str">
+        <f>CONCATENATE("&lt;h1 style="&amp;CHAR(34)&amp;"font-family: Verdana, Geneva, sans-serif; text-align:center"&amp;CHAR(34)&amp;"&gt;",Schedule!E26,"&lt;/h1&gt;
+---")</f>
+        <v>&lt;h1 style="font-family: Verdana, Geneva, sans-serif; text-align:center"&gt;Time Series Analysis&lt;/h1&gt;
+---</v>
+      </c>
+      <c r="E25" s="11" t="str">
+        <f>CONCATENATE("
+### Description
+",IF(ISBLANK(Schedule!F26),"*None*",Schedule!F26),"
+### Learning Objectives
+",IF(ISBLANK(Schedule!G26),"*None*",Schedule!G26),"
+### Readings
+",IF(Schedule!L26,CONCATENATE("[Check here](",Configuration!B$20,Configuration!B$19,"/sessions/notebooks/)"),"*None*"),"
+### Notebooks
+",IF(Schedule!M26,CONCATENATE("[Check here](",Configuration!B$20,Configuration!B$19,"/sessions/assignments/)"),"*None*"))</f>
+        <v xml:space="preserve">
+### Description
+Time series and panel data is a bit different and requires a different approach.  Here we cover some of the basics. 
+### Learning Objectives
+*None*
+### Readings
+[Check here](https://rpi-data.github.io/course-intro-ml-app/sessions/notebooks/)
+### Notebooks
+*None*</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="15" customHeight="1">
+      <c r="A26" s="42" t="str">
+        <f>IF(ISBLANK(Schedule!B27),"",CONCATENATE("session",Schedule!B27))</f>
+        <v>session24</v>
+      </c>
+      <c r="B26" s="21" t="str">
+        <f t="shared" si="1"/>
+        <v>&lt;h1 style="font-family: Verdana, Geneva, sans-serif; text-align:center"&gt;Image Data and Deep Learning&lt;/h1&gt;
+---
+### Description
+Image data is different and deep learning has transformed the ability of machines to process image data. In this lecture we will get an overview of image processing and deep learning techniques. 
+### Learning Objectives
+*None*
+### Readings
+*None*
+### Notebooks
+*None*</v>
+      </c>
+      <c r="C26" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="D26" s="42" t="str">
+        <f>CONCATENATE("&lt;h1 style="&amp;CHAR(34)&amp;"font-family: Verdana, Geneva, sans-serif; text-align:center"&amp;CHAR(34)&amp;"&gt;",Schedule!E27,"&lt;/h1&gt;
+---")</f>
+        <v>&lt;h1 style="font-family: Verdana, Geneva, sans-serif; text-align:center"&gt;Image Data and Deep Learning&lt;/h1&gt;
+---</v>
+      </c>
+      <c r="E26" s="11" t="str">
+        <f>CONCATENATE("
+### Description
+",IF(ISBLANK(Schedule!F27),"*None*",Schedule!F27),"
+### Learning Objectives
+",IF(ISBLANK(Schedule!G27),"*None*",Schedule!G27),"
+### Readings
+",IF(Schedule!L27,CONCATENATE("[Check here](",Configuration!B$20,Configuration!B$19,"/sessions/notebooks/)"),"*None*"),"
+### Notebooks
+",IF(Schedule!M27,CONCATENATE("[Check here](",Configuration!B$20,Configuration!B$19,"/sessions/assignments/)"),"*None*"))</f>
+        <v xml:space="preserve">
+### Description
+Image data is different and deep learning has transformed the ability of machines to process image data. In this lecture we will get an overview of image processing and deep learning techniques. 
+### Learning Objectives
+*None*
+### Readings
+*None*
+### Notebooks
+*None*</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" ht="15" customHeight="1">
+      <c r="A27" s="42" t="str">
+        <f>IF(ISBLANK(Schedule!B28),"",CONCATENATE("session",Schedule!B28))</f>
+        <v>session25</v>
+      </c>
+      <c r="B27" s="21" t="str">
+        <f t="shared" si="1"/>
+        <v>&lt;h1 style="font-family: Verdana, Geneva, sans-serif; text-align:center"&gt;Image Data and Deep Learning&lt;/h1&gt;
+---
+### Description
+Lab/homework
+### Learning Objectives
+*None*
+### Readings
+*None*
+### Notebooks
+*None*</v>
+      </c>
+      <c r="C27" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="D27" s="42" t="str">
+        <f>CONCATENATE("&lt;h1 style="&amp;CHAR(34)&amp;"font-family: Verdana, Geneva, sans-serif; text-align:center"&amp;CHAR(34)&amp;"&gt;",Schedule!E28,"&lt;/h1&gt;
+---")</f>
+        <v>&lt;h1 style="font-family: Verdana, Geneva, sans-serif; text-align:center"&gt;Image Data and Deep Learning&lt;/h1&gt;
+---</v>
+      </c>
+      <c r="E27" s="11" t="str">
+        <f>CONCATENATE("
+### Description
+",IF(ISBLANK(Schedule!F28),"*None*",Schedule!F28),"
+### Learning Objectives
+",IF(ISBLANK(Schedule!G28),"*None*",Schedule!G28),"
+### Readings
+",IF(Schedule!L28,CONCATENATE("[Check here](",Configuration!B$20,Configuration!B$19,"/sessions/notebooks/)"),"*None*"),"
+### Notebooks
+",IF(Schedule!M28,CONCATENATE("[Check here](",Configuration!B$20,Configuration!B$19,"/sessions/assignments/)"),"*None*"))</f>
+        <v xml:space="preserve">
+### Description
+Lab/homework
+### Learning Objectives
+*None*
+### Readings
+*None*
+### Notebooks
+*None*</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" ht="15" customHeight="1">
+      <c r="A28" s="42" t="str">
+        <f>IF(ISBLANK(Schedule!B29),"",CONCATENATE("session",Schedule!B29))</f>
+        <v>session26</v>
+      </c>
+      <c r="B28" s="21" t="str">
+        <f t="shared" si="1"/>
+        <v>&lt;h1 style="font-family: Verdana, Geneva, sans-serif; text-align:center"&gt;Automl and Modeling Packages&lt;/h1&gt;
+---
+### Description
+Increasingly there are tools to automate the process of selecting models. 
+### Learning Objectives
+*None*
+### Readings
+*None*
+### Notebooks
+*None*</v>
+      </c>
+      <c r="C28" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="D28" s="42" t="str">
+        <f>CONCATENATE("&lt;h1 style="&amp;CHAR(34)&amp;"font-family: Verdana, Geneva, sans-serif; text-align:center"&amp;CHAR(34)&amp;"&gt;",Schedule!E29,"&lt;/h1&gt;
+---")</f>
+        <v>&lt;h1 style="font-family: Verdana, Geneva, sans-serif; text-align:center"&gt;Automl and Modeling Packages&lt;/h1&gt;
+---</v>
+      </c>
+      <c r="E28" s="11" t="str">
+        <f>CONCATENATE("
+### Description
+",IF(ISBLANK(Schedule!F29),"*None*",Schedule!F29),"
+### Learning Objectives
+",IF(ISBLANK(Schedule!G29),"*None*",Schedule!G29),"
+### Readings
+",IF(Schedule!L29,CONCATENATE("[Check here](",Configuration!B$20,Configuration!B$19,"/sessions/notebooks/)"),"*None*"),"
+### Notebooks
+",IF(Schedule!M29,CONCATENATE("[Check here](",Configuration!B$20,Configuration!B$19,"/sessions/assignments/)"),"*None*"))</f>
+        <v xml:space="preserve">
+### Description
+Increasingly there are tools to automate the process of selecting models. 
+### Learning Objectives
+*None*
+### Readings
+*None*
+### Notebooks
+*None*</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" ht="15" customHeight="1">
+      <c r="A29" s="42" t="str">
+        <f>IF(ISBLANK(Schedule!B30),"",CONCATENATE("session",Schedule!B30))</f>
+        <v/>
+      </c>
+      <c r="B29" s="21" t="str">
+        <f t="shared" si="1"/>
+        <v>&lt;h1 style="font-family: Verdana, Geneva, sans-serif; text-align:center"&gt;Thanksgiving&lt;/h1&gt;
+---
+### Description
+*None*
+### Learning Objectives
+*None*
+### Readings
+*None*
+### Notebooks
+*None*</v>
+      </c>
+      <c r="C29" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="D29" s="42" t="str">
+        <f>CONCATENATE("&lt;h1 style="&amp;CHAR(34)&amp;"font-family: Verdana, Geneva, sans-serif; text-align:center"&amp;CHAR(34)&amp;"&gt;",Schedule!E30,"&lt;/h1&gt;
+---")</f>
+        <v>&lt;h1 style="font-family: Verdana, Geneva, sans-serif; text-align:center"&gt;Thanksgiving&lt;/h1&gt;
+---</v>
+      </c>
+      <c r="E29" s="11" t="str">
+        <f>CONCATENATE("
+### Description
+",IF(ISBLANK(Schedule!F30),"*None*",Schedule!F30),"
+### Learning Objectives
+",IF(ISBLANK(Schedule!G30),"*None*",Schedule!G30),"
+### Readings
+",IF(Schedule!L30,CONCATENATE("[Check here](",Configuration!B$20,Configuration!B$19,"/sessions/notebooks/)"),"*None*"),"
+### Notebooks
+",IF(Schedule!M30,CONCATENATE("[Check here](",Configuration!B$20,Configuration!B$19,"/sessions/assignments/)"),"*None*"))</f>
+        <v xml:space="preserve">
+### Description
+*None*
+### Learning Objectives
+*None*
+### Readings
+*None*
+### Notebooks
+*None*</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" ht="15" customHeight="1">
+      <c r="A30" s="42" t="str">
+        <f>IF(ISBLANK(Schedule!B31),"",CONCATENATE("session",Schedule!B31))</f>
+        <v>session27</v>
+      </c>
+      <c r="B30" s="21" t="str">
+        <f t="shared" si="1"/>
+        <v>&lt;h1 style="font-family: Verdana, Geneva, sans-serif; text-align:center"&gt;Automl and Model Search&lt;/h1&gt;
+---
+### Description
+Lab/homework
+### Learning Objectives
+*None*
+### Readings
+*None*
+### Notebooks
+*None*</v>
+      </c>
+      <c r="C30" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="D30" s="42" t="str">
+        <f>CONCATENATE("&lt;h1 style="&amp;CHAR(34)&amp;"font-family: Verdana, Geneva, sans-serif; text-align:center"&amp;CHAR(34)&amp;"&gt;",Schedule!E31,"&lt;/h1&gt;
+---")</f>
+        <v>&lt;h1 style="font-family: Verdana, Geneva, sans-serif; text-align:center"&gt;Automl and Model Search&lt;/h1&gt;
+---</v>
+      </c>
+      <c r="E30" s="11" t="str">
+        <f>CONCATENATE("
+### Description
+",IF(ISBLANK(Schedule!F31),"*None*",Schedule!F31),"
+### Learning Objectives
+",IF(ISBLANK(Schedule!G31),"*None*",Schedule!G31),"
+### Readings
+",IF(Schedule!L31,CONCATENATE("[Check here](",Configuration!B$20,Configuration!B$19,"/sessions/notebooks/)"),"*None*"),"
+### Notebooks
+",IF(Schedule!M31,CONCATENATE("[Check here](",Configuration!B$20,Configuration!B$19,"/sessions/assignments/)"),"*None*"))</f>
+        <v xml:space="preserve">
+### Description
+Lab/homework
+### Learning Objectives
+*None*
+### Readings
+*None*
+### Notebooks
+*None*</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" ht="15" customHeight="1">
+      <c r="A31" s="42" t="str">
+        <f>IF(ISBLANK(Schedule!B32),"",CONCATENATE("session",Schedule!B32))</f>
+        <v>session28</v>
+      </c>
+      <c r="B31" s="21" t="str">
+        <f t="shared" si="1"/>
+        <v>&lt;h1 style="font-family: Verdana, Geneva, sans-serif; text-align:center"&gt;Final Presentations&lt;/h1&gt;
+---
+### Description
+*None*
+### Learning Objectives
+*None*
+### Readings
+*None*
+### Notebooks
+*None*</v>
+      </c>
+      <c r="C31" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="D31" s="42" t="str">
+        <f>CONCATENATE("&lt;h1 style="&amp;CHAR(34)&amp;"font-family: Verdana, Geneva, sans-serif; text-align:center"&amp;CHAR(34)&amp;"&gt;",Schedule!E32,"&lt;/h1&gt;
+---")</f>
+        <v>&lt;h1 style="font-family: Verdana, Geneva, sans-serif; text-align:center"&gt;Final Presentations&lt;/h1&gt;
+---</v>
+      </c>
+      <c r="E31" s="11" t="str">
+        <f>CONCATENATE("
+### Description
+",IF(ISBLANK(Schedule!F32),"*None*",Schedule!F32),"
+### Learning Objectives
+",IF(ISBLANK(Schedule!G32),"*None*",Schedule!G32),"
+### Readings
+",IF(Schedule!L32,CONCATENATE("[Check here](",Configuration!B$20,Configuration!B$19,"/sessions/notebooks/)"),"*None*"),"
+### Notebooks
+",IF(Schedule!M32,CONCATENATE("[Check here](",Configuration!B$20,Configuration!B$19,"/sessions/assignments/)"),"*None*"))</f>
+        <v xml:space="preserve">
+### Description
+*None*
+### Learning Objectives
+*None*
+### Readings
+*None*
+### Notebooks
+*None*</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" ht="15" customHeight="1">
+      <c r="A32" s="42" t="str">
+        <f>IF(ISBLANK(Schedule!B33),"",CONCATENATE("session",Schedule!B33))</f>
+        <v>session29</v>
+      </c>
+      <c r="B32" s="21" t="str">
+        <f t="shared" si="1"/>
+        <v>&lt;h1 style="font-family: Verdana, Geneva, sans-serif; text-align:center"&gt;Final Presentations&lt;/h1&gt;
+---
+### Description
+*None*
+### Learning Objectives
+*None*
+### Readings
+*None*
+### Notebooks
+*None*</v>
+      </c>
+      <c r="C32" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="D32" s="42" t="str">
+        <f>CONCATENATE("&lt;h1 style="&amp;CHAR(34)&amp;"font-family: Verdana, Geneva, sans-serif; text-align:center"&amp;CHAR(34)&amp;"&gt;",Schedule!E33,"&lt;/h1&gt;
+---")</f>
+        <v>&lt;h1 style="font-family: Verdana, Geneva, sans-serif; text-align:center"&gt;Final Presentations&lt;/h1&gt;
+---</v>
+      </c>
+      <c r="E32" s="11" t="str">
+        <f>CONCATENATE("
+### Description
+",IF(ISBLANK(Schedule!F33),"*None*",Schedule!F33),"
+### Learning Objectives
+",IF(ISBLANK(Schedule!G33),"*None*",Schedule!G33),"
+### Readings
+",IF(Schedule!L33,CONCATENATE("[Check here](",Configuration!B$20,Configuration!B$19,"/sessions/notebooks/)"),"*None*"),"
+### Notebooks
+",IF(Schedule!M33,CONCATENATE("[Check here](",Configuration!B$20,Configuration!B$19,"/sessions/assignments/)"),"*None*"))</f>
+        <v xml:space="preserve">
+### Description
+*None*
+### Learning Objectives
+*None*
+### Readings
+*None*
+### Notebooks
+*None*</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" ht="15" customHeight="1">
+      <c r="A33" s="42" t="str">
+        <f>IF(ISBLANK(Schedule!B34),"",CONCATENATE("session",Schedule!B34))</f>
+        <v/>
+      </c>
+      <c r="B33" s="21" t="str">
+        <f t="shared" si="1"/>
+        <v>&lt;h1 style="font-family: Verdana, Geneva, sans-serif; text-align:center"&gt;Final Exam&lt;/h1&gt;
+---
+### Description
+*None*
+### Learning Objectives
+*None*
+### Readings
+*None*
+### Notebooks
+*None*</v>
+      </c>
+      <c r="C33" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="D33" s="42" t="str">
+        <f>CONCATENATE("&lt;h1 style="&amp;CHAR(34)&amp;"font-family: Verdana, Geneva, sans-serif; text-align:center"&amp;CHAR(34)&amp;"&gt;",Schedule!E34,"&lt;/h1&gt;
+---")</f>
+        <v>&lt;h1 style="font-family: Verdana, Geneva, sans-serif; text-align:center"&gt;Final Exam&lt;/h1&gt;
+---</v>
+      </c>
+      <c r="E33" s="11" t="str">
+        <f>CONCATENATE("
+### Description
+",IF(ISBLANK(Schedule!F34),"*None*",Schedule!F34),"
+### Learning Objectives
+",IF(ISBLANK(Schedule!G34),"*None*",Schedule!G34),"
+### Readings
+",IF(Schedule!L34,CONCATENATE("[Check here](",Configuration!B$20,Configuration!B$19,"/sessions/notebooks/)"),"*None*"),"
+### Notebooks
+",IF(Schedule!M34,CONCATENATE("[Check here](",Configuration!B$20,Configuration!B$19,"/sessions/assignments/)"),"*None*"))</f>
+        <v xml:space="preserve">
+### Description
+*None*
+### Learning Objectives
+*None*
+### Readings
+*None*
+### Notebooks
+*None*</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4865,8 +6270,8 @@
   </sheetPr>
   <dimension ref="A1:F24"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.09765625" defaultRowHeight="15" customHeight="1"/>
@@ -4885,7 +6290,11 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="15.6">
+    <row r="2" spans="1:6" ht="15" customHeight="1">
+      <c r="A2" s="41" t="str">
+        <f>IF(ISBLANK(Schedule!H3),"",CONCATENATE("assign",Schedule!H3))</f>
+        <v/>
+      </c>
       <c r="B2" s="21" t="str">
         <f>CONCATENATE(C2,D2)</f>
         <v/>
@@ -4905,7 +6314,11 @@
       </c>
       <c r="F2" s="41"/>
     </row>
-    <row r="3" spans="1:6" ht="15.6">
+    <row r="3" spans="1:6" ht="15" customHeight="1">
+      <c r="A3" s="41" t="str">
+        <f>IF(ISBLANK(Schedule!H4),"",CONCATENATE("assign",Schedule!H4))</f>
+        <v/>
+      </c>
       <c r="B3" s="21" t="str">
         <f>CONCATENATE(C3,D3)</f>
         <v/>
@@ -4924,7 +6337,7 @@
         <v/>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="156">
+    <row r="4" spans="1:6" ht="15" customHeight="1">
       <c r="A4" s="41" t="str">
         <f>IF(ISBLANK(Schedule!H5),"",CONCATENATE("assign",Schedule!H5))</f>
         <v>assign1</v>
@@ -4936,7 +6349,9 @@
 ### Description
 This introductory assignment introduces the basics of loading files from a variety of formats. 
 ### Instructions
-*None*</v>
+*None*
+### Link
+[Assignment 3](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/04-viz-api-scraper/hm-03/hm03.ipynb)</v>
       </c>
       <c r="C4" s="42" t="str">
         <f>IF(ISBLANK(Schedule!H5),"",CONCATENATE("&lt;h1 style="&amp;CHAR(34)&amp;"font-family: Verdana, Geneva, sans-serif; text-align:center"&amp;CHAR(34)&amp;"&gt;Assignment ",Schedule!H5,"&lt;/h1&gt;
@@ -4949,12 +6364,16 @@
 ### Description
 ",IF(ISBLANK(Schedule!I5),"*None*",Schedule!I5),"
 ### Instructions
-",IF(ISBLANK(Schedule!J5),"*None*",Schedule!J5)))</f>
+",IF(ISBLANK(Schedule!J5),"*None*",Schedule!J5),"
+### Link
+",IF(ISBLANK(Schedule!K10),"*None*",Schedule!R10)))</f>
         <v xml:space="preserve">
 ### Description
 This introductory assignment introduces the basics of loading files from a variety of formats. 
 ### Instructions
-*None*</v>
+*None*
+### Link
+[Assignment 3](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/04-viz-api-scraper/hm-03/hm03.ipynb)</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="15" customHeight="1">
@@ -4976,7 +6395,9 @@
 ### Description
 ",IF(ISBLANK(Schedule!I6),"*None*",Schedule!I6),"
 ### Instructions
-",IF(ISBLANK(Schedule!J6),"*None*",Schedule!J6)))</f>
+",IF(ISBLANK(Schedule!J6),"*None*",Schedule!J6),"
+### Link
+",IF(ISBLANK(Schedule!K11),"*None*",Schedule!R11)))</f>
         <v/>
       </c>
     </row>
@@ -4999,11 +6420,13 @@
 ### Description
 ",IF(ISBLANK(Schedule!I7),"*None*",Schedule!I7),"
 ### Instructions
-",IF(ISBLANK(Schedule!J7),"*None*",Schedule!J7)))</f>
+",IF(ISBLANK(Schedule!J7),"*None*",Schedule!J7),"
+### Link
+",IF(ISBLANK(Schedule!K12),"*None*",Schedule!R12)))</f>
         <v/>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="140.4">
+    <row r="7" spans="1:6" ht="15" customHeight="1">
       <c r="A7" s="41" t="str">
         <f>IF(ISBLANK(Schedule!H8),"",CONCATENATE("assign",Schedule!H8))</f>
         <v>assign2</v>
@@ -5015,6 +6438,8 @@
 ### Description
 *None*
 ### Instructions
+*None*
+### Link
 *None*</v>
       </c>
       <c r="C7" s="42" t="str">
@@ -5028,11 +6453,15 @@
 ### Description
 ",IF(ISBLANK(Schedule!I8),"*None*",Schedule!I8),"
 ### Instructions
-",IF(ISBLANK(Schedule!J8),"*None*",Schedule!J8)))</f>
+",IF(ISBLANK(Schedule!J8),"*None*",Schedule!J8),"
+### Link
+",IF(ISBLANK(Schedule!K13),"*None*",Schedule!R13)))</f>
         <v xml:space="preserve">
 ### Description
 *None*
 ### Instructions
+*None*
+### Link
 *None*</v>
       </c>
     </row>
@@ -5055,7 +6484,9 @@
 ### Description
 ",IF(ISBLANK(Schedule!I9),"*None*",Schedule!I9),"
 ### Instructions
-",IF(ISBLANK(Schedule!J9),"*None*",Schedule!J9)))</f>
+",IF(ISBLANK(Schedule!J9),"*None*",Schedule!J9),"
+### Link
+",IF(ISBLANK(Schedule!K14),"*None*",Schedule!R14)))</f>
         <v/>
       </c>
     </row>
@@ -5071,6 +6502,8 @@
 ### Description
 *None*
 ### Instructions
+*None*
+### Link
 *None*</v>
       </c>
       <c r="C9" s="42" t="str">
@@ -5084,11 +6517,15 @@
 ### Description
 ",IF(ISBLANK(Schedule!I10),"*None*",Schedule!I10),"
 ### Instructions
-",IF(ISBLANK(Schedule!J10),"*None*",Schedule!J10)))</f>
+",IF(ISBLANK(Schedule!J10),"*None*",Schedule!J10),"
+### Link
+",IF(ISBLANK(Schedule!K15),"*None*",Schedule!R15)))</f>
         <v xml:space="preserve">
 ### Description
 *None*
 ### Instructions
+*None*
+### Link
 *None*</v>
       </c>
     </row>
@@ -5111,7 +6548,9 @@
 ### Description
 ",IF(ISBLANK(Schedule!I11),"*None*",Schedule!I11),"
 ### Instructions
-",IF(ISBLANK(Schedule!J11),"*None*",Schedule!J11)))</f>
+",IF(ISBLANK(Schedule!J11),"*None*",Schedule!J11),"
+### Link
+",IF(ISBLANK(Schedule!K16),"*None*",Schedule!R16)))</f>
         <v/>
       </c>
     </row>
@@ -5127,6 +6566,8 @@
 ### Description
 *None*
 ### Instructions
+*None*
+### Link
 *None*</v>
       </c>
       <c r="C11" s="42" t="str">
@@ -5140,11 +6581,15 @@
 ### Description
 ",IF(ISBLANK(Schedule!I12),"*None*",Schedule!I12),"
 ### Instructions
-",IF(ISBLANK(Schedule!J12),"*None*",Schedule!J12)))</f>
+",IF(ISBLANK(Schedule!J12),"*None*",Schedule!J12),"
+### Link
+",IF(ISBLANK(Schedule!K17),"*None*",Schedule!R17)))</f>
         <v xml:space="preserve">
 ### Description
 *None*
 ### Instructions
+*None*
+### Link
 *None*</v>
       </c>
     </row>
@@ -5167,7 +6612,9 @@
 ### Description
 ",IF(ISBLANK(Schedule!I13),"*None*",Schedule!I13),"
 ### Instructions
-",IF(ISBLANK(Schedule!J13),"*None*",Schedule!J13)))</f>
+",IF(ISBLANK(Schedule!J13),"*None*",Schedule!J13),"
+### Link
+",IF(ISBLANK(Schedule!K18),"*None*",Schedule!R18)))</f>
         <v/>
       </c>
     </row>
@@ -5183,6 +6630,8 @@
 ### Description
 *None*
 ### Instructions
+*None*
+### Link
 *None*</v>
       </c>
       <c r="C13" s="42" t="str">
@@ -5196,11 +6645,15 @@
 ### Description
 ",IF(ISBLANK(Schedule!I14),"*None*",Schedule!I14),"
 ### Instructions
-",IF(ISBLANK(Schedule!J14),"*None*",Schedule!J14)))</f>
+",IF(ISBLANK(Schedule!J14),"*None*",Schedule!J14),"
+### Link
+",IF(ISBLANK(Schedule!K19),"*None*",Schedule!R19)))</f>
         <v xml:space="preserve">
 ### Description
 *None*
 ### Instructions
+*None*
+### Link
 *None*</v>
       </c>
     </row>
@@ -5223,7 +6676,9 @@
 ### Description
 ",IF(ISBLANK(Schedule!I15),"*None*",Schedule!I15),"
 ### Instructions
-",IF(ISBLANK(Schedule!J15),"*None*",Schedule!J15)))</f>
+",IF(ISBLANK(Schedule!J15),"*None*",Schedule!J15),"
+### Link
+",IF(ISBLANK(Schedule!K20),"*None*",Schedule!R20)))</f>
         <v/>
       </c>
     </row>
@@ -5239,6 +6694,8 @@
 ### Description
 *None*
 ### Instructions
+*None*
+### Link
 *None*</v>
       </c>
       <c r="C15" s="42" t="str">
@@ -5252,11 +6709,15 @@
 ### Description
 ",IF(ISBLANK(Schedule!I16),"*None*",Schedule!I16),"
 ### Instructions
-",IF(ISBLANK(Schedule!J16),"*None*",Schedule!J16)))</f>
+",IF(ISBLANK(Schedule!J16),"*None*",Schedule!J16),"
+### Link
+",IF(ISBLANK(Schedule!K21),"*None*",Schedule!R21)))</f>
         <v xml:space="preserve">
 ### Description
 *None*
 ### Instructions
+*None*
+### Link
 *None*</v>
       </c>
     </row>
@@ -5279,7 +6740,9 @@
 ### Description
 ",IF(ISBLANK(Schedule!I17),"*None*",Schedule!I17),"
 ### Instructions
-",IF(ISBLANK(Schedule!J17),"*None*",Schedule!J17)))</f>
+",IF(ISBLANK(Schedule!J17),"*None*",Schedule!J17),"
+### Link
+",IF(ISBLANK(Schedule!K22),"*None*",Schedule!R22)))</f>
         <v/>
       </c>
     </row>
@@ -5295,6 +6758,8 @@
 ### Description
 *None*
 ### Instructions
+*None*
+### Link
 *None*</v>
       </c>
       <c r="C17" s="42" t="str">
@@ -5308,11 +6773,15 @@
 ### Description
 ",IF(ISBLANK(Schedule!I18),"*None*",Schedule!I18),"
 ### Instructions
-",IF(ISBLANK(Schedule!J18),"*None*",Schedule!J18)))</f>
+",IF(ISBLANK(Schedule!J18),"*None*",Schedule!J18),"
+### Link
+",IF(ISBLANK(Schedule!K23),"*None*",Schedule!R23)))</f>
         <v xml:space="preserve">
 ### Description
 *None*
 ### Instructions
+*None*
+### Link
 *None*</v>
       </c>
     </row>
@@ -5335,7 +6804,9 @@
 ### Description
 ",IF(ISBLANK(Schedule!I19),"*None*",Schedule!I19),"
 ### Instructions
-",IF(ISBLANK(Schedule!J19),"*None*",Schedule!J19)))</f>
+",IF(ISBLANK(Schedule!J19),"*None*",Schedule!J19),"
+### Link
+",IF(ISBLANK(Schedule!K24),"*None*",Schedule!R24)))</f>
         <v/>
       </c>
     </row>
@@ -5358,7 +6829,9 @@
 ### Description
 ",IF(ISBLANK(Schedule!I20),"*None*",Schedule!I20),"
 ### Instructions
-",IF(ISBLANK(Schedule!J20),"*None*",Schedule!J20)))</f>
+",IF(ISBLANK(Schedule!J20),"*None*",Schedule!J20),"
+### Link
+",IF(ISBLANK(Schedule!K25),"*None*",Schedule!R25)))</f>
         <v/>
       </c>
     </row>
@@ -5381,7 +6854,9 @@
 ### Description
 ",IF(ISBLANK(Schedule!I21),"*None*",Schedule!I21),"
 ### Instructions
-",IF(ISBLANK(Schedule!J21),"*None*",Schedule!J21)))</f>
+",IF(ISBLANK(Schedule!J21),"*None*",Schedule!J21),"
+### Link
+",IF(ISBLANK(Schedule!K26),"*None*",Schedule!R26)))</f>
         <v/>
       </c>
     </row>
@@ -5404,7 +6879,9 @@
 ### Description
 ",IF(ISBLANK(Schedule!I22),"*None*",Schedule!I22),"
 ### Instructions
-",IF(ISBLANK(Schedule!J22),"*None*",Schedule!J22)))</f>
+",IF(ISBLANK(Schedule!J22),"*None*",Schedule!J22),"
+### Link
+",IF(ISBLANK(Schedule!K27),"*None*",Schedule!R27)))</f>
         <v/>
       </c>
     </row>
@@ -5427,7 +6904,9 @@
 ### Description
 ",IF(ISBLANK(Schedule!I23),"*None*",Schedule!I23),"
 ### Instructions
-",IF(ISBLANK(Schedule!J23),"*None*",Schedule!J23)))</f>
+",IF(ISBLANK(Schedule!J23),"*None*",Schedule!J23),"
+### Link
+",IF(ISBLANK(Schedule!K28),"*None*",Schedule!R28)))</f>
         <v/>
       </c>
     </row>
@@ -5450,7 +6929,9 @@
 ### Description
 ",IF(ISBLANK(Schedule!I24),"*None*",Schedule!I24),"
 ### Instructions
-",IF(ISBLANK(Schedule!J24),"*None*",Schedule!J24)))</f>
+",IF(ISBLANK(Schedule!J24),"*None*",Schedule!J24),"
+### Link
+",IF(ISBLANK(Schedule!K29),"*None*",Schedule!R29)))</f>
         <v/>
       </c>
     </row>
@@ -5466,6 +6947,8 @@
 ### Description
 *None*
 ### Instructions
+*None*
+### Link
 *None*</v>
       </c>
       <c r="C24" s="42" t="str">
@@ -5479,11 +6962,15 @@
 ### Description
 ",IF(ISBLANK(Schedule!I25),"*None*",Schedule!I25),"
 ### Instructions
-",IF(ISBLANK(Schedule!J25),"*None*",Schedule!J25)))</f>
+",IF(ISBLANK(Schedule!J25),"*None*",Schedule!J25),"
+### Link
+",IF(ISBLANK(Schedule!K30),"*None*",Schedule!R30)))</f>
         <v xml:space="preserve">
 ### Description
 *None*
 ### Instructions
+*None*
+### Link
 *None*</v>
       </c>
     </row>
@@ -5674,10 +7161,10 @@
       </c>
     </row>
     <row r="5" spans="1:2" ht="15.75" customHeight="1">
-      <c r="A5" s="96">
+      <c r="A5" s="98">
         <v>43709</v>
       </c>
-      <c r="B5" s="97"/>
+      <c r="B5" s="99"/>
     </row>
     <row r="6" spans="1:2" ht="15.75" customHeight="1">
       <c r="A6" s="6">
@@ -5720,10 +7207,10 @@
       </c>
     </row>
     <row r="11" spans="1:2" ht="15.75" customHeight="1">
-      <c r="A11" s="96">
+      <c r="A11" s="98">
         <v>43739</v>
       </c>
-      <c r="B11" s="97"/>
+      <c r="B11" s="99"/>
     </row>
     <row r="12" spans="1:2" ht="15.75" customHeight="1">
       <c r="A12" s="6">
@@ -5774,10 +7261,10 @@
       </c>
     </row>
     <row r="18" spans="1:2" ht="15.75" customHeight="1">
-      <c r="A18" s="96">
+      <c r="A18" s="98">
         <v>43770</v>
       </c>
-      <c r="B18" s="97"/>
+      <c r="B18" s="99"/>
     </row>
     <row r="19" spans="1:2" ht="15.75" customHeight="1">
       <c r="A19" s="8" t="s">
@@ -5844,10 +7331,10 @@
       </c>
     </row>
     <row r="27" spans="1:2" ht="15.75" customHeight="1">
-      <c r="A27" s="96">
+      <c r="A27" s="98">
         <v>43800</v>
       </c>
-      <c r="B27" s="97"/>
+      <c r="B27" s="99"/>
     </row>
     <row r="28" spans="1:2" ht="15.75" customHeight="1">
       <c r="A28" s="6">
@@ -5930,10 +7417,10 @@
       </c>
     </row>
     <row r="38" spans="1:2" ht="15.75" customHeight="1">
-      <c r="A38" s="96">
+      <c r="A38" s="98">
         <v>43831</v>
       </c>
-      <c r="B38" s="97"/>
+      <c r="B38" s="99"/>
     </row>
     <row r="39" spans="1:2" ht="15.75" customHeight="1">
       <c r="A39" s="8" t="s">
@@ -5984,10 +7471,10 @@
       </c>
     </row>
     <row r="45" spans="1:2" ht="15.75" customHeight="1">
-      <c r="A45" s="96">
+      <c r="A45" s="98">
         <v>43862</v>
       </c>
-      <c r="B45" s="97"/>
+      <c r="B45" s="99"/>
     </row>
     <row r="46" spans="1:2" ht="15.75" customHeight="1">
       <c r="A46" s="6">
@@ -6014,10 +7501,10 @@
       </c>
     </row>
     <row r="49" spans="1:2" ht="15.75" customHeight="1">
-      <c r="A49" s="96">
+      <c r="A49" s="98">
         <v>43891</v>
       </c>
-      <c r="B49" s="97"/>
+      <c r="B49" s="99"/>
     </row>
     <row r="50" spans="1:2" ht="15.75" customHeight="1">
       <c r="A50" s="6">
@@ -6092,10 +7579,10 @@
       </c>
     </row>
     <row r="59" spans="1:2" ht="15.75" customHeight="1">
-      <c r="A59" s="96">
+      <c r="A59" s="98">
         <v>43922</v>
       </c>
-      <c r="B59" s="97"/>
+      <c r="B59" s="99"/>
     </row>
     <row r="60" spans="1:2" ht="15.75" customHeight="1">
       <c r="A60" s="6">
@@ -6138,10 +7625,10 @@
       </c>
     </row>
     <row r="65" spans="1:2" ht="15.75" customHeight="1">
-      <c r="A65" s="96">
+      <c r="A65" s="98">
         <v>43952</v>
       </c>
-      <c r="B65" s="97"/>
+      <c r="B65" s="99"/>
     </row>
     <row r="66" spans="1:2" ht="15.75" customHeight="1">
       <c r="A66" s="8" t="s">
@@ -28503,11 +29990,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:R956"/>
   <sheetViews>
-    <sheetView zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <pane xSplit="5" ySplit="2" topLeftCell="G12" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <pane xSplit="5" ySplit="2" topLeftCell="F3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="G9" sqref="G9"/>
+      <selection pane="bottomRight" activeCell="T7" sqref="T7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.09765625" defaultRowHeight="15.6"/>
@@ -28528,21 +30015,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" s="43" customFormat="1" ht="18.3" customHeight="1">
-      <c r="A1" s="90"/>
-      <c r="B1" s="91"/>
-      <c r="C1" s="91"/>
-      <c r="D1" s="91"/>
-      <c r="E1" s="91"/>
-      <c r="F1" s="92" t="s">
+      <c r="A1" s="92"/>
+      <c r="B1" s="93"/>
+      <c r="C1" s="93"/>
+      <c r="D1" s="93"/>
+      <c r="E1" s="93"/>
+      <c r="F1" s="94" t="s">
         <v>863</v>
       </c>
-      <c r="G1" s="92"/>
-      <c r="H1" s="93" t="s">
+      <c r="G1" s="94"/>
+      <c r="H1" s="95" t="s">
         <v>873</v>
       </c>
-      <c r="I1" s="94"/>
-      <c r="J1" s="94"/>
-      <c r="K1" s="95"/>
+      <c r="I1" s="96"/>
+      <c r="J1" s="96"/>
+      <c r="K1" s="97"/>
       <c r="L1" s="49"/>
       <c r="M1" s="84"/>
       <c r="N1" s="80"/>
@@ -28642,8 +30129,8 @@
         <v>**Course Overview &amp; Introduction to the Data Science Lifecycle** &lt;br&gt; [more](https://rpi-data.github.io/course-intro-ml-app/sessions/session1/)</v>
       </c>
       <c r="R3" s="72" t="str">
-        <f t="shared" ref="R3:R34" si="1">CONCATENATE("[Link](",K3,")")</f>
-        <v>[Link]()</v>
+        <f>CONCATENATE("[Assignment ",H3,"](",K3,")")</f>
+        <v>[Assignment ]()</v>
       </c>
     </row>
     <row r="4" spans="1:18" ht="15.6" customHeight="1">
@@ -28677,7 +30164,7 @@
         <v/>
       </c>
       <c r="P4" s="72" t="str">
-        <f t="shared" ref="P4:P35" si="2">IF(ISBLANK(H4),"",CONCATENATE(" &lt;br&gt; *",N4,"* &lt;br&gt;"))</f>
+        <f t="shared" ref="P4:P35" si="1">IF(ISBLANK(H4),"",CONCATENATE(" &lt;br&gt; *",N4,"* &lt;br&gt;"))</f>
         <v/>
       </c>
       <c r="Q4" s="72" t="str">
@@ -28685,8 +30172,8 @@
         <v xml:space="preserve">**Labor Day - no classes (Tuesday follows Monday schedule)** &lt;br&gt; </v>
       </c>
       <c r="R4" s="72" t="str">
-        <f t="shared" si="1"/>
-        <v>[Link]()</v>
+        <f t="shared" ref="R4:R34" si="2">CONCATENATE("[Assignment ",H4,"](",K4,")")</f>
+        <v>[Assignment ]()</v>
       </c>
     </row>
     <row r="5" spans="1:18" ht="124.8">
@@ -28719,7 +30206,7 @@
         <v>99</v>
       </c>
       <c r="J5" s="63"/>
-      <c r="K5" s="99" t="s">
+      <c r="K5" s="90" t="s">
         <v>761</v>
       </c>
       <c r="L5" s="79" t="b">
@@ -28737,7 +30224,7 @@
         <v>[more](https://rpi-data.github.io/course-intro-ml-app/sessions/session2/)</v>
       </c>
       <c r="P5" s="72" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v xml:space="preserve"> &lt;br&gt; *Assignment 1 due 09/17* &lt;br&gt;</v>
       </c>
       <c r="Q5" s="72" t="str">
@@ -28745,8 +30232,8 @@
         <v>**Python Basics** &lt;br&gt; [more](https://rpi-data.github.io/course-intro-ml-app/sessions/session2/) &lt;br&gt; *Assignment 1 due 09/17* &lt;br&gt;</v>
       </c>
       <c r="R5" s="72" t="str">
-        <f t="shared" si="1"/>
-        <v>[Link](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/02-intro-python/hm-01/hm01.ipynb)</v>
+        <f t="shared" si="2"/>
+        <v>[Assignment 1](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/02-intro-python/hm-01/hm01.ipynb)</v>
       </c>
     </row>
     <row r="6" spans="1:18">
@@ -28786,7 +30273,7 @@
         <v>[more](https://rpi-data.github.io/course-intro-ml-app/sessions/session3/)</v>
       </c>
       <c r="P6" s="72" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="Q6" s="72" t="str">
@@ -28794,8 +30281,8 @@
         <v>**Python Basics** &lt;br&gt; [more](https://rpi-data.github.io/course-intro-ml-app/sessions/session3/)</v>
       </c>
       <c r="R6" s="72" t="str">
-        <f t="shared" si="1"/>
-        <v>[Link]()</v>
+        <f t="shared" si="2"/>
+        <v>[Assignment ]()</v>
       </c>
     </row>
     <row r="7" spans="1:18" ht="140.4">
@@ -28836,7 +30323,7 @@
         <v>[more](https://rpi-data.github.io/course-intro-ml-app/sessions/session4/)</v>
       </c>
       <c r="P7" s="72" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="Q7" s="72" t="str">
@@ -28844,8 +30331,8 @@
         <v>**Python conditionals, loops, functions, aggregating.** &lt;br&gt; [more](https://rpi-data.github.io/course-intro-ml-app/sessions/session4/)</v>
       </c>
       <c r="R7" s="72" t="str">
-        <f t="shared" si="1"/>
-        <v>[Link]()</v>
+        <f t="shared" si="2"/>
+        <v>[Assignment ]()</v>
       </c>
     </row>
     <row r="8" spans="1:18" ht="46.8">
@@ -28874,7 +30361,7 @@
       <c r="H8" s="58">
         <v>2</v>
       </c>
-      <c r="K8" s="99" t="s">
+      <c r="K8" s="90" t="s">
         <v>826</v>
       </c>
       <c r="L8" s="51" t="b">
@@ -28892,7 +30379,7 @@
         <v>[more](https://rpi-data.github.io/course-intro-ml-app/sessions/session5/)</v>
       </c>
       <c r="P8" s="72" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v xml:space="preserve"> &lt;br&gt; *Assignment 2 due 09/26* &lt;br&gt;</v>
       </c>
       <c r="Q8" s="72" t="str">
@@ -28900,8 +30387,8 @@
         <v>**Python conditionals, loops, functions, aggregating (continued)** &lt;br&gt; [more](https://rpi-data.github.io/course-intro-ml-app/sessions/session5/) &lt;br&gt; *Assignment 2 due 09/26* &lt;br&gt;</v>
       </c>
       <c r="R8" s="72" t="str">
-        <f t="shared" si="1"/>
-        <v>[Link](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/03-python/hm-02/hm02.ipynb)</v>
+        <f t="shared" si="2"/>
+        <v>[Assignment 2](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/03-python/hm-02/hm02.ipynb)</v>
       </c>
     </row>
     <row r="9" spans="1:18" ht="93.6">
@@ -28942,7 +30429,7 @@
         <v>[more](https://rpi-data.github.io/course-intro-ml-app/sessions/session6/)</v>
       </c>
       <c r="P9" s="72" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="Q9" s="72" t="str">
@@ -28950,8 +30437,8 @@
         <v>**Python visualization, data manipulation , and feature creation.** &lt;br&gt; [more](https://rpi-data.github.io/course-intro-ml-app/sessions/session6/)</v>
       </c>
       <c r="R9" s="72" t="str">
-        <f t="shared" si="1"/>
-        <v>[Link]()</v>
+        <f t="shared" si="2"/>
+        <v>[Assignment ]()</v>
       </c>
     </row>
     <row r="10" spans="1:18" ht="46.8">
@@ -28980,7 +30467,7 @@
       <c r="H10" s="58">
         <v>3</v>
       </c>
-      <c r="K10" s="99" t="s">
+      <c r="K10" s="90" t="s">
         <v>838</v>
       </c>
       <c r="L10" s="51" t="b">
@@ -28998,7 +30485,7 @@
         <v>[more](https://rpi-data.github.io/course-intro-ml-app/sessions/session7/)</v>
       </c>
       <c r="P10" s="72" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v xml:space="preserve"> &lt;br&gt; *Assignment 3 due 10/03* &lt;br&gt;</v>
       </c>
       <c r="Q10" s="72" t="str">
@@ -29006,8 +30493,8 @@
         <v>**Python visualization, data manipulation , and feature creation (continued)** &lt;br&gt; [more](https://rpi-data.github.io/course-intro-ml-app/sessions/session7/) &lt;br&gt; *Assignment 3 due 10/03* &lt;br&gt;</v>
       </c>
       <c r="R10" s="72" t="str">
-        <f t="shared" si="1"/>
-        <v>[Link](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/04-viz-api-scraper/hm-03/hm03.ipynb)</v>
+        <f t="shared" si="2"/>
+        <v>[Assignment 3](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/04-viz-api-scraper/hm-03/hm03.ipynb)</v>
       </c>
     </row>
     <row r="11" spans="1:18" ht="31.2">
@@ -29048,7 +30535,7 @@
         <v>[more](https://rpi-data.github.io/course-intro-ml-app/sessions/session8/)</v>
       </c>
       <c r="P11" s="72" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="Q11" s="72" t="str">
@@ -29056,8 +30543,8 @@
         <v>**Visualization with Tableau** &lt;br&gt; [more](https://rpi-data.github.io/course-intro-ml-app/sessions/session8/)</v>
       </c>
       <c r="R11" s="72" t="str">
-        <f t="shared" si="1"/>
-        <v>[Link]()</v>
+        <f t="shared" si="2"/>
+        <v>[Assignment ]()</v>
       </c>
     </row>
     <row r="12" spans="1:18">
@@ -29101,7 +30588,7 @@
         <v>[more](https://rpi-data.github.io/course-intro-ml-app/sessions/session9/)</v>
       </c>
       <c r="P12" s="72" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v xml:space="preserve"> &lt;br&gt; *Assignment 4 due 10/10* &lt;br&gt;</v>
       </c>
       <c r="Q12" s="72" t="str">
@@ -29109,8 +30596,8 @@
         <v>**Visualization with Tableau** &lt;br&gt; [more](https://rpi-data.github.io/course-intro-ml-app/sessions/session9/) &lt;br&gt; *Assignment 4 due 10/10* &lt;br&gt;</v>
       </c>
       <c r="R12" s="72" t="str">
-        <f t="shared" si="1"/>
-        <v>[Link]()</v>
+        <f t="shared" si="2"/>
+        <v>[Assignment 4]()</v>
       </c>
     </row>
     <row r="13" spans="1:18" ht="93.6">
@@ -29151,7 +30638,7 @@
         <v>[more](https://rpi-data.github.io/course-intro-ml-app/sessions/session10/)</v>
       </c>
       <c r="P13" s="72" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="Q13" s="72" t="str">
@@ -29159,8 +30646,8 @@
         <v>**Introduction to R** &lt;br&gt; [more](https://rpi-data.github.io/course-intro-ml-app/sessions/session10/)</v>
       </c>
       <c r="R13" s="72" t="str">
-        <f t="shared" si="1"/>
-        <v>[Link]()</v>
+        <f t="shared" si="2"/>
+        <v>[Assignment ]()</v>
       </c>
     </row>
     <row r="14" spans="1:18">
@@ -29203,7 +30690,7 @@
         <v>[more](https://rpi-data.github.io/course-intro-ml-app/sessions/session11/)</v>
       </c>
       <c r="P14" s="72" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v xml:space="preserve"> &lt;br&gt; *Assignment 5 due 10/17* &lt;br&gt;</v>
       </c>
       <c r="Q14" s="72" t="str">
@@ -29211,8 +30698,8 @@
         <v>**Introduction to R** &lt;br&gt; [more](https://rpi-data.github.io/course-intro-ml-app/sessions/session11/) &lt;br&gt; *Assignment 5 due 10/17* &lt;br&gt;</v>
       </c>
       <c r="R14" s="72" t="str">
-        <f t="shared" si="1"/>
-        <v>[Link]()</v>
+        <f t="shared" si="2"/>
+        <v>[Assignment 5]()</v>
       </c>
     </row>
     <row r="15" spans="1:18" ht="93.6">
@@ -29238,7 +30725,7 @@
         <v>639</v>
       </c>
       <c r="G15" s="69"/>
-      <c r="L15" s="98" t="b">
+      <c r="L15" s="89" t="b">
         <v>1</v>
       </c>
       <c r="M15" s="86" t="b">
@@ -29253,7 +30740,7 @@
         <v>[more](https://rpi-data.github.io/course-intro-ml-app/sessions/session12/)</v>
       </c>
       <c r="P15" s="72" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="Q15" s="72" t="str">
@@ -29261,8 +30748,8 @@
         <v>**Overview of Modeling** &lt;br&gt; [more](https://rpi-data.github.io/course-intro-ml-app/sessions/session12/)</v>
       </c>
       <c r="R15" s="72" t="str">
-        <f t="shared" si="1"/>
-        <v>[Link]()</v>
+        <f t="shared" si="2"/>
+        <v>[Assignment ]()</v>
       </c>
     </row>
     <row r="16" spans="1:18">
@@ -29305,7 +30792,7 @@
         <v>[more](https://rpi-data.github.io/course-intro-ml-app/sessions/session13/)</v>
       </c>
       <c r="P16" s="72" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v xml:space="preserve"> &lt;br&gt; *Assignment 6 due 10/24* &lt;br&gt;</v>
       </c>
       <c r="Q16" s="72" t="str">
@@ -29313,8 +30800,8 @@
         <v>**Overview of Modeling** &lt;br&gt; [more](https://rpi-data.github.io/course-intro-ml-app/sessions/session13/) &lt;br&gt; *Assignment 6 due 10/24* &lt;br&gt;</v>
       </c>
       <c r="R16" s="72" t="str">
-        <f t="shared" si="1"/>
-        <v>[Link]()</v>
+        <f t="shared" si="2"/>
+        <v>[Assignment 6]()</v>
       </c>
     </row>
     <row r="17" spans="1:18" ht="31.2">
@@ -29353,7 +30840,7 @@
         <v>[more](https://rpi-data.github.io/course-intro-ml-app/sessions/session14/)</v>
       </c>
       <c r="P17" s="72" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="Q17" s="72" t="str">
@@ -29361,8 +30848,8 @@
         <v>**Review/Kaggle Project Introduction** &lt;br&gt; [more](https://rpi-data.github.io/course-intro-ml-app/sessions/session14/)</v>
       </c>
       <c r="R17" s="72" t="str">
-        <f t="shared" si="1"/>
-        <v>[Link]()</v>
+        <f t="shared" si="2"/>
+        <v>[Assignment ]()</v>
       </c>
     </row>
     <row r="18" spans="1:18">
@@ -29402,7 +30889,7 @@
         <v>[more](https://rpi-data.github.io/course-intro-ml-app/sessions/session15/)</v>
       </c>
       <c r="P18" s="72" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v xml:space="preserve"> &lt;br&gt; *Assignment 7 due 10/31* &lt;br&gt;</v>
       </c>
       <c r="Q18" s="72" t="str">
@@ -29410,8 +30897,8 @@
         <v>**Midterm** &lt;br&gt; [more](https://rpi-data.github.io/course-intro-ml-app/sessions/session15/) &lt;br&gt; *Assignment 7 due 10/31* &lt;br&gt;</v>
       </c>
       <c r="R18" s="72" t="str">
-        <f t="shared" si="1"/>
-        <v>[Link]()</v>
+        <f t="shared" si="2"/>
+        <v>[Assignment 7]()</v>
       </c>
     </row>
     <row r="19" spans="1:18" ht="46.8">
@@ -29452,7 +30939,7 @@
         <v>[more](https://rpi-data.github.io/course-intro-ml-app/sessions/session16/)</v>
       </c>
       <c r="P19" s="72" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="Q19" s="72" t="str">
@@ -29460,8 +30947,8 @@
         <v>**Classification** &lt;br&gt; [more](https://rpi-data.github.io/course-intro-ml-app/sessions/session16/)</v>
       </c>
       <c r="R19" s="72" t="str">
-        <f t="shared" si="1"/>
-        <v>[Link]()</v>
+        <f t="shared" si="2"/>
+        <v>[Assignment ]()</v>
       </c>
     </row>
     <row r="20" spans="1:18">
@@ -29502,7 +30989,7 @@
         <v>[more](https://rpi-data.github.io/course-intro-ml-app/sessions/session17/)</v>
       </c>
       <c r="P20" s="72" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="Q20" s="72" t="str">
@@ -29510,8 +30997,8 @@
         <v>**Classification** &lt;br&gt; [more](https://rpi-data.github.io/course-intro-ml-app/sessions/session17/)</v>
       </c>
       <c r="R20" s="72" t="str">
-        <f t="shared" si="1"/>
-        <v>[Link]()</v>
+        <f t="shared" si="2"/>
+        <v>[Assignment ]()</v>
       </c>
     </row>
     <row r="21" spans="1:18" ht="31.2">
@@ -29552,7 +31039,7 @@
         <v>[more](https://rpi-data.github.io/course-intro-ml-app/sessions/session18/)</v>
       </c>
       <c r="P21" s="72" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="Q21" s="72" t="str">
@@ -29560,8 +31047,8 @@
         <v>**Regression** &lt;br&gt; [more](https://rpi-data.github.io/course-intro-ml-app/sessions/session18/)</v>
       </c>
       <c r="R21" s="72" t="str">
-        <f t="shared" si="1"/>
-        <v>[Link]()</v>
+        <f t="shared" si="2"/>
+        <v>[Assignment ]()</v>
       </c>
     </row>
     <row r="22" spans="1:18">
@@ -29602,7 +31089,7 @@
         <v>[more](https://rpi-data.github.io/course-intro-ml-app/sessions/session19/)</v>
       </c>
       <c r="P22" s="72" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="Q22" s="72" t="str">
@@ -29610,8 +31097,8 @@
         <v>**Regression** &lt;br&gt; [more](https://rpi-data.github.io/course-intro-ml-app/sessions/session19/)</v>
       </c>
       <c r="R22" s="72" t="str">
-        <f t="shared" si="1"/>
-        <v>[Link]()</v>
+        <f t="shared" si="2"/>
+        <v>[Assignment ]()</v>
       </c>
     </row>
     <row r="23" spans="1:18" ht="31.2">
@@ -29652,7 +31139,7 @@
         <v>[more](https://rpi-data.github.io/course-intro-ml-app/sessions/session20/)</v>
       </c>
       <c r="P23" s="72" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="Q23" s="72" t="str">
@@ -29660,8 +31147,8 @@
         <v>**Text and NLP** &lt;br&gt; [more](https://rpi-data.github.io/course-intro-ml-app/sessions/session20/)</v>
       </c>
       <c r="R23" s="72" t="str">
-        <f t="shared" si="1"/>
-        <v>[Link]()</v>
+        <f t="shared" si="2"/>
+        <v>[Assignment ]()</v>
       </c>
     </row>
     <row r="24" spans="1:18">
@@ -29702,7 +31189,7 @@
         <v>[more](https://rpi-data.github.io/course-intro-ml-app/sessions/session21/)</v>
       </c>
       <c r="P24" s="72" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="Q24" s="72" t="str">
@@ -29710,8 +31197,8 @@
         <v>**Text and NLP** &lt;br&gt; [more](https://rpi-data.github.io/course-intro-ml-app/sessions/session21/)</v>
       </c>
       <c r="R24" s="72" t="str">
-        <f t="shared" si="1"/>
-        <v>[Link]()</v>
+        <f t="shared" si="2"/>
+        <v>[Assignment ]()</v>
       </c>
     </row>
     <row r="25" spans="1:18" ht="46.8">
@@ -29755,7 +31242,7 @@
         <v>[more](https://rpi-data.github.io/course-intro-ml-app/sessions/session22/)</v>
       </c>
       <c r="P25" s="72" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v xml:space="preserve"> &lt;br&gt; *Assignment 8 due 11/25* &lt;br&gt;</v>
       </c>
       <c r="Q25" s="72" t="str">
@@ -29763,8 +31250,8 @@
         <v>**Introduction to Big Data** &lt;br&gt; [more](https://rpi-data.github.io/course-intro-ml-app/sessions/session22/) &lt;br&gt; *Assignment 8 due 11/25* &lt;br&gt;</v>
       </c>
       <c r="R25" s="72" t="str">
-        <f t="shared" si="1"/>
-        <v>[Link]()</v>
+        <f t="shared" si="2"/>
+        <v>[Assignment 8]()</v>
       </c>
     </row>
     <row r="26" spans="1:18" ht="46.8">
@@ -29805,7 +31292,7 @@
         <v>[more](https://rpi-data.github.io/course-intro-ml-app/sessions/session23/)</v>
       </c>
       <c r="P26" s="72" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="Q26" s="72" t="str">
@@ -29813,8 +31300,8 @@
         <v>**Time Series Analysis** &lt;br&gt; [more](https://rpi-data.github.io/course-intro-ml-app/sessions/session23/)</v>
       </c>
       <c r="R26" s="72" t="str">
-        <f t="shared" si="1"/>
-        <v>[Link]()</v>
+        <f t="shared" si="2"/>
+        <v>[Assignment ]()</v>
       </c>
     </row>
     <row r="27" spans="1:18" ht="78">
@@ -29855,7 +31342,7 @@
         <v>[more](https://rpi-data.github.io/course-intro-ml-app/sessions/session24/)</v>
       </c>
       <c r="P27" s="72" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="Q27" s="72" t="str">
@@ -29863,8 +31350,8 @@
         <v>**Image Data and Deep Learning** &lt;br&gt; [more](https://rpi-data.github.io/course-intro-ml-app/sessions/session24/)</v>
       </c>
       <c r="R27" s="72" t="str">
-        <f t="shared" si="1"/>
-        <v>[Link]()</v>
+        <f t="shared" si="2"/>
+        <v>[Assignment ]()</v>
       </c>
     </row>
     <row r="28" spans="1:18" ht="31.2">
@@ -29905,7 +31392,7 @@
         <v>[more](https://rpi-data.github.io/course-intro-ml-app/sessions/session25/)</v>
       </c>
       <c r="P28" s="72" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="Q28" s="72" t="str">
@@ -29913,8 +31400,8 @@
         <v>**Image Data and Deep Learning** &lt;br&gt; [more](https://rpi-data.github.io/course-intro-ml-app/sessions/session25/)</v>
       </c>
       <c r="R28" s="72" t="str">
-        <f t="shared" si="1"/>
-        <v>[Link]()</v>
+        <f t="shared" si="2"/>
+        <v>[Assignment ]()</v>
       </c>
     </row>
     <row r="29" spans="1:18" ht="31.2">
@@ -29955,7 +31442,7 @@
         <v>[more](https://rpi-data.github.io/course-intro-ml-app/sessions/session26/)</v>
       </c>
       <c r="P29" s="72" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="Q29" s="72" t="str">
@@ -29963,8 +31450,8 @@
         <v>**Automl and Modeling Packages** &lt;br&gt; [more](https://rpi-data.github.io/course-intro-ml-app/sessions/session26/)</v>
       </c>
       <c r="R29" s="72" t="str">
-        <f t="shared" si="1"/>
-        <v>[Link]()</v>
+        <f t="shared" si="2"/>
+        <v>[Assignment ]()</v>
       </c>
     </row>
     <row r="30" spans="1:18">
@@ -29999,7 +31486,7 @@
         <v/>
       </c>
       <c r="P30" s="72" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="Q30" s="72" t="str">
@@ -30007,8 +31494,8 @@
         <v xml:space="preserve">**Thanksgiving** &lt;br&gt; </v>
       </c>
       <c r="R30" s="72" t="str">
-        <f t="shared" si="1"/>
-        <v>[Link]()</v>
+        <f t="shared" si="2"/>
+        <v>[Assignment ]()</v>
       </c>
     </row>
     <row r="31" spans="1:18">
@@ -30048,7 +31535,7 @@
         <v>[more](https://rpi-data.github.io/course-intro-ml-app/sessions/session27/)</v>
       </c>
       <c r="P31" s="72" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="Q31" s="72" t="str">
@@ -30056,8 +31543,8 @@
         <v>**Automl and Model Search** &lt;br&gt; [more](https://rpi-data.github.io/course-intro-ml-app/sessions/session27/)</v>
       </c>
       <c r="R31" s="72" t="str">
-        <f t="shared" si="1"/>
-        <v>[Link]()</v>
+        <f t="shared" si="2"/>
+        <v>[Assignment ]()</v>
       </c>
     </row>
     <row r="32" spans="1:18">
@@ -30096,7 +31583,7 @@
         <v>[more](https://rpi-data.github.io/course-intro-ml-app/sessions/session28/)</v>
       </c>
       <c r="P32" s="72" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="Q32" s="72" t="str">
@@ -30104,8 +31591,8 @@
         <v>**Final Presentations** &lt;br&gt; [more](https://rpi-data.github.io/course-intro-ml-app/sessions/session28/)</v>
       </c>
       <c r="R32" s="72" t="str">
-        <f t="shared" si="1"/>
-        <v>[Link]()</v>
+        <f t="shared" si="2"/>
+        <v>[Assignment ]()</v>
       </c>
     </row>
     <row r="33" spans="1:18">
@@ -30143,7 +31630,7 @@
         <v>[more](https://rpi-data.github.io/course-intro-ml-app/sessions/session29/)</v>
       </c>
       <c r="P33" s="72" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="Q33" s="72" t="str">
@@ -30151,8 +31638,8 @@
         <v>**Final Presentations** &lt;br&gt; [more](https://rpi-data.github.io/course-intro-ml-app/sessions/session29/)</v>
       </c>
       <c r="R33" s="72" t="str">
-        <f t="shared" si="1"/>
-        <v>[Link]()</v>
+        <f t="shared" si="2"/>
+        <v>[Assignment ]()</v>
       </c>
     </row>
     <row r="34" spans="1:18">
@@ -30185,7 +31672,7 @@
         <v/>
       </c>
       <c r="P34" s="72" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="Q34" s="72" t="str">
@@ -30193,8 +31680,8 @@
         <v xml:space="preserve">**Final Exam** &lt;br&gt; </v>
       </c>
       <c r="R34" s="72" t="str">
-        <f t="shared" si="1"/>
-        <v>[Link]()</v>
+        <f t="shared" si="2"/>
+        <v>[Assignment ]()</v>
       </c>
     </row>
     <row r="35" spans="1:18">
@@ -30207,7 +31694,7 @@
         <v/>
       </c>
       <c r="P35" s="72" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>

</xml_diff>

<commit_message>
Fix convert notebook and session entries
</commit_message>
<xml_diff>
--- a/book.xlsx
+++ b/book.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sjgar\Documents\GitHub\course-intro-ml-app\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{132D947C-7146-44DE-889D-FE4D5A3FFEE4}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C3F436B-A0BC-41F4-ABE9-55730686E879}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="12504" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,9 +27,8 @@
     <sheet name="notebooks_md" sheetId="12" state="hidden" r:id="rId12"/>
     <sheet name="assignments_md" sheetId="13" state="hidden" r:id="rId13"/>
     <sheet name="session_md" sheetId="4" state="hidden" r:id="rId14"/>
-    <sheet name="assign_md" sheetId="23" state="hidden" r:id="rId15"/>
-    <sheet name="grading_md" sheetId="15" state="hidden" r:id="rId16"/>
-    <sheet name="Sheet1" sheetId="6" state="hidden" r:id="rId17"/>
+    <sheet name="grading_md" sheetId="15" state="hidden" r:id="rId15"/>
+    <sheet name="Sheet1" sheetId="6" state="hidden" r:id="rId16"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -43,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4141" uniqueCount="906">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4137" uniqueCount="906">
   <si>
     <t>Wk</t>
   </si>
@@ -2286,9 +2285,6 @@
     <t>Pandas</t>
   </si>
   <si>
-    <t>Lab</t>
-  </si>
-  <si>
     <t>https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/02-intro-python/01-intro-python-overview.ipynb</t>
   </si>
   <si>
@@ -2298,9 +2294,6 @@
     <t>https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/02-intro-python/04-intro-python-pandas.ipynb</t>
   </si>
   <si>
-    <t>https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/02-intro-python/lab/lab.ipynb</t>
-  </si>
-  <si>
     <t>https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/02-intro-python/hm-01/hm01.ipynb</t>
   </si>
   <si>
@@ -2485,9 +2478,6 @@
   </si>
   <si>
     <t>Assignment 2</t>
-  </si>
-  <si>
-    <t>Assignment 1</t>
   </si>
   <si>
     <t>https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/03-python/04-intro-python-groupby.ipynb</t>
@@ -2899,6 +2889,15 @@
   </si>
   <si>
     <t xml:space="preserve"> (Whether to add numbers to chapters in your Table of Contents. If true, you can control this at the Chapter level below)</t>
+  </si>
+  <si>
+    <t>Session entries</t>
+  </si>
+  <si>
+    <t>Session entries (grouped)</t>
+  </si>
+  <si>
+    <t>Session entries (per section)</t>
   </si>
 </sst>
 </file>
@@ -3344,7 +3343,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="117">
+  <cellXfs count="120">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -3533,6 +3532,13 @@
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
     <xf numFmtId="49" fontId="5" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -3935,7 +3941,7 @@
   <dimension ref="A1:F55"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="B52" sqref="B52"/>
+      <selection activeCell="B42" sqref="B42:E42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.09765625" defaultRowHeight="15" customHeight="1"/>
@@ -3955,56 +3961,56 @@
       <c r="A2" s="29" t="s">
         <v>656</v>
       </c>
-      <c r="B2" s="94" t="s">
-        <v>863</v>
-      </c>
-      <c r="C2" s="94"/>
-      <c r="D2" s="94"/>
-      <c r="E2" s="94"/>
+      <c r="B2" s="97" t="s">
+        <v>860</v>
+      </c>
+      <c r="C2" s="97"/>
+      <c r="D2" s="97"/>
+      <c r="E2" s="97"/>
     </row>
     <row r="3" spans="1:5" s="4" customFormat="1" ht="15" customHeight="1">
       <c r="A3" s="9" t="s">
         <v>691</v>
       </c>
-      <c r="B3" s="92" t="s">
+      <c r="B3" s="95" t="s">
         <v>672</v>
       </c>
-      <c r="C3" s="92"/>
-      <c r="D3" s="92"/>
-      <c r="E3" s="92"/>
+      <c r="C3" s="95"/>
+      <c r="D3" s="95"/>
+      <c r="E3" s="95"/>
     </row>
     <row r="4" spans="1:5" s="4" customFormat="1" ht="15" customHeight="1">
       <c r="A4" s="9" t="s">
         <v>694</v>
       </c>
-      <c r="B4" s="92" t="s">
+      <c r="B4" s="95" t="s">
         <v>692</v>
       </c>
-      <c r="C4" s="92"/>
-      <c r="D4" s="92"/>
-      <c r="E4" s="92"/>
+      <c r="C4" s="95"/>
+      <c r="D4" s="95"/>
+      <c r="E4" s="95"/>
     </row>
     <row r="5" spans="1:5" s="4" customFormat="1" ht="15" customHeight="1">
       <c r="A5" s="9" t="s">
         <v>693</v>
       </c>
-      <c r="B5" s="92" t="s">
+      <c r="B5" s="95" t="s">
         <v>695</v>
       </c>
-      <c r="C5" s="92"/>
-      <c r="D5" s="92"/>
-      <c r="E5" s="92"/>
+      <c r="C5" s="95"/>
+      <c r="D5" s="95"/>
+      <c r="E5" s="95"/>
     </row>
     <row r="6" spans="1:5" ht="15" customHeight="1">
       <c r="A6" s="1" t="s">
         <v>696</v>
       </c>
-      <c r="B6" s="93">
+      <c r="B6" s="96">
         <v>14</v>
       </c>
-      <c r="C6" s="93"/>
-      <c r="D6" s="93"/>
-      <c r="E6" s="93"/>
+      <c r="C6" s="96"/>
+      <c r="D6" s="96"/>
+      <c r="E6" s="96"/>
     </row>
     <row r="7" spans="1:5" s="29" customFormat="1" ht="15" customHeight="1">
       <c r="A7" s="1"/>
@@ -4014,54 +4020,54 @@
       <c r="A8" s="1" t="s">
         <v>678</v>
       </c>
-      <c r="B8" s="92" t="s">
+      <c r="B8" s="95" t="s">
         <v>673</v>
       </c>
-      <c r="C8" s="92"/>
-      <c r="D8" s="92"/>
-      <c r="E8" s="92"/>
+      <c r="C8" s="95"/>
+      <c r="D8" s="95"/>
+      <c r="E8" s="95"/>
     </row>
     <row r="9" spans="1:5" s="4" customFormat="1" ht="15" customHeight="1">
       <c r="A9" s="1" t="s">
         <v>679</v>
       </c>
-      <c r="B9" s="91" t="s">
+      <c r="B9" s="94" t="s">
         <v>675</v>
       </c>
-      <c r="C9" s="91"/>
-      <c r="D9" s="91"/>
-      <c r="E9" s="91"/>
+      <c r="C9" s="94"/>
+      <c r="D9" s="94"/>
+      <c r="E9" s="94"/>
     </row>
     <row r="10" spans="1:5" s="4" customFormat="1" ht="15" customHeight="1">
       <c r="A10" s="1" t="s">
         <v>680</v>
       </c>
-      <c r="B10" s="93" t="s">
+      <c r="B10" s="96" t="s">
         <v>683</v>
       </c>
-      <c r="C10" s="93"/>
-      <c r="D10" s="93"/>
-      <c r="E10" s="93"/>
+      <c r="C10" s="96"/>
+      <c r="D10" s="96"/>
+      <c r="E10" s="96"/>
     </row>
     <row r="11" spans="1:5" s="29" customFormat="1" ht="15" customHeight="1">
       <c r="A11" s="1" t="s">
-        <v>865</v>
-      </c>
-      <c r="B11" s="93"/>
-      <c r="C11" s="93"/>
-      <c r="D11" s="93"/>
-      <c r="E11" s="93"/>
+        <v>862</v>
+      </c>
+      <c r="B11" s="96"/>
+      <c r="C11" s="96"/>
+      <c r="D11" s="96"/>
+      <c r="E11" s="96"/>
     </row>
     <row r="12" spans="1:5" s="4" customFormat="1" ht="15" customHeight="1">
       <c r="A12" s="1" t="s">
         <v>681</v>
       </c>
-      <c r="B12" s="93" t="s">
+      <c r="B12" s="96" t="s">
         <v>684</v>
       </c>
-      <c r="C12" s="93"/>
-      <c r="D12" s="93"/>
-      <c r="E12" s="93"/>
+      <c r="C12" s="96"/>
+      <c r="D12" s="96"/>
+      <c r="E12" s="96"/>
     </row>
     <row r="13" spans="1:5" s="29" customFormat="1" ht="15" customHeight="1">
       <c r="A13" s="1"/>
@@ -4071,52 +4077,52 @@
       <c r="A14" s="1" t="s">
         <v>682</v>
       </c>
-      <c r="B14" s="93" t="s">
+      <c r="B14" s="96" t="s">
         <v>685</v>
       </c>
-      <c r="C14" s="93"/>
-      <c r="D14" s="93"/>
-      <c r="E14" s="93"/>
+      <c r="C14" s="96"/>
+      <c r="D14" s="96"/>
+      <c r="E14" s="96"/>
     </row>
     <row r="15" spans="1:5" s="4" customFormat="1" ht="15" customHeight="1">
       <c r="A15" s="1" t="s">
         <v>679</v>
       </c>
-      <c r="B15" s="91" t="s">
+      <c r="B15" s="94" t="s">
         <v>686</v>
       </c>
-      <c r="C15" s="91"/>
-      <c r="D15" s="91"/>
-      <c r="E15" s="91"/>
+      <c r="C15" s="94"/>
+      <c r="D15" s="94"/>
+      <c r="E15" s="94"/>
     </row>
     <row r="16" spans="1:5" s="4" customFormat="1" ht="15" customHeight="1">
       <c r="A16" s="1" t="s">
         <v>680</v>
       </c>
-      <c r="B16" s="93" t="s">
+      <c r="B16" s="96" t="s">
         <v>687</v>
       </c>
-      <c r="C16" s="93"/>
-      <c r="D16" s="93"/>
-      <c r="E16" s="93"/>
+      <c r="C16" s="96"/>
+      <c r="D16" s="96"/>
+      <c r="E16" s="96"/>
     </row>
     <row r="17" spans="1:6" s="29" customFormat="1" ht="15" customHeight="1">
       <c r="A17" s="1" t="s">
-        <v>865</v>
-      </c>
-      <c r="B17" s="93"/>
-      <c r="C17" s="93"/>
-      <c r="D17" s="93"/>
-      <c r="E17" s="93"/>
+        <v>862</v>
+      </c>
+      <c r="B17" s="96"/>
+      <c r="C17" s="96"/>
+      <c r="D17" s="96"/>
+      <c r="E17" s="96"/>
     </row>
     <row r="18" spans="1:6" s="29" customFormat="1" ht="15" customHeight="1">
       <c r="A18" s="1" t="s">
         <v>681</v>
       </c>
-      <c r="B18" s="93"/>
-      <c r="C18" s="93"/>
-      <c r="D18" s="93"/>
-      <c r="E18" s="93"/>
+      <c r="B18" s="96"/>
+      <c r="C18" s="96"/>
+      <c r="D18" s="96"/>
+      <c r="E18" s="96"/>
     </row>
     <row r="19" spans="1:6" s="29" customFormat="1" ht="15" customHeight="1">
       <c r="A19" s="1"/>
@@ -4126,12 +4132,12 @@
       <c r="A20" s="22" t="s">
         <v>688</v>
       </c>
-      <c r="B20" s="95" t="s">
+      <c r="B20" s="98" t="s">
         <v>689</v>
       </c>
-      <c r="C20" s="95"/>
-      <c r="D20" s="95"/>
-      <c r="E20" s="95"/>
+      <c r="C20" s="98"/>
+      <c r="D20" s="98"/>
+      <c r="E20" s="98"/>
     </row>
     <row r="21" spans="1:6" s="29" customFormat="1" ht="14.7" customHeight="1">
       <c r="A21" s="22"/>
@@ -4142,32 +4148,32 @@
     </row>
     <row r="22" spans="1:6" s="4" customFormat="1" ht="99" customHeight="1">
       <c r="A22" s="22" t="s">
-        <v>861</v>
-      </c>
-      <c r="B22" s="95" t="s">
+        <v>858</v>
+      </c>
+      <c r="B22" s="98" t="s">
         <v>697</v>
       </c>
-      <c r="C22" s="95"/>
-      <c r="D22" s="95"/>
-      <c r="E22" s="95"/>
+      <c r="C22" s="98"/>
+      <c r="D22" s="98"/>
+      <c r="E22" s="98"/>
     </row>
     <row r="23" spans="1:6" s="29" customFormat="1" ht="38.1" customHeight="1">
       <c r="A23" s="22" t="s">
-        <v>862</v>
-      </c>
-      <c r="B23" s="96"/>
-      <c r="C23" s="96"/>
-      <c r="D23" s="96"/>
-      <c r="E23" s="96"/>
+        <v>859</v>
+      </c>
+      <c r="B23" s="99"/>
+      <c r="C23" s="99"/>
+      <c r="D23" s="99"/>
+      <c r="E23" s="99"/>
     </row>
     <row r="24" spans="1:6" s="29" customFormat="1" ht="38.1" customHeight="1">
       <c r="A24" s="22" t="s">
-        <v>864</v>
-      </c>
-      <c r="B24" s="96"/>
-      <c r="C24" s="96"/>
-      <c r="D24" s="96"/>
-      <c r="E24" s="96"/>
+        <v>861</v>
+      </c>
+      <c r="B24" s="99"/>
+      <c r="C24" s="99"/>
+      <c r="D24" s="99"/>
+      <c r="E24" s="99"/>
     </row>
     <row r="25" spans="1:6" s="4" customFormat="1" ht="15" customHeight="1">
       <c r="A25" s="1"/>
@@ -4183,39 +4189,39 @@
       <c r="A27" s="1" t="s">
         <v>665</v>
       </c>
-      <c r="B27" s="92" t="s">
+      <c r="B27" s="95" t="s">
         <v>674</v>
       </c>
-      <c r="C27" s="92"/>
-      <c r="D27" s="92"/>
-      <c r="E27" s="92"/>
+      <c r="C27" s="95"/>
+      <c r="D27" s="95"/>
+      <c r="E27" s="95"/>
     </row>
     <row r="28" spans="1:6" s="4" customFormat="1" ht="15" customHeight="1">
       <c r="A28" s="1" t="s">
         <v>668</v>
       </c>
-      <c r="B28" s="92" t="s">
+      <c r="B28" s="95" t="s">
         <v>705</v>
       </c>
-      <c r="C28" s="92"/>
-      <c r="D28" s="92"/>
-      <c r="E28" s="92"/>
+      <c r="C28" s="95"/>
+      <c r="D28" s="95"/>
+      <c r="E28" s="95"/>
       <c r="F28" s="14" t="s">
-        <v>900</v>
+        <v>897</v>
       </c>
     </row>
     <row r="29" spans="1:6" s="4" customFormat="1" ht="15" customHeight="1">
       <c r="A29" s="1" t="s">
         <v>667</v>
       </c>
-      <c r="B29" s="91" t="s">
+      <c r="B29" s="94" t="s">
         <v>704</v>
       </c>
-      <c r="C29" s="91"/>
-      <c r="D29" s="91"/>
-      <c r="E29" s="91"/>
+      <c r="C29" s="94"/>
+      <c r="D29" s="94"/>
+      <c r="E29" s="94"/>
       <c r="F29" s="14" t="s">
-        <v>901</v>
+        <v>898</v>
       </c>
     </row>
     <row r="30" spans="1:6" s="4" customFormat="1" ht="15" customHeight="1">
@@ -4232,56 +4238,56 @@
       <c r="A32" s="9" t="s">
         <v>722</v>
       </c>
-      <c r="B32" s="90" t="s">
+      <c r="B32" s="93" t="s">
         <v>18</v>
       </c>
-      <c r="C32" s="90"/>
-      <c r="D32" s="90"/>
-      <c r="E32" s="90"/>
+      <c r="C32" s="93"/>
+      <c r="D32" s="93"/>
+      <c r="E32" s="93"/>
       <c r="F32" s="14" t="s">
-        <v>902</v>
+        <v>899</v>
       </c>
     </row>
     <row r="33" spans="1:6" s="4" customFormat="1" ht="15" customHeight="1">
       <c r="A33" s="9" t="s">
         <v>669</v>
       </c>
-      <c r="B33" s="90" t="s">
+      <c r="B33" s="93" t="s">
         <v>676</v>
       </c>
-      <c r="C33" s="90"/>
-      <c r="D33" s="90"/>
-      <c r="E33" s="90"/>
+      <c r="C33" s="93"/>
+      <c r="D33" s="93"/>
+      <c r="E33" s="93"/>
       <c r="F33" s="14" t="s">
-        <v>903</v>
+        <v>900</v>
       </c>
     </row>
     <row r="34" spans="1:6" s="4" customFormat="1" ht="15" customHeight="1">
       <c r="A34" s="9" t="s">
         <v>671</v>
       </c>
-      <c r="B34" s="91" t="s">
+      <c r="B34" s="94" t="s">
         <v>677</v>
       </c>
-      <c r="C34" s="91"/>
-      <c r="D34" s="91"/>
-      <c r="E34" s="91"/>
+      <c r="C34" s="94"/>
+      <c r="D34" s="94"/>
+      <c r="E34" s="94"/>
       <c r="F34" s="14" t="s">
-        <v>904</v>
+        <v>901</v>
       </c>
     </row>
     <row r="35" spans="1:6" s="4" customFormat="1" ht="15" customHeight="1">
       <c r="A35" s="9" t="s">
-        <v>869</v>
-      </c>
-      <c r="B35" s="90" t="s">
+        <v>866</v>
+      </c>
+      <c r="B35" s="93" t="s">
         <v>670</v>
       </c>
-      <c r="C35" s="90"/>
-      <c r="D35" s="90"/>
-      <c r="E35" s="90"/>
+      <c r="C35" s="93"/>
+      <c r="D35" s="93"/>
+      <c r="E35" s="93"/>
       <c r="F35" s="14" t="s">
-        <v>905</v>
+        <v>902</v>
       </c>
     </row>
     <row r="36" spans="1:6" s="4" customFormat="1" ht="15" customHeight="1">
@@ -4291,74 +4297,74 @@
     </row>
     <row r="37" spans="1:6" ht="18.3">
       <c r="A37" s="15" t="s">
-        <v>855</v>
+        <v>852</v>
       </c>
     </row>
     <row r="38" spans="1:6" ht="15" customHeight="1">
       <c r="A38" s="9" t="s">
         <v>709</v>
       </c>
-      <c r="B38" s="93" t="s">
+      <c r="B38" s="96" t="s">
         <v>659</v>
       </c>
-      <c r="C38" s="93"/>
-      <c r="D38" s="93"/>
-      <c r="E38" s="93"/>
+      <c r="C38" s="96"/>
+      <c r="D38" s="96"/>
+      <c r="E38" s="96"/>
     </row>
     <row r="39" spans="1:6" ht="15" customHeight="1">
       <c r="A39" s="9" t="s">
         <v>730</v>
       </c>
-      <c r="B39" s="91" t="s">
+      <c r="B39" s="94" t="s">
         <v>662</v>
       </c>
-      <c r="C39" s="91"/>
-      <c r="D39" s="91"/>
-      <c r="E39" s="91"/>
+      <c r="C39" s="94"/>
+      <c r="D39" s="94"/>
+      <c r="E39" s="94"/>
     </row>
     <row r="40" spans="1:6" ht="15" customHeight="1">
       <c r="A40" s="9" t="s">
         <v>710</v>
       </c>
-      <c r="B40" s="90" t="s">
+      <c r="B40" s="93" t="s">
         <v>660</v>
       </c>
-      <c r="C40" s="90"/>
-      <c r="D40" s="90"/>
-      <c r="E40" s="90"/>
+      <c r="C40" s="93"/>
+      <c r="D40" s="93"/>
+      <c r="E40" s="93"/>
     </row>
     <row r="41" spans="1:6" ht="15" customHeight="1">
       <c r="A41" s="9" t="s">
         <v>730</v>
       </c>
-      <c r="B41" s="91" t="s">
+      <c r="B41" s="94" t="s">
         <v>663</v>
       </c>
-      <c r="C41" s="91"/>
-      <c r="D41" s="91"/>
-      <c r="E41" s="91"/>
+      <c r="C41" s="94"/>
+      <c r="D41" s="94"/>
+      <c r="E41" s="94"/>
     </row>
     <row r="42" spans="1:6" ht="15" customHeight="1">
       <c r="A42" s="9" t="s">
         <v>711</v>
       </c>
-      <c r="B42" s="90" t="s">
+      <c r="B42" s="93" t="s">
         <v>661</v>
       </c>
-      <c r="C42" s="90"/>
-      <c r="D42" s="90"/>
-      <c r="E42" s="90"/>
+      <c r="C42" s="93"/>
+      <c r="D42" s="93"/>
+      <c r="E42" s="93"/>
     </row>
     <row r="43" spans="1:6" ht="15" customHeight="1">
       <c r="A43" s="9" t="s">
         <v>730</v>
       </c>
-      <c r="B43" s="91" t="s">
+      <c r="B43" s="94" t="s">
         <v>664</v>
       </c>
-      <c r="C43" s="91"/>
-      <c r="D43" s="91"/>
-      <c r="E43" s="91"/>
+      <c r="C43" s="94"/>
+      <c r="D43" s="94"/>
+      <c r="E43" s="94"/>
     </row>
     <row r="45" spans="1:6" ht="18.3">
       <c r="A45" s="32" t="s">
@@ -4401,7 +4407,7 @@
       <c r="A50" s="86" t="s">
         <v>31</v>
       </c>
-      <c r="B50" s="81" t="s">
+      <c r="B50" s="91" t="s">
         <v>716</v>
       </c>
     </row>
@@ -4410,16 +4416,16 @@
       <c r="B51" s="82"/>
     </row>
     <row r="52" spans="1:2" ht="15" customHeight="1">
-      <c r="A52" s="88"/>
-      <c r="B52" s="83"/>
+      <c r="A52" s="87"/>
+      <c r="B52" s="92"/>
     </row>
     <row r="53" spans="1:2" ht="15" customHeight="1">
-      <c r="A53" s="89"/>
-      <c r="B53" s="84"/>
+      <c r="A53" s="87"/>
+      <c r="B53" s="92"/>
     </row>
     <row r="54" spans="1:2" ht="15" customHeight="1">
-      <c r="A54" s="89"/>
-      <c r="B54" s="84"/>
+      <c r="A54" s="88"/>
+      <c r="B54" s="83"/>
     </row>
     <row r="55" spans="1:2" ht="15" customHeight="1">
       <c r="A55" s="89"/>
@@ -4493,12 +4499,12 @@
   <sheetData>
     <row r="1" spans="1:4" s="4" customFormat="1" ht="46.8">
       <c r="A1" s="10" t="s">
-        <v>896</v>
+        <v>893</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="15" customHeight="1">
       <c r="A2" s="9" t="s">
-        <v>749</v>
+        <v>747</v>
       </c>
       <c r="B2" s="5"/>
       <c r="C2" s="5"/>
@@ -4506,7 +4512,7 @@
     </row>
     <row r="3" spans="1:4" ht="15" customHeight="1">
       <c r="A3" s="9" t="s">
-        <v>750</v>
+        <v>748</v>
       </c>
       <c r="D3" s="2"/>
     </row>
@@ -4724,17 +4730,17 @@
   <sheetData>
     <row r="1" spans="1:1" ht="46.8">
       <c r="A1" s="30" t="s">
-        <v>848</v>
+        <v>845</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" s="9" t="s">
-        <v>847</v>
+        <v>844</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" s="9" t="s">
-        <v>850</v>
+        <v>847</v>
       </c>
     </row>
     <row r="4" spans="1:1">
@@ -4990,25 +4996,25 @@
     <row r="11" spans="1:4">
       <c r="A11" s="29" t="str">
         <f>IF(Notebooks!G9="","",CONCATENATE("| [",Notebooks!A9,"](",Configuration!B$29,Configuration!B$28,"/sessions/session",Notebooks!A9,") | ",Notebooks!G9," |"))</f>
-        <v/>
+        <v>| [2](https://rpi-data.github.io/course-intro-ml-app/sessions/session2) | Python Overview - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/02-intro-python/01-intro-python-overview.ipynb)&lt;br&gt;Basic Data Structures - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/02-intro-python/02-intro-python-datastructures.ipynbhttps://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/02-intro-python/03-intro-python-numpy.ipynb)&lt;br&gt;Numpy - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/02-intro-python/04-intro-python-pandas.ipynb)&lt;br&gt;Pandas - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/02-intro-python/04-intro-python-pandas.ipynb) |</v>
       </c>
       <c r="B11" s="29"/>
       <c r="C11" s="29"/>
       <c r="D11" s="29"/>
     </row>
     <row r="12" spans="1:4">
-      <c r="A12" s="29" t="str">
-        <f>IF(Notebooks!G10="","",CONCATENATE("| [",Notebooks!A10,"](",Configuration!B$29,Configuration!B$28,"/sessions/session",Notebooks!A10,") | ",Notebooks!G10," |"))</f>
-        <v/>
+      <c r="A12" s="29" t="e">
+        <f>IF(Notebooks!#REF!="","",CONCATENATE("| [",Notebooks!#REF!,"](",Configuration!B$29,Configuration!B$28,"/sessions/session",Notebooks!#REF!,") | ",Notebooks!#REF!," |"))</f>
+        <v>#REF!</v>
       </c>
       <c r="B12" s="29"/>
       <c r="C12" s="29"/>
       <c r="D12" s="29"/>
     </row>
     <row r="13" spans="1:4">
-      <c r="A13" s="29" t="str">
-        <f>IF(Notebooks!G11="","",CONCATENATE("| [",Notebooks!A11,"](",Configuration!B$29,Configuration!B$28,"/sessions/session",Notebooks!A11,") | ",Notebooks!G11," |"))</f>
-        <v>| [2](https://rpi-data.github.io/course-intro-ml-app/sessions/session2) | Python Overview - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/02-intro-python/01-intro-python-overview.ipynb)&lt;br&gt;Basic Data Structures - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/02-intro-python/02-intro-python-datastructures.ipynbhttps://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/02-intro-python/03-intro-python-numpy.ipynb)&lt;br&gt;Numpy - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/02-intro-python/04-intro-python-pandas.ipynb)&lt;br&gt;Pandas - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/02-intro-python/04-intro-python-pandas.ipynb)&lt;br&gt;Lab - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/02-intro-python/lab/lab.ipynb)&lt;br&gt;Assignment 1 - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/02-intro-python/hm-01/hm01.ipynb) |</v>
+      <c r="A13" s="29" t="e">
+        <f>IF(Notebooks!#REF!="","",CONCATENATE("| [",Notebooks!#REF!,"](",Configuration!B$29,Configuration!B$28,"/sessions/session",Notebooks!#REF!,") | ",Notebooks!#REF!," |"))</f>
+        <v>#REF!</v>
       </c>
       <c r="B13" s="29"/>
       <c r="C13" s="29"/>
@@ -5016,7 +5022,7 @@
     </row>
     <row r="14" spans="1:4">
       <c r="A14" s="29" t="str">
-        <f>IF(Notebooks!G12="","",CONCATENATE("| [",Notebooks!A12,"](",Configuration!B$29,Configuration!B$28,"/sessions/session",Notebooks!A12,") | ",Notebooks!G12," |"))</f>
+        <f>IF(Notebooks!G10="","",CONCATENATE("| [",Notebooks!A10,"](",Configuration!B$29,Configuration!B$28,"/sessions/session",Notebooks!A10,") | ",Notebooks!G10," |"))</f>
         <v/>
       </c>
       <c r="B14" s="29"/>
@@ -5025,7 +5031,7 @@
     </row>
     <row r="15" spans="1:4">
       <c r="A15" s="29" t="str">
-        <f>IF(Notebooks!G13="","",CONCATENATE("| [",Notebooks!A13,"](",Configuration!B$29,Configuration!B$28,"/sessions/session",Notebooks!A13,") | ",Notebooks!G13," |"))</f>
+        <f>IF(Notebooks!G11="","",CONCATENATE("| [",Notebooks!A11,"](",Configuration!B$29,Configuration!B$28,"/sessions/session",Notebooks!A11,") | ",Notebooks!G11," |"))</f>
         <v/>
       </c>
       <c r="B15" s="29"/>
@@ -5034,7 +5040,7 @@
     </row>
     <row r="16" spans="1:4">
       <c r="A16" s="29" t="str">
-        <f>IF(Notebooks!G14="","",CONCATENATE("| [",Notebooks!A14,"](",Configuration!B$29,Configuration!B$28,"/sessions/session",Notebooks!A14,") | ",Notebooks!G14," |"))</f>
+        <f>IF(Notebooks!G12="","",CONCATENATE("| [",Notebooks!A12,"](",Configuration!B$29,Configuration!B$28,"/sessions/session",Notebooks!A12,") | ",Notebooks!G12," |"))</f>
         <v/>
       </c>
       <c r="B16" s="29"/>
@@ -5043,7 +5049,7 @@
     </row>
     <row r="17" spans="1:4">
       <c r="A17" s="29" t="str">
-        <f>IF(Notebooks!G15="","",CONCATENATE("| [",Notebooks!A15,"](",Configuration!B$29,Configuration!B$28,"/sessions/session",Notebooks!A15,") | ",Notebooks!G15," |"))</f>
+        <f>IF(Notebooks!G13="","",CONCATENATE("| [",Notebooks!A13,"](",Configuration!B$29,Configuration!B$28,"/sessions/session",Notebooks!A13,") | ",Notebooks!G13," |"))</f>
         <v/>
       </c>
       <c r="B17" s="29"/>
@@ -5052,7 +5058,7 @@
     </row>
     <row r="18" spans="1:4">
       <c r="A18" s="29" t="str">
-        <f>IF(Notebooks!G16="","",CONCATENATE("| [",Notebooks!A16,"](",Configuration!B$29,Configuration!B$28,"/sessions/session",Notebooks!A16,") | ",Notebooks!G16," |"))</f>
+        <f>IF(Notebooks!G14="","",CONCATENATE("| [",Notebooks!A14,"](",Configuration!B$29,Configuration!B$28,"/sessions/session",Notebooks!A14,") | ",Notebooks!G14," |"))</f>
         <v/>
       </c>
       <c r="B18" s="29"/>
@@ -5061,7 +5067,7 @@
     </row>
     <row r="19" spans="1:4">
       <c r="A19" s="29" t="str">
-        <f>IF(Notebooks!G17="","",CONCATENATE("| [",Notebooks!A17,"](",Configuration!B$29,Configuration!B$28,"/sessions/session",Notebooks!A17,") | ",Notebooks!G17," |"))</f>
+        <f>IF(Notebooks!G15="","",CONCATENATE("| [",Notebooks!A15,"](",Configuration!B$29,Configuration!B$28,"/sessions/session",Notebooks!A15,") | ",Notebooks!G15," |"))</f>
         <v>| [4](https://rpi-data.github.io/course-intro-ml-app/sessions/session4) | Conditional-Loops - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/03-python/01-intro-python-conditionals-loops.ipynb)&lt;br&gt;Functions - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/03-python/02-intro-python-functions.ipynb)&lt;br&gt;Null Values - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/03-python/03-intro-python-null-values.ipynb)&lt;br&gt;Groupby - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/03-python/04-intro-python-groupby.ipynb)&lt;br&gt;Kaggle Baseline - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/03-python/05-intro-kaggle-baseline.ipynb)&lt;br&gt;Assignment 2 - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/03-python/hm-02/hm02.ipynb) |</v>
       </c>
       <c r="B19" s="29"/>
@@ -5070,7 +5076,7 @@
     </row>
     <row r="20" spans="1:4">
       <c r="A20" s="29" t="str">
-        <f>IF(Notebooks!G18="","",CONCATENATE("| [",Notebooks!A18,"](",Configuration!B$29,Configuration!B$28,"/sessions/session",Notebooks!A18,") | ",Notebooks!G18," |"))</f>
+        <f>IF(Notebooks!G16="","",CONCATENATE("| [",Notebooks!A16,"](",Configuration!B$29,Configuration!B$28,"/sessions/session",Notebooks!A16,") | ",Notebooks!G16," |"))</f>
         <v/>
       </c>
       <c r="B20" s="29"/>
@@ -5079,7 +5085,7 @@
     </row>
     <row r="21" spans="1:4">
       <c r="A21" s="29" t="str">
-        <f>IF(Notebooks!G19="","",CONCATENATE("| [",Notebooks!A19,"](",Configuration!B$29,Configuration!B$28,"/sessions/session",Notebooks!A19,") | ",Notebooks!G19," |"))</f>
+        <f>IF(Notebooks!G17="","",CONCATENATE("| [",Notebooks!A17,"](",Configuration!B$29,Configuration!B$28,"/sessions/session",Notebooks!A17,") | ",Notebooks!G17," |"))</f>
         <v/>
       </c>
       <c r="B21" s="29"/>
@@ -5088,7 +5094,7 @@
     </row>
     <row r="22" spans="1:4">
       <c r="A22" s="29" t="str">
-        <f>IF(Notebooks!G20="","",CONCATENATE("| [",Notebooks!A20,"](",Configuration!B$29,Configuration!B$28,"/sessions/session",Notebooks!A20,") | ",Notebooks!G20," |"))</f>
+        <f>IF(Notebooks!G18="","",CONCATENATE("| [",Notebooks!A18,"](",Configuration!B$29,Configuration!B$28,"/sessions/session",Notebooks!A18,") | ",Notebooks!G18," |"))</f>
         <v/>
       </c>
       <c r="B22" s="29"/>
@@ -5097,7 +5103,7 @@
     </row>
     <row r="23" spans="1:4">
       <c r="A23" s="29" t="str">
-        <f>IF(Notebooks!G21="","",CONCATENATE("| [",Notebooks!A21,"](",Configuration!B$29,Configuration!B$28,"/sessions/session",Notebooks!A21,") | ",Notebooks!G21," |"))</f>
+        <f>IF(Notebooks!G19="","",CONCATENATE("| [",Notebooks!A19,"](",Configuration!B$29,Configuration!B$28,"/sessions/session",Notebooks!A19,") | ",Notebooks!G19," |"))</f>
         <v/>
       </c>
       <c r="B23" s="29"/>
@@ -5106,7 +5112,7 @@
     </row>
     <row r="24" spans="1:4">
       <c r="A24" s="29" t="str">
-        <f>IF(Notebooks!G22="","",CONCATENATE("| [",Notebooks!A22,"](",Configuration!B$29,Configuration!B$28,"/sessions/session",Notebooks!A22,") | ",Notebooks!G22," |"))</f>
+        <f>IF(Notebooks!G20="","",CONCATENATE("| [",Notebooks!A20,"](",Configuration!B$29,Configuration!B$28,"/sessions/session",Notebooks!A20,") | ",Notebooks!G20," |"))</f>
         <v/>
       </c>
       <c r="B24" s="29"/>
@@ -5115,7 +5121,7 @@
     </row>
     <row r="25" spans="1:4">
       <c r="A25" s="29" t="str">
-        <f>IF(Notebooks!G23="","",CONCATENATE("| [",Notebooks!A23,"](",Configuration!B$29,Configuration!B$28,"/sessions/session",Notebooks!A23,") | ",Notebooks!G23," |"))</f>
+        <f>IF(Notebooks!G21="","",CONCATENATE("| [",Notebooks!A21,"](",Configuration!B$29,Configuration!B$28,"/sessions/session",Notebooks!A21,") | ",Notebooks!G21," |"))</f>
         <v>| [6](https://rpi-data.github.io/course-intro-ml-app/sessions/session6) | Twitter - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/04-viz-api-scraper/01_intro_api_twitter.ipynb)&lt;br&gt;Web Mining - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/04-viz-api-scraper/02_intro_python_webmining.ipynb)&lt;br&gt;Visualizations - Seaborn - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/04-viz-api-scraper/03_visualization_python_seaborn.ipynb)&lt;br&gt;Strings - Regular Expressions - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/04-viz-api-scraper/04_strings_and_regular_expressions.ipynb)&lt;br&gt;Feature Dummies - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/04-viz-api-scraper/05_features_dummies.ipynb)&lt;br&gt;Assignment 3 - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/04-viz-api-scraper/hm-03/hm03.ipynb) |</v>
       </c>
       <c r="B25" s="29"/>
@@ -5124,7 +5130,7 @@
     </row>
     <row r="26" spans="1:4">
       <c r="A26" s="29" t="str">
-        <f>IF(Notebooks!G24="","",CONCATENATE("| [",Notebooks!A24,"](",Configuration!B$29,Configuration!B$28,"/sessions/session",Notebooks!A24,") | ",Notebooks!G24," |"))</f>
+        <f>IF(Notebooks!G22="","",CONCATENATE("| [",Notebooks!A22,"](",Configuration!B$29,Configuration!B$28,"/sessions/session",Notebooks!A22,") | ",Notebooks!G22," |"))</f>
         <v/>
       </c>
       <c r="B26" s="29"/>
@@ -5133,7 +5139,7 @@
     </row>
     <row r="27" spans="1:4">
       <c r="A27" s="29" t="str">
-        <f>IF(Notebooks!G25="","",CONCATENATE("| [",Notebooks!A25,"](",Configuration!B$29,Configuration!B$28,"/sessions/session",Notebooks!A25,") | ",Notebooks!G25," |"))</f>
+        <f>IF(Notebooks!G23="","",CONCATENATE("| [",Notebooks!A23,"](",Configuration!B$29,Configuration!B$28,"/sessions/session",Notebooks!A23,") | ",Notebooks!G23," |"))</f>
         <v/>
       </c>
       <c r="B27" s="29"/>
@@ -5142,7 +5148,7 @@
     </row>
     <row r="28" spans="1:4">
       <c r="A28" s="29" t="str">
-        <f>IF(Notebooks!G26="","",CONCATENATE("| [",Notebooks!A26,"](",Configuration!B$29,Configuration!B$28,"/sessions/session",Notebooks!A26,") | ",Notebooks!G26," |"))</f>
+        <f>IF(Notebooks!G24="","",CONCATENATE("| [",Notebooks!A24,"](",Configuration!B$29,Configuration!B$28,"/sessions/session",Notebooks!A24,") | ",Notebooks!G24," |"))</f>
         <v/>
       </c>
       <c r="B28" s="29"/>
@@ -5151,7 +5157,7 @@
     </row>
     <row r="29" spans="1:4">
       <c r="A29" s="29" t="str">
-        <f>IF(Notebooks!G27="","",CONCATENATE("| [",Notebooks!A27,"](",Configuration!B$29,Configuration!B$28,"/sessions/session",Notebooks!A27,") | ",Notebooks!G27," |"))</f>
+        <f>IF(Notebooks!G25="","",CONCATENATE("| [",Notebooks!A25,"](",Configuration!B$29,Configuration!B$28,"/sessions/session",Notebooks!A25,") | ",Notebooks!G25," |"))</f>
         <v/>
       </c>
       <c r="B29" s="29"/>
@@ -5160,7 +5166,7 @@
     </row>
     <row r="30" spans="1:4">
       <c r="A30" s="29" t="str">
-        <f>IF(Notebooks!G28="","",CONCATENATE("| [",Notebooks!A28,"](",Configuration!B$29,Configuration!B$28,"/sessions/session",Notebooks!A28,") | ",Notebooks!G28," |"))</f>
+        <f>IF(Notebooks!G26="","",CONCATENATE("| [",Notebooks!A26,"](",Configuration!B$29,Configuration!B$28,"/sessions/session",Notebooks!A26,") | ",Notebooks!G26," |"))</f>
         <v/>
       </c>
       <c r="B30" s="29"/>
@@ -5169,7 +5175,7 @@
     </row>
     <row r="31" spans="1:4">
       <c r="A31" s="29" t="str">
-        <f>IF(Notebooks!G29="","",CONCATENATE("| [",Notebooks!A29,"](",Configuration!B$29,Configuration!B$28,"/sessions/session",Notebooks!A29,") | ",Notebooks!G29," |"))</f>
+        <f>IF(Notebooks!G27="","",CONCATENATE("| [",Notebooks!A27,"](",Configuration!B$29,Configuration!B$28,"/sessions/session",Notebooks!A27,") | ",Notebooks!G27," |"))</f>
         <v/>
       </c>
       <c r="B31" s="29"/>
@@ -5178,7 +5184,7 @@
     </row>
     <row r="32" spans="1:4">
       <c r="A32" s="29" t="str">
-        <f>IF(Notebooks!G30="","",CONCATENATE("| [",Notebooks!A30,"](",Configuration!B$29,Configuration!B$28,"/sessions/session",Notebooks!A30,") | ",Notebooks!G30," |"))</f>
+        <f>IF(Notebooks!G28="","",CONCATENATE("| [",Notebooks!A28,"](",Configuration!B$29,Configuration!B$28,"/sessions/session",Notebooks!A28,") | ",Notebooks!G28," |"))</f>
         <v>| [9](https://rpi-data.github.io/course-intro-ml-app/sessions/session9) | The Simplest Neural Network with Numpy - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/05-intro-modeling/01-Neural-Networks.ipynb)&lt;br&gt;Train Test Split - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/05-intro-modeling/01-training-test-split.ipynb)&lt;br&gt;Introduction to Logistic Regression - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/05-intro-modeling/02-intro-logistic-knn.ipynb)&lt;br&gt;K Nearest Neighbor - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/05-intro-modeling/03-knn.ipynb)&lt;br&gt;ROC and SVM - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/05-intro-modeling/04-svm-roc.ipynb)&lt;br&gt;HM5A Visualization &amp; Screen Scraping - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/05-intro-modeling/hm5/homework_05A.ipynb)&lt;br&gt;HM5B Intro Modeling - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/05-intro-modeling/hm5/homework_05B.ipynb) |</v>
       </c>
       <c r="B32" s="29"/>
@@ -5187,7 +5193,7 @@
     </row>
     <row r="33" spans="1:4">
       <c r="A33" s="29" t="str">
-        <f>IF(Notebooks!G31="","",CONCATENATE("| [",Notebooks!A31,"](",Configuration!B$29,Configuration!B$28,"/sessions/session",Notebooks!A31,") | ",Notebooks!G31," |"))</f>
+        <f>IF(Notebooks!G29="","",CONCATENATE("| [",Notebooks!A29,"](",Configuration!B$29,Configuration!B$28,"/sessions/session",Notebooks!A29,") | ",Notebooks!G29," |"))</f>
         <v/>
       </c>
       <c r="B33" s="29"/>
@@ -5196,7 +5202,7 @@
     </row>
     <row r="34" spans="1:4">
       <c r="A34" s="29" t="str">
-        <f>IF(Notebooks!G32="","",CONCATENATE("| [",Notebooks!A32,"](",Configuration!B$29,Configuration!B$28,"/sessions/session",Notebooks!A32,") | ",Notebooks!G32," |"))</f>
+        <f>IF(Notebooks!G30="","",CONCATENATE("| [",Notebooks!A30,"](",Configuration!B$29,Configuration!B$28,"/sessions/session",Notebooks!A30,") | ",Notebooks!G30," |"))</f>
         <v/>
       </c>
       <c r="B34" s="29"/>
@@ -5205,7 +5211,7 @@
     </row>
     <row r="35" spans="1:4">
       <c r="A35" s="29" t="str">
-        <f>IF(Notebooks!G33="","",CONCATENATE("| [",Notebooks!A33,"](",Configuration!B$29,Configuration!B$28,"/sessions/session",Notebooks!A33,") | ",Notebooks!G33," |"))</f>
+        <f>IF(Notebooks!G31="","",CONCATENATE("| [",Notebooks!A31,"](",Configuration!B$29,Configuration!B$28,"/sessions/session",Notebooks!A31,") | ",Notebooks!G31," |"))</f>
         <v>| [13](https://rpi-data.github.io/course-intro-ml-app/sessions/session13) | Matrix Regression - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/07-intro-modeling2/Python/01-matrix-regression-gradient-decent-python.ipynb)&lt;br&gt;Regression Basics - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/07-intro-modeling2/Python/02-regression-boston-housing-python.ipynb)&lt;br&gt;Ridge and Lasso Regression - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/07-intro-modeling2/Python/03-ridge-lasso-python.ipynb) |</v>
       </c>
       <c r="B35" s="29"/>
@@ -5214,7 +5220,7 @@
     </row>
     <row r="36" spans="1:4">
       <c r="A36" s="29" t="str">
-        <f>IF(Notebooks!G34="","",CONCATENATE("| [",Notebooks!A34,"](",Configuration!B$29,Configuration!B$28,"/sessions/session",Notebooks!A34,") | ",Notebooks!G34," |"))</f>
+        <f>IF(Notebooks!G32="","",CONCATENATE("| [",Notebooks!A32,"](",Configuration!B$29,Configuration!B$28,"/sessions/session",Notebooks!A32,") | ",Notebooks!G32," |"))</f>
         <v/>
       </c>
       <c r="B36" s="29"/>
@@ -5223,7 +5229,7 @@
     </row>
     <row r="37" spans="1:4">
       <c r="A37" s="29" t="str">
-        <f>IF(Notebooks!G35="","",CONCATENATE("| [",Notebooks!A35,"](",Configuration!B$29,Configuration!B$28,"/sessions/session",Notebooks!A35,") | ",Notebooks!G35," |"))</f>
+        <f>IF(Notebooks!G33="","",CONCATENATE("| [",Notebooks!A33,"](",Configuration!B$29,Configuration!B$28,"/sessions/session",Notebooks!A33,") | ",Notebooks!G33," |"))</f>
         <v>| [15](https://rpi-data.github.io/course-intro-ml-app/sessions/session15) | Ridge and Lasso Regression - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/07-intro-modeling2/Python/03-ridge-lasso-python.ipynb)&lt;br&gt;PCA - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/07-intro-modeling2/Python/04_introduction_pca.ipynb) |</v>
       </c>
       <c r="B37" s="29"/>
@@ -5256,12 +5262,12 @@
     </row>
     <row r="2" spans="1:1">
       <c r="A2" s="9" t="s">
-        <v>751</v>
+        <v>749</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" s="9" t="s">
-        <v>748</v>
+        <v>746</v>
       </c>
     </row>
     <row r="4" spans="1:1">
@@ -5475,7 +5481,7 @@
   <dimension ref="A1:G33"/>
   <sheetViews>
     <sheetView zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.09765625" defaultRowHeight="15" customHeight="1"/>
@@ -5499,7 +5505,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="15" customHeight="1">
+    <row r="2" spans="1:7" ht="14.7" customHeight="1">
       <c r="A2" s="31" t="str">
         <f>IF(ISBLANK(Schedule!B3),"",CONCATENATE("session",Schedule!B3))</f>
         <v>session1</v>
@@ -5516,7 +5522,7 @@
 ### Readings
 *None*
 ### Notebooks
-What is Jupyter? - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/01-overview/01-notebook-basics/01-what-is-jupyter.ipynb#scrollTo=mdFTkIqGwgOJ)&lt;br&gt;Notebook Basics - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/01-overview/01-notebook-basics/02-notebook-basics.ipynb)&lt;br&gt;Running Code - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/01-overview/01-notebook-basics/03-running-code.ipynb)&lt;br&gt;Markdown - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/01-overview/01-notebook-basics/04-markdown.ipynb)</v>
+[What is Jupyter?](https://rpi-data.github.io/course-intro-ml-app/notebooks/01-what-is-jupyter.html)&lt;br&gt;[Notebook Basics](https://rpi-data.github.io/course-intro-ml-app/notebooks/02-notebook-basics.html)&lt;br&gt;[Running Code](https://rpi-data.github.io/course-intro-ml-app/notebooks/03-running-code.html)&lt;br&gt;[Markdown](https://rpi-data.github.io/course-intro-ml-app/notebooks/04-markdown.html)</v>
       </c>
       <c r="C2" s="12" t="s">
         <v>18</v>
@@ -5536,7 +5542,7 @@
 ### Readings
 ",IF(Schedule!L3,LOOKUP(Schedule!B3,Readings!A:A,Readings!F:F),"*None*"),"
 ### Notebooks
-",IF(Schedule!M3,LOOKUP(Schedule!B3,Notebooks!A:A,Notebooks!G:G),"*None*"))</f>
+",IF(Schedule!M3,LOOKUP(Schedule!B3,Notebooks!A:A,Notebooks!L:L),"*None*"))</f>
         <v xml:space="preserve">
 ### Description
 In this class we motivate the overall field of data science, machine learning, and the emerging area of AI.  Explore introduction. 
@@ -5546,7 +5552,7 @@
 ### Readings
 *None*
 ### Notebooks
-What is Jupyter? - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/01-overview/01-notebook-basics/01-what-is-jupyter.ipynb#scrollTo=mdFTkIqGwgOJ)&lt;br&gt;Notebook Basics - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/01-overview/01-notebook-basics/02-notebook-basics.ipynb)&lt;br&gt;Running Code - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/01-overview/01-notebook-basics/03-running-code.ipynb)&lt;br&gt;Markdown - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/01-overview/01-notebook-basics/04-markdown.ipynb)</v>
+[What is Jupyter?](https://rpi-data.github.io/course-intro-ml-app/notebooks/01-what-is-jupyter.html)&lt;br&gt;[Notebook Basics](https://rpi-data.github.io/course-intro-ml-app/notebooks/02-notebook-basics.html)&lt;br&gt;[Running Code](https://rpi-data.github.io/course-intro-ml-app/notebooks/03-running-code.html)&lt;br&gt;[Markdown](https://rpi-data.github.io/course-intro-ml-app/notebooks/04-markdown.html)</v>
       </c>
       <c r="G2" s="26"/>
     </row>
@@ -5586,7 +5592,7 @@
 ### Readings
 ",IF(Schedule!L4,LOOKUP(Schedule!B4,Readings!A:A,Readings!F:F),"*None*"),"
 ### Notebooks
-",IF(Schedule!M4,LOOKUP(Schedule!B4,Notebooks!A:A,Notebooks!G:G),"*None*"))</f>
+",IF(Schedule!M4,LOOKUP(Schedule!B4,Notebooks!A:A,Notebooks!L:L),"*None*"))</f>
         <v xml:space="preserve">
 ### Description
 *None*
@@ -5616,7 +5622,7 @@
 ### Readings
 [Doing Data Science (Chapter 1)](http://proquestcombo.safaribooksonline.com.libproxy.rpi.edu/book/databases/9781449363871)&lt;br&gt;[Data Science for Business (Chapter 1)](http://proquestcombo.safaribooksonline.com.libproxy.rpi.edu/book/databases/business-intelligence/9781449374273)&lt;br&gt;[Command Line Cheat Sheet](https://www.git-tower.com/blog/command-line-cheat-sheet/)&lt;br&gt;[Assignment Process](/assignments)&lt;br&gt;[Running Jupyter locally](http://rpi.analyticsdojo.com/setup/anaconda/)
 ### Notebooks
-Python Overview - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/02-intro-python/01-intro-python-overview.ipynb)&lt;br&gt;Basic Data Structures - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/02-intro-python/02-intro-python-datastructures.ipynbhttps://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/02-intro-python/03-intro-python-numpy.ipynb)&lt;br&gt;Numpy - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/02-intro-python/04-intro-python-pandas.ipynb)&lt;br&gt;Pandas - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/02-intro-python/04-intro-python-pandas.ipynb)&lt;br&gt;Lab - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/02-intro-python/lab/lab.ipynb)&lt;br&gt;Assignment 1 - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/02-intro-python/hm-01/hm01.ipynb)</v>
+[Python Overview](https://rpi-data.github.io/course-intro-ml-app/notebooks/05-intro-python-overview.html)&lt;br&gt;[Basic Data Structures](https://rpi-data.github.io/course-intro-ml-app/notebooks/06-intro-python-datastructures.html)&lt;br&gt;[Numpy](https://rpi-data.github.io/course-intro-ml-app/notebooks/07-intro-python-numpy.html)&lt;br&gt;[Pandas](https://rpi-data.github.io/course-intro-ml-app/notebooks/08-intro-python-pandas.html)</v>
       </c>
       <c r="C4" s="12" t="s">
         <v>18</v>
@@ -5636,7 +5642,7 @@
 ### Readings
 ",IF(Schedule!L5,LOOKUP(Schedule!B5,Readings!A:A,Readings!F:F),"*None*"),"
 ### Notebooks
-",IF(Schedule!M5,LOOKUP(Schedule!B5,Notebooks!A:A,Notebooks!G:G),"*None*"))</f>
+",IF(Schedule!M5,LOOKUP(Schedule!B5,Notebooks!A:A,Notebooks!L:L),"*None*"))</f>
         <v xml:space="preserve">
 ### Description
 This class introduces some basic computational background the Python computational environment, packages, colab, linux command line, git.  Introduction to coding includes basic data structures (sets, dictionaries, lists) along with packages specific for analytics (Numpy and Pandas). 
@@ -5647,7 +5653,7 @@
 ### Readings
 [Doing Data Science (Chapter 1)](http://proquestcombo.safaribooksonline.com.libproxy.rpi.edu/book/databases/9781449363871)&lt;br&gt;[Data Science for Business (Chapter 1)](http://proquestcombo.safaribooksonline.com.libproxy.rpi.edu/book/databases/business-intelligence/9781449374273)&lt;br&gt;[Command Line Cheat Sheet](https://www.git-tower.com/blog/command-line-cheat-sheet/)&lt;br&gt;[Assignment Process](/assignments)&lt;br&gt;[Running Jupyter locally](http://rpi.analyticsdojo.com/setup/anaconda/)
 ### Notebooks
-Python Overview - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/02-intro-python/01-intro-python-overview.ipynb)&lt;br&gt;Basic Data Structures - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/02-intro-python/02-intro-python-datastructures.ipynbhttps://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/02-intro-python/03-intro-python-numpy.ipynb)&lt;br&gt;Numpy - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/02-intro-python/04-intro-python-pandas.ipynb)&lt;br&gt;Pandas - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/02-intro-python/04-intro-python-pandas.ipynb)&lt;br&gt;Lab - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/02-intro-python/lab/lab.ipynb)&lt;br&gt;Assignment 1 - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/02-intro-python/hm-01/hm01.ipynb)</v>
+[Python Overview](https://rpi-data.github.io/course-intro-ml-app/notebooks/05-intro-python-overview.html)&lt;br&gt;[Basic Data Structures](https://rpi-data.github.io/course-intro-ml-app/notebooks/06-intro-python-datastructures.html)&lt;br&gt;[Numpy](https://rpi-data.github.io/course-intro-ml-app/notebooks/07-intro-python-numpy.html)&lt;br&gt;[Pandas](https://rpi-data.github.io/course-intro-ml-app/notebooks/08-intro-python-pandas.html)</v>
       </c>
       <c r="F4" s="31"/>
     </row>
@@ -5687,7 +5693,7 @@
 ### Readings
 ",IF(Schedule!L6,LOOKUP(Schedule!B6,Readings!A:A,Readings!F:F),"*None*"),"
 ### Notebooks
-",IF(Schedule!M6,LOOKUP(Schedule!B6,Notebooks!A:A,Notebooks!G:G),"*None*"))</f>
+",IF(Schedule!M6,LOOKUP(Schedule!B6,Notebooks!A:A,Notebooks!L:L),"*None*"))</f>
         <v xml:space="preserve">
 ### Description
 Lab/homework
@@ -5715,7 +5721,7 @@
 ### Readings
 [Principles of Data Wrangling (Chapters 1-3)](http://proquestcombo.safaribooksonline.com.libproxy.rpi.edu/book/databases/business-intelligence/9781491938911)
 ### Notebooks
-Conditional-Loops - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/03-python/01-intro-python-conditionals-loops.ipynb)&lt;br&gt;Functions - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/03-python/02-intro-python-functions.ipynb)&lt;br&gt;Null Values - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/03-python/03-intro-python-null-values.ipynb)&lt;br&gt;Groupby - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/03-python/04-intro-python-groupby.ipynb)&lt;br&gt;Kaggle Baseline - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/03-python/05-intro-kaggle-baseline.ipynb)&lt;br&gt;Assignment 2 - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/03-python/hm-02/hm02.ipynb)</v>
+&lt;br&gt;&lt;br&gt;&lt;br&gt;&lt;br&gt;&lt;br&gt;</v>
       </c>
       <c r="C6" s="12" t="s">
         <v>18</v>
@@ -5735,7 +5741,7 @@
 ### Readings
 ",IF(Schedule!L7,LOOKUP(Schedule!B7,Readings!A:A,Readings!F:F),"*None*"),"
 ### Notebooks
-",IF(Schedule!M7,LOOKUP(Schedule!B7,Notebooks!A:A,Notebooks!G:G),"*None*"))</f>
+",IF(Schedule!M7,LOOKUP(Schedule!B7,Notebooks!A:A,Notebooks!L:L),"*None*"))</f>
         <v xml:space="preserve">
 ### Description
 This lecture discusses the general strategic impact of data, open data, data encoding, data provenance, data wrangling, includeing merging, aggregation, filtering. Continued introduction to coding includes conditionals, loops, functions, missing values, filtering, group-by.  We will also introduce a basic Kaggle model for the Titantic dataset. 
@@ -5744,7 +5750,7 @@
 ### Readings
 [Principles of Data Wrangling (Chapters 1-3)](http://proquestcombo.safaribooksonline.com.libproxy.rpi.edu/book/databases/business-intelligence/9781491938911)
 ### Notebooks
-Conditional-Loops - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/03-python/01-intro-python-conditionals-loops.ipynb)&lt;br&gt;Functions - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/03-python/02-intro-python-functions.ipynb)&lt;br&gt;Null Values - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/03-python/03-intro-python-null-values.ipynb)&lt;br&gt;Groupby - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/03-python/04-intro-python-groupby.ipynb)&lt;br&gt;Kaggle Baseline - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/03-python/05-intro-kaggle-baseline.ipynb)&lt;br&gt;Assignment 2 - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/03-python/hm-02/hm02.ipynb)</v>
+&lt;br&gt;&lt;br&gt;&lt;br&gt;&lt;br&gt;&lt;br&gt;</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="15" customHeight="1">
@@ -5783,7 +5789,7 @@
 ### Readings
 ",IF(Schedule!L8,LOOKUP(Schedule!B8,Readings!A:A,Readings!F:F),"*None*"),"
 ### Notebooks
-",IF(Schedule!M8,LOOKUP(Schedule!B8,Notebooks!A:A,Notebooks!G:G),"*None*"))</f>
+",IF(Schedule!M8,LOOKUP(Schedule!B8,Notebooks!A:A,Notebooks!L:L),"*None*"))</f>
         <v xml:space="preserve">
 ### Description
 Lab/homework
@@ -5811,7 +5817,7 @@
 ### Readings
 [Introduction to Machine Learning with Python (Chapter 1)](http://proquestcombo.safaribooksonline.com.libproxy.rpi.edu/book/programming/machine-learning/9781449369880)
 ### Notebooks
-Twitter - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/04-viz-api-scraper/01_intro_api_twitter.ipynb)&lt;br&gt;Web Mining - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/04-viz-api-scraper/02_intro_python_webmining.ipynb)&lt;br&gt;Visualizations - Seaborn - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/04-viz-api-scraper/03_visualization_python_seaborn.ipynb)&lt;br&gt;Strings - Regular Expressions - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/04-viz-api-scraper/04_strings_and_regular_expressions.ipynb)&lt;br&gt;Feature Dummies - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/04-viz-api-scraper/05_features_dummies.ipynb)&lt;br&gt;Assignment 3 - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/04-viz-api-scraper/hm-03/hm03.ipynb)</v>
+&lt;br&gt;&lt;br&gt;&lt;br&gt;&lt;br&gt;&lt;br&gt;</v>
       </c>
       <c r="C8" s="12" t="s">
         <v>18</v>
@@ -5831,7 +5837,7 @@
 ### Readings
 ",IF(Schedule!L9,LOOKUP(Schedule!B9,Readings!A:A,Readings!F:F),"*None*"),"
 ### Notebooks
-",IF(Schedule!M9,LOOKUP(Schedule!B9,Notebooks!A:A,Notebooks!G:G),"*None*"))</f>
+",IF(Schedule!M9,LOOKUP(Schedule!B9,Notebooks!A:A,Notebooks!L:L),"*None*"))</f>
         <v xml:space="preserve">
 ### Description
 Introduction to APIs, web scraping feature creation, and feature creation/extraction.  The genaral goal is to get students to the point where they are able to start to do some data manipulation and utilize code they haven't created (packages, functions)
@@ -5840,7 +5846,7 @@
 ### Readings
 [Introduction to Machine Learning with Python (Chapter 1)](http://proquestcombo.safaribooksonline.com.libproxy.rpi.edu/book/programming/machine-learning/9781449369880)
 ### Notebooks
-Twitter - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/04-viz-api-scraper/01_intro_api_twitter.ipynb)&lt;br&gt;Web Mining - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/04-viz-api-scraper/02_intro_python_webmining.ipynb)&lt;br&gt;Visualizations - Seaborn - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/04-viz-api-scraper/03_visualization_python_seaborn.ipynb)&lt;br&gt;Strings - Regular Expressions - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/04-viz-api-scraper/04_strings_and_regular_expressions.ipynb)&lt;br&gt;Feature Dummies - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/04-viz-api-scraper/05_features_dummies.ipynb)&lt;br&gt;Assignment 3 - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/04-viz-api-scraper/hm-03/hm03.ipynb)</v>
+&lt;br&gt;&lt;br&gt;&lt;br&gt;&lt;br&gt;&lt;br&gt;</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="15" customHeight="1">
@@ -5879,7 +5885,7 @@
 ### Readings
 ",IF(Schedule!L10,LOOKUP(Schedule!B10,Readings!A:A,Readings!F:F),"*None*"),"
 ### Notebooks
-",IF(Schedule!M10,LOOKUP(Schedule!B10,Notebooks!A:A,Notebooks!G:G),"*None*"))</f>
+",IF(Schedule!M10,LOOKUP(Schedule!B10,Notebooks!A:A,Notebooks!L:L),"*None*"))</f>
         <v xml:space="preserve">
 ### Description
 Lab/homework
@@ -5927,7 +5933,7 @@
 ### Readings
 ",IF(Schedule!L11,LOOKUP(Schedule!B11,Readings!A:A,Readings!F:F),"*None*"),"
 ### Notebooks
-",IF(Schedule!M11,LOOKUP(Schedule!B11,Notebooks!A:A,Notebooks!G:G),"*None*"))</f>
+",IF(Schedule!M11,LOOKUP(Schedule!B11,Notebooks!A:A,Notebooks!L:L),"*None*"))</f>
         <v xml:space="preserve">
 ### Description
 Visualization is an important component of data understanding. 
@@ -5955,7 +5961,7 @@
 ### Readings
 *None*
 ### Notebooks
-The Simplest Neural Network with Numpy - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/05-intro-modeling/01-Neural-Networks.ipynb)&lt;br&gt;Train Test Split - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/05-intro-modeling/01-training-test-split.ipynb)&lt;br&gt;Introduction to Logistic Regression - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/05-intro-modeling/02-intro-logistic-knn.ipynb)&lt;br&gt;K Nearest Neighbor - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/05-intro-modeling/03-knn.ipynb)&lt;br&gt;ROC and SVM - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/05-intro-modeling/04-svm-roc.ipynb)&lt;br&gt;HM5A Visualization &amp; Screen Scraping - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/05-intro-modeling/hm5/homework_05A.ipynb)&lt;br&gt;HM5B Intro Modeling - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/05-intro-modeling/hm5/homework_05B.ipynb)</v>
+&lt;br&gt;&lt;br&gt;&lt;br&gt;&lt;br&gt;&lt;br&gt;&lt;br&gt;</v>
       </c>
       <c r="C11" s="12" t="s">
         <v>18</v>
@@ -5975,7 +5981,7 @@
 ### Readings
 ",IF(Schedule!L12,LOOKUP(Schedule!B12,Readings!A:A,Readings!F:F),"*None*"),"
 ### Notebooks
-",IF(Schedule!M12,LOOKUP(Schedule!B12,Notebooks!A:A,Notebooks!G:G),"*None*"))</f>
+",IF(Schedule!M12,LOOKUP(Schedule!B12,Notebooks!A:A,Notebooks!L:L),"*None*"))</f>
         <v xml:space="preserve">
 ### Description
 Lab/homework
@@ -5984,7 +5990,7 @@
 ### Readings
 *None*
 ### Notebooks
-The Simplest Neural Network with Numpy - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/05-intro-modeling/01-Neural-Networks.ipynb)&lt;br&gt;Train Test Split - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/05-intro-modeling/01-training-test-split.ipynb)&lt;br&gt;Introduction to Logistic Regression - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/05-intro-modeling/02-intro-logistic-knn.ipynb)&lt;br&gt;K Nearest Neighbor - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/05-intro-modeling/03-knn.ipynb)&lt;br&gt;ROC and SVM - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/05-intro-modeling/04-svm-roc.ipynb)&lt;br&gt;HM5A Visualization &amp; Screen Scraping - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/05-intro-modeling/hm5/homework_05A.ipynb)&lt;br&gt;HM5B Intro Modeling - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/05-intro-modeling/hm5/homework_05B.ipynb)</v>
+&lt;br&gt;&lt;br&gt;&lt;br&gt;&lt;br&gt;&lt;br&gt;&lt;br&gt;</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="15" customHeight="1">
@@ -6023,7 +6029,7 @@
 ### Readings
 ",IF(Schedule!L13,LOOKUP(Schedule!B13,Readings!A:A,Readings!F:F),"*None*"),"
 ### Notebooks
-",IF(Schedule!M13,LOOKUP(Schedule!B13,Notebooks!A:A,Notebooks!G:G),"*None*"))</f>
+",IF(Schedule!M13,LOOKUP(Schedule!B13,Notebooks!A:A,Notebooks!L:L),"*None*"))</f>
         <v xml:space="preserve">
 ### Description
 The goal of this class is to get you familiar to using R. While we will be Jupyter notebooks, we will also examine using RStudio. Now that you have already started with Python, many of the concepts will map.
@@ -6071,7 +6077,7 @@
 ### Readings
 ",IF(Schedule!L14,LOOKUP(Schedule!B14,Readings!A:A,Readings!F:F),"*None*"),"
 ### Notebooks
-",IF(Schedule!M14,LOOKUP(Schedule!B14,Notebooks!A:A,Notebooks!G:G),"*None*"))</f>
+",IF(Schedule!M14,LOOKUP(Schedule!B14,Notebooks!A:A,Notebooks!L:L),"*None*"))</f>
         <v xml:space="preserve">
 ### Description
 Lab/homework
@@ -6119,7 +6125,7 @@
 ### Readings
 ",IF(Schedule!L15,LOOKUP(Schedule!B15,Readings!A:A,Readings!F:F),"*None*"),"
 ### Notebooks
-",IF(Schedule!M15,LOOKUP(Schedule!B15,Notebooks!A:A,Notebooks!G:G),"*None*"))</f>
+",IF(Schedule!M15,LOOKUP(Schedule!B15,Notebooks!A:A,Notebooks!L:L),"*None*"))</f>
         <v xml:space="preserve">
 ### Description
 We examine the basics of classess of supervised, unsupervised, reenforcement learning. Also examine overfitting and how cross validation is used for overfitting and how hypterparameters are used to optimize models. 
@@ -6147,7 +6153,7 @@
 ### Readings
 *None*
 ### Notebooks
-Matrix Regression - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/07-intro-modeling2/Python/01-matrix-regression-gradient-decent-python.ipynb)&lt;br&gt;Regression Basics - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/07-intro-modeling2/Python/02-regression-boston-housing-python.ipynb)&lt;br&gt;Ridge and Lasso Regression - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/07-intro-modeling2/Python/03-ridge-lasso-python.ipynb)</v>
+&lt;br&gt;&lt;br&gt;</v>
       </c>
       <c r="C15" s="12" t="s">
         <v>18</v>
@@ -6167,7 +6173,7 @@
 ### Readings
 ",IF(Schedule!L16,LOOKUP(Schedule!B16,Readings!A:A,Readings!F:F),"*None*"),"
 ### Notebooks
-",IF(Schedule!M16,LOOKUP(Schedule!B16,Notebooks!A:A,Notebooks!G:G),"*None*"))</f>
+",IF(Schedule!M16,LOOKUP(Schedule!B16,Notebooks!A:A,Notebooks!L:L),"*None*"))</f>
         <v xml:space="preserve">
 ### Description
 Lab/homework
@@ -6176,7 +6182,7 @@
 ### Readings
 *None*
 ### Notebooks
-Matrix Regression - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/07-intro-modeling2/Python/01-matrix-regression-gradient-decent-python.ipynb)&lt;br&gt;Regression Basics - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/07-intro-modeling2/Python/02-regression-boston-housing-python.ipynb)&lt;br&gt;Ridge and Lasso Regression - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/07-intro-modeling2/Python/03-ridge-lasso-python.ipynb)</v>
+&lt;br&gt;&lt;br&gt;</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="15" customHeight="1">
@@ -6215,7 +6221,7 @@
 ### Readings
 ",IF(Schedule!L17,LOOKUP(Schedule!B17,Readings!A:A,Readings!F:F),"*None*"),"
 ### Notebooks
-",IF(Schedule!M17,LOOKUP(Schedule!B17,Notebooks!A:A,Notebooks!G:G),"*None*"))</f>
+",IF(Schedule!M17,LOOKUP(Schedule!B17,Notebooks!A:A,Notebooks!L:L),"*None*"))</f>
         <v xml:space="preserve">
 ### Description
 *None*
@@ -6243,7 +6249,7 @@
 ### Readings
 *None*
 ### Notebooks
-Ridge and Lasso Regression - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/07-intro-modeling2/Python/03-ridge-lasso-python.ipynb)&lt;br&gt;PCA - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/07-intro-modeling2/Python/04_introduction_pca.ipynb)</v>
+&lt;br&gt;</v>
       </c>
       <c r="C17" s="12" t="s">
         <v>18</v>
@@ -6263,7 +6269,7 @@
 ### Readings
 ",IF(Schedule!L18,LOOKUP(Schedule!B18,Readings!A:A,Readings!F:F),"*None*"),"
 ### Notebooks
-",IF(Schedule!M18,LOOKUP(Schedule!B18,Notebooks!A:A,Notebooks!G:G),"*None*"))</f>
+",IF(Schedule!M18,LOOKUP(Schedule!B18,Notebooks!A:A,Notebooks!L:L),"*None*"))</f>
         <v xml:space="preserve">
 ### Description
 *None*
@@ -6272,7 +6278,7 @@
 ### Readings
 *None*
 ### Notebooks
-Ridge and Lasso Regression - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/07-intro-modeling2/Python/03-ridge-lasso-python.ipynb)&lt;br&gt;PCA - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/07-intro-modeling2/Python/04_introduction_pca.ipynb)</v>
+&lt;br&gt;</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="15" customHeight="1">
@@ -6311,7 +6317,7 @@
 ### Readings
 ",IF(Schedule!L19,LOOKUP(Schedule!B19,Readings!A:A,Readings!F:F),"*None*"),"
 ### Notebooks
-",IF(Schedule!M19,LOOKUP(Schedule!B19,Notebooks!A:A,Notebooks!G:G),"*None*"))</f>
+",IF(Schedule!M19,LOOKUP(Schedule!B19,Notebooks!A:A,Notebooks!L:L),"*None*"))</f>
         <v xml:space="preserve">
 ### Description
 Classifcation is one of the critical machine learning applications.  In this class we review a variety of different approaches. 
@@ -6359,7 +6365,7 @@
 ### Readings
 ",IF(Schedule!L20,LOOKUP(Schedule!B20,Readings!A:A,Readings!F:F),"*None*"),"
 ### Notebooks
-",IF(Schedule!M20,LOOKUP(Schedule!B20,Notebooks!A:A,Notebooks!G:G),"*None*"))</f>
+",IF(Schedule!M20,LOOKUP(Schedule!B20,Notebooks!A:A,Notebooks!L:L),"*None*"))</f>
         <v xml:space="preserve">
 ### Description
 Lab/homework
@@ -6407,7 +6413,7 @@
 ### Readings
 ",IF(Schedule!L21,LOOKUP(Schedule!B21,Readings!A:A,Readings!F:F),"*None*"),"
 ### Notebooks
-",IF(Schedule!M21,LOOKUP(Schedule!B21,Notebooks!A:A,Notebooks!G:G),"*None*"))</f>
+",IF(Schedule!M21,LOOKUP(Schedule!B21,Notebooks!A:A,Notebooks!L:L),"*None*"))</f>
         <v xml:space="preserve">
 ### Description
 Regression models similarly a a major type of machine learning application.  In this 
@@ -6455,7 +6461,7 @@
 ### Readings
 ",IF(Schedule!L22,LOOKUP(Schedule!B22,Readings!A:A,Readings!F:F),"*None*"),"
 ### Notebooks
-",IF(Schedule!M22,LOOKUP(Schedule!B22,Notebooks!A:A,Notebooks!G:G),"*None*"))</f>
+",IF(Schedule!M22,LOOKUP(Schedule!B22,Notebooks!A:A,Notebooks!L:L),"*None*"))</f>
         <v xml:space="preserve">
 ### Description
 Lab/homework
@@ -6503,7 +6509,7 @@
 ### Readings
 ",IF(Schedule!L23,LOOKUP(Schedule!B23,Readings!A:A,Readings!F:F),"*None*"),"
 ### Notebooks
-",IF(Schedule!M23,LOOKUP(Schedule!B23,Notebooks!A:A,Notebooks!G:G),"*None*"))</f>
+",IF(Schedule!M23,LOOKUP(Schedule!B23,Notebooks!A:A,Notebooks!L:L),"*None*"))</f>
         <v xml:space="preserve">
 ### Description
 The goal of this class is to investigate basic concepts surrounding text mining.
@@ -6551,7 +6557,7 @@
 ### Readings
 ",IF(Schedule!L24,LOOKUP(Schedule!B24,Readings!A:A,Readings!F:F),"*None*"),"
 ### Notebooks
-",IF(Schedule!M24,LOOKUP(Schedule!B24,Notebooks!A:A,Notebooks!G:G),"*None*"))</f>
+",IF(Schedule!M24,LOOKUP(Schedule!B24,Notebooks!A:A,Notebooks!L:L),"*None*"))</f>
         <v xml:space="preserve">
 ### Description
 Lab/homework
@@ -6599,7 +6605,7 @@
 ### Readings
 ",IF(Schedule!L25,LOOKUP(Schedule!B25,Readings!A:A,Readings!F:F),"*None*"),"
 ### Notebooks
-",IF(Schedule!M25,LOOKUP(Schedule!B25,Notebooks!A:A,Notebooks!G:G),"*None*"))</f>
+",IF(Schedule!M25,LOOKUP(Schedule!B25,Notebooks!A:A,Notebooks!L:L),"*None*"))</f>
         <v xml:space="preserve">
 ### Description
 The goal here is to provide an overview of how data processes can be scaled with Spark.
@@ -6647,7 +6653,7 @@
 ### Readings
 ",IF(Schedule!L26,LOOKUP(Schedule!B26,Readings!A:A,Readings!F:F),"*None*"),"
 ### Notebooks
-",IF(Schedule!M26,LOOKUP(Schedule!B26,Notebooks!A:A,Notebooks!G:G),"*None*"))</f>
+",IF(Schedule!M26,LOOKUP(Schedule!B26,Notebooks!A:A,Notebooks!L:L),"*None*"))</f>
         <v xml:space="preserve">
 ### Description
 Time series and panel data is a bit different and requires a different approach.  Here we cover some of the basics. 
@@ -6695,7 +6701,7 @@
 ### Readings
 ",IF(Schedule!L27,LOOKUP(Schedule!B27,Readings!A:A,Readings!F:F),"*None*"),"
 ### Notebooks
-",IF(Schedule!M27,LOOKUP(Schedule!B27,Notebooks!A:A,Notebooks!G:G),"*None*"))</f>
+",IF(Schedule!M27,LOOKUP(Schedule!B27,Notebooks!A:A,Notebooks!L:L),"*None*"))</f>
         <v xml:space="preserve">
 ### Description
 Image data is different and deep learning has transformed the ability of machines to process image data. In this lecture we will get an overview of image processing and deep learning techniques. 
@@ -6743,7 +6749,7 @@
 ### Readings
 ",IF(Schedule!L28,LOOKUP(Schedule!B28,Readings!A:A,Readings!F:F),"*None*"),"
 ### Notebooks
-",IF(Schedule!M28,LOOKUP(Schedule!B28,Notebooks!A:A,Notebooks!G:G),"*None*"))</f>
+",IF(Schedule!M28,LOOKUP(Schedule!B28,Notebooks!A:A,Notebooks!L:L),"*None*"))</f>
         <v xml:space="preserve">
 ### Description
 Lab/homework
@@ -6791,7 +6797,7 @@
 ### Readings
 ",IF(Schedule!L29,LOOKUP(Schedule!B29,Readings!A:A,Readings!F:F),"*None*"),"
 ### Notebooks
-",IF(Schedule!M29,LOOKUP(Schedule!B29,Notebooks!A:A,Notebooks!G:G),"*None*"))</f>
+",IF(Schedule!M29,LOOKUP(Schedule!B29,Notebooks!A:A,Notebooks!L:L),"*None*"))</f>
         <v xml:space="preserve">
 ### Description
 Increasingly there are tools to automate the process of selecting models. 
@@ -6839,7 +6845,7 @@
 ### Readings
 ",IF(Schedule!L30,LOOKUP(Schedule!B30,Readings!A:A,Readings!F:F),"*None*"),"
 ### Notebooks
-",IF(Schedule!M30,LOOKUP(Schedule!B30,Notebooks!A:A,Notebooks!G:G),"*None*"))</f>
+",IF(Schedule!M30,LOOKUP(Schedule!B30,Notebooks!A:A,Notebooks!L:L),"*None*"))</f>
         <v xml:space="preserve">
 ### Description
 *None*
@@ -6887,7 +6893,7 @@
 ### Readings
 ",IF(Schedule!L31,LOOKUP(Schedule!B31,Readings!A:A,Readings!F:F),"*None*"),"
 ### Notebooks
-",IF(Schedule!M31,LOOKUP(Schedule!B31,Notebooks!A:A,Notebooks!G:G),"*None*"))</f>
+",IF(Schedule!M31,LOOKUP(Schedule!B31,Notebooks!A:A,Notebooks!L:L),"*None*"))</f>
         <v xml:space="preserve">
 ### Description
 Lab/homework
@@ -6935,7 +6941,7 @@
 ### Readings
 ",IF(Schedule!L32,LOOKUP(Schedule!B32,Readings!A:A,Readings!F:F),"*None*"),"
 ### Notebooks
-",IF(Schedule!M32,LOOKUP(Schedule!B32,Notebooks!A:A,Notebooks!G:G),"*None*"))</f>
+",IF(Schedule!M32,LOOKUP(Schedule!B32,Notebooks!A:A,Notebooks!L:L),"*None*"))</f>
         <v xml:space="preserve">
 ### Description
 *None*
@@ -6983,7 +6989,7 @@
 ### Readings
 ",IF(Schedule!L33,LOOKUP(Schedule!B33,Readings!A:A,Readings!F:F),"*None*"),"
 ### Notebooks
-",IF(Schedule!M33,LOOKUP(Schedule!B33,Notebooks!A:A,Notebooks!G:G),"*None*"))</f>
+",IF(Schedule!M33,LOOKUP(Schedule!B33,Notebooks!A:A,Notebooks!L:L),"*None*"))</f>
         <v xml:space="preserve">
 ### Description
 *None*
@@ -7031,7 +7037,7 @@
 ### Readings
 ",IF(Schedule!L34,LOOKUP(Schedule!B34,Readings!A:A,Readings!F:F),"*None*"),"
 ### Notebooks
-",IF(Schedule!M34,LOOKUP(Schedule!B34,Notebooks!A:A,Notebooks!G:G),"*None*"))</f>
+",IF(Schedule!M34,LOOKUP(Schedule!B34,Notebooks!A:A,Notebooks!L:L),"*None*"))</f>
         <v xml:space="preserve">
 ### Description
 *None*
@@ -7049,642 +7055,6 @@
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{515BB05E-4CB6-4E1D-95DD-C7D7E7D05461}">
-  <sheetPr>
-    <outlinePr summaryBelow="0" summaryRight="0"/>
-  </sheetPr>
-  <dimension ref="A1:F24"/>
-  <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="11.09765625" defaultRowHeight="15" customHeight="1"/>
-  <cols>
-    <col min="1" max="1" width="11.09765625" style="31"/>
-    <col min="2" max="4" width="45" style="31" customWidth="1"/>
-    <col min="5" max="16384" width="11.09765625" style="31"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" ht="15.6">
-      <c r="B1" s="11"/>
-      <c r="C1" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="D1" s="11" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" ht="15" customHeight="1">
-      <c r="A2" s="30" t="str">
-        <f>IF(ISBLANK(Schedule!H3),"",CONCATENATE("assign",Schedule!H3))</f>
-        <v/>
-      </c>
-      <c r="B2" s="19" t="str">
-        <f>CONCATENATE(C2,D2)</f>
-        <v/>
-      </c>
-      <c r="C2" s="31" t="str">
-        <f>IF(ISBLANK(Schedule!H3),"",CONCATENATE("&lt;h1 style="&amp;CHAR(34)&amp;"font-family: Verdana, Geneva, sans-serif; text-align:center;"&amp;CHAR(34)&amp;"&gt;Assignment ",Schedule!H3,"&lt;/h1&gt;
----"))</f>
-        <v/>
-      </c>
-      <c r="D2" s="11" t="str">
-        <f>IF(ISBLANK(Schedule!H3),"",CONCATENATE("
-### Description
-",IF(ISBLANK(Schedule!I3),"*None*",Schedule!I3),"
-### Instructions
-",IF(ISBLANK(Schedule!J3),"*None*",Schedule!J3),"
-### Link
-",IF(ISBLANK(Schedule!K8),"*None*",Schedule!R8)))</f>
-        <v/>
-      </c>
-      <c r="F2" s="30"/>
-    </row>
-    <row r="3" spans="1:6" ht="15" customHeight="1">
-      <c r="A3" s="30" t="str">
-        <f>IF(ISBLANK(Schedule!H4),"",CONCATENATE("assign",Schedule!H4))</f>
-        <v/>
-      </c>
-      <c r="B3" s="19" t="str">
-        <f>CONCATENATE(C3,D3)</f>
-        <v/>
-      </c>
-      <c r="C3" s="31" t="str">
-        <f>IF(ISBLANK(Schedule!H4),"",CONCATENATE("&lt;h1 style="&amp;CHAR(34)&amp;"font-family: Verdana, Geneva, sans-serif; text-align:center;"&amp;CHAR(34)&amp;"&gt;Assignment ",Schedule!H4,"&lt;/h1&gt;
----"))</f>
-        <v/>
-      </c>
-      <c r="D3" s="11" t="str">
-        <f>IF(ISBLANK(Schedule!H4),"",CONCATENATE("
-### Description
-",IF(ISBLANK(Schedule!I4),"*None*",Schedule!I4),"
-### Instructions
-",IF(ISBLANK(Schedule!J4),"*None*",Schedule!J4),"
-### Link
-",IF(ISBLANK(Schedule!K9),"*None*",Schedule!R9)))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="15" customHeight="1">
-      <c r="A4" s="30" t="str">
-        <f>IF(ISBLANK(Schedule!H5),"",CONCATENATE("assign",Schedule!H5))</f>
-        <v>assign1</v>
-      </c>
-      <c r="B4" s="19" t="str">
-        <f>CONCATENATE(C4,D4)</f>
-        <v>&lt;h1 style="font-family: Verdana, Geneva, sans-serif; text-align:center"&gt;Assignment 1&lt;/h1&gt;
----
-### Description
-This introductory assignment introduces the basics of loading files from a variety of formats. 
-### Instructions
-*None*
-### Link
-[![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/04-viz-api-scraper/hm-03/hm03.ipynb)</v>
-      </c>
-      <c r="C4" s="31" t="str">
-        <f>IF(ISBLANK(Schedule!H5),"",CONCATENATE("&lt;h1 style="&amp;CHAR(34)&amp;"font-family: Verdana, Geneva, sans-serif; text-align:center"&amp;CHAR(34)&amp;"&gt;Assignment ",Schedule!H5,"&lt;/h1&gt;
----"))</f>
-        <v>&lt;h1 style="font-family: Verdana, Geneva, sans-serif; text-align:center"&gt;Assignment 1&lt;/h1&gt;
----</v>
-      </c>
-      <c r="D4" s="11" t="str">
-        <f>IF(ISBLANK(Schedule!H5),"",CONCATENATE("
-### Description
-",IF(ISBLANK(Schedule!I5),"*None*",Schedule!I5),"
-### Instructions
-",IF(ISBLANK(Schedule!J5),"*None*",Schedule!J5),"
-### Link
-",IF(ISBLANK(Schedule!K10),"*None*",Schedule!R10)))</f>
-        <v xml:space="preserve">
-### Description
-This introductory assignment introduces the basics of loading files from a variety of formats. 
-### Instructions
-*None*
-### Link
-[![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/04-viz-api-scraper/hm-03/hm03.ipynb)</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="15" customHeight="1">
-      <c r="A5" s="30" t="str">
-        <f>IF(ISBLANK(Schedule!H6),"",CONCATENATE("assign",Schedule!H6))</f>
-        <v/>
-      </c>
-      <c r="B5" s="19" t="str">
-        <f t="shared" ref="B5:B24" si="0">CONCATENATE(C5,D5)</f>
-        <v/>
-      </c>
-      <c r="C5" s="31" t="str">
-        <f>IF(ISBLANK(Schedule!H6),"",CONCATENATE("&lt;h1 style="&amp;CHAR(34)&amp;"font-family: Verdana, Geneva, sans-serif; text-align:center"&amp;CHAR(34)&amp;"&gt;Assignment ",Schedule!H6,"&lt;/h1&gt;
----"))</f>
-        <v/>
-      </c>
-      <c r="D5" s="11" t="str">
-        <f>IF(ISBLANK(Schedule!H6),"",CONCATENATE("
-### Description
-",IF(ISBLANK(Schedule!I6),"*None*",Schedule!I6),"
-### Instructions
-",IF(ISBLANK(Schedule!J6),"*None*",Schedule!J6),"
-### Link
-",IF(ISBLANK(Schedule!K11),"*None*",Schedule!R11)))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="15" customHeight="1">
-      <c r="A6" s="30" t="str">
-        <f>IF(ISBLANK(Schedule!H7),"",CONCATENATE("assign",Schedule!H7))</f>
-        <v/>
-      </c>
-      <c r="B6" s="19" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="C6" s="31" t="str">
-        <f>IF(ISBLANK(Schedule!H7),"",CONCATENATE("&lt;h1 style="&amp;CHAR(34)&amp;"font-family: Verdana, Geneva, sans-serif; text-align:center"&amp;CHAR(34)&amp;"&gt;Assignment ",Schedule!H7,"&lt;/h1&gt;
----"))</f>
-        <v/>
-      </c>
-      <c r="D6" s="11" t="str">
-        <f>IF(ISBLANK(Schedule!H7),"",CONCATENATE("
-### Description
-",IF(ISBLANK(Schedule!I7),"*None*",Schedule!I7),"
-### Instructions
-",IF(ISBLANK(Schedule!J7),"*None*",Schedule!J7),"
-### Link
-",IF(ISBLANK(Schedule!K12),"*None*",Schedule!R12)))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="15" customHeight="1">
-      <c r="A7" s="30" t="str">
-        <f>IF(ISBLANK(Schedule!H8),"",CONCATENATE("assign",Schedule!H8))</f>
-        <v>assign2</v>
-      </c>
-      <c r="B7" s="19" t="str">
-        <f t="shared" si="0"/>
-        <v>&lt;h1 style="font-family: Verdana, Geneva, sans-serif; text-align:center"&gt;Assignment 2&lt;/h1&gt;
----
-### Description
-*None*
-### Instructions
-*None*
-### Link
-*None*</v>
-      </c>
-      <c r="C7" s="31" t="str">
-        <f>IF(ISBLANK(Schedule!H8),"",CONCATENATE("&lt;h1 style="&amp;CHAR(34)&amp;"font-family: Verdana, Geneva, sans-serif; text-align:center"&amp;CHAR(34)&amp;"&gt;Assignment ",Schedule!H8,"&lt;/h1&gt;
----"))</f>
-        <v>&lt;h1 style="font-family: Verdana, Geneva, sans-serif; text-align:center"&gt;Assignment 2&lt;/h1&gt;
----</v>
-      </c>
-      <c r="D7" s="11" t="str">
-        <f>IF(ISBLANK(Schedule!H8),"",CONCATENATE("
-### Description
-",IF(ISBLANK(Schedule!I8),"*None*",Schedule!I8),"
-### Instructions
-",IF(ISBLANK(Schedule!J8),"*None*",Schedule!J8),"
-### Link
-",IF(ISBLANK(Schedule!K13),"*None*",Schedule!R13)))</f>
-        <v xml:space="preserve">
-### Description
-*None*
-### Instructions
-*None*
-### Link
-*None*</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="15" customHeight="1">
-      <c r="A8" s="30" t="str">
-        <f>IF(ISBLANK(Schedule!H9),"",CONCATENATE("assign",Schedule!H9))</f>
-        <v/>
-      </c>
-      <c r="B8" s="19" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="C8" s="31" t="str">
-        <f>IF(ISBLANK(Schedule!H9),"",CONCATENATE("&lt;h1 style="&amp;CHAR(34)&amp;"font-family: Verdana, Geneva, sans-serif; text-align:center"&amp;CHAR(34)&amp;"&gt;Assignment ",Schedule!H9,"&lt;/h1&gt;
----"))</f>
-        <v/>
-      </c>
-      <c r="D8" s="11" t="str">
-        <f>IF(ISBLANK(Schedule!H9),"",CONCATENATE("
-### Description
-",IF(ISBLANK(Schedule!I9),"*None*",Schedule!I9),"
-### Instructions
-",IF(ISBLANK(Schedule!J9),"*None*",Schedule!J9),"
-### Link
-",IF(ISBLANK(Schedule!K14),"*None*",Schedule!R14)))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="15" customHeight="1">
-      <c r="A9" s="30" t="str">
-        <f>IF(ISBLANK(Schedule!H10),"",CONCATENATE("assign",Schedule!H10))</f>
-        <v/>
-      </c>
-      <c r="B9" s="19" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="C9" s="31" t="str">
-        <f>IF(ISBLANK(Schedule!H10),"",CONCATENATE("&lt;h1 style="&amp;CHAR(34)&amp;"font-family: Verdana, Geneva, sans-serif; text-align:center"&amp;CHAR(34)&amp;"&gt;Assignment ",Schedule!H10,"&lt;/h1&gt;
----"))</f>
-        <v/>
-      </c>
-      <c r="D9" s="11" t="str">
-        <f>IF(ISBLANK(Schedule!H10),"",CONCATENATE("
-### Description
-",IF(ISBLANK(Schedule!I10),"*None*",Schedule!I10),"
-### Instructions
-",IF(ISBLANK(Schedule!J10),"*None*",Schedule!J10),"
-### Link
-",IF(ISBLANK(Schedule!K15),"*None*",Schedule!R15)))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="10" spans="1:6" ht="15" customHeight="1">
-      <c r="A10" s="30" t="str">
-        <f>IF(ISBLANK(Schedule!H11),"",CONCATENATE("assign",Schedule!H11))</f>
-        <v/>
-      </c>
-      <c r="B10" s="19" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="C10" s="31" t="str">
-        <f>IF(ISBLANK(Schedule!H11),"",CONCATENATE("&lt;h1 style="&amp;CHAR(34)&amp;"font-family: Verdana, Geneva, sans-serif; text-align:center"&amp;CHAR(34)&amp;"&gt;Assignment ",Schedule!H11,"&lt;/h1&gt;
----"))</f>
-        <v/>
-      </c>
-      <c r="D10" s="11" t="str">
-        <f>IF(ISBLANK(Schedule!H11),"",CONCATENATE("
-### Description
-",IF(ISBLANK(Schedule!I11),"*None*",Schedule!I11),"
-### Instructions
-",IF(ISBLANK(Schedule!J11),"*None*",Schedule!J11),"
-### Link
-",IF(ISBLANK(Schedule!K16),"*None*",Schedule!R16)))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="11" spans="1:6" ht="15" customHeight="1">
-      <c r="A11" s="30" t="str">
-        <f>IF(ISBLANK(Schedule!H12),"",CONCATENATE("assign",Schedule!H12))</f>
-        <v/>
-      </c>
-      <c r="B11" s="19" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="C11" s="31" t="str">
-        <f>IF(ISBLANK(Schedule!H12),"",CONCATENATE("&lt;h1 style="&amp;CHAR(34)&amp;"font-family: Verdana, Geneva, sans-serif; text-align:center"&amp;CHAR(34)&amp;"&gt;Assignment ",Schedule!H12,"&lt;/h1&gt;
----"))</f>
-        <v/>
-      </c>
-      <c r="D11" s="11" t="str">
-        <f>IF(ISBLANK(Schedule!H12),"",CONCATENATE("
-### Description
-",IF(ISBLANK(Schedule!I12),"*None*",Schedule!I12),"
-### Instructions
-",IF(ISBLANK(Schedule!J12),"*None*",Schedule!J12),"
-### Link
-",IF(ISBLANK(Schedule!K17),"*None*",Schedule!R17)))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="12" spans="1:6" ht="15" customHeight="1">
-      <c r="A12" s="30" t="str">
-        <f>IF(ISBLANK(Schedule!H13),"",CONCATENATE("assign",Schedule!H13))</f>
-        <v/>
-      </c>
-      <c r="B12" s="19" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="C12" s="31" t="str">
-        <f>IF(ISBLANK(Schedule!H13),"",CONCATENATE("&lt;h1 style="&amp;CHAR(34)&amp;"font-family: Verdana, Geneva, sans-serif; text-align:center"&amp;CHAR(34)&amp;"&gt;Assignment ",Schedule!H13,"&lt;/h1&gt;
----"))</f>
-        <v/>
-      </c>
-      <c r="D12" s="11" t="str">
-        <f>IF(ISBLANK(Schedule!H13),"",CONCATENATE("
-### Description
-",IF(ISBLANK(Schedule!I13),"*None*",Schedule!I13),"
-### Instructions
-",IF(ISBLANK(Schedule!J13),"*None*",Schedule!J13),"
-### Link
-",IF(ISBLANK(Schedule!K18),"*None*",Schedule!R18)))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="13" spans="1:6" ht="15" customHeight="1">
-      <c r="A13" s="30" t="str">
-        <f>IF(ISBLANK(Schedule!H14),"",CONCATENATE("assign",Schedule!H14))</f>
-        <v/>
-      </c>
-      <c r="B13" s="19" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="C13" s="31" t="str">
-        <f>IF(ISBLANK(Schedule!H14),"",CONCATENATE("&lt;h1 style="&amp;CHAR(34)&amp;"font-family: Verdana, Geneva, sans-serif; text-align:center"&amp;CHAR(34)&amp;"&gt;Assignment ",Schedule!H14,"&lt;/h1&gt;
----"))</f>
-        <v/>
-      </c>
-      <c r="D13" s="11" t="str">
-        <f>IF(ISBLANK(Schedule!H14),"",CONCATENATE("
-### Description
-",IF(ISBLANK(Schedule!I14),"*None*",Schedule!I14),"
-### Instructions
-",IF(ISBLANK(Schedule!J14),"*None*",Schedule!J14),"
-### Link
-",IF(ISBLANK(Schedule!K19),"*None*",Schedule!R19)))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="14" spans="1:6" ht="15" customHeight="1">
-      <c r="A14" s="30" t="str">
-        <f>IF(ISBLANK(Schedule!H15),"",CONCATENATE("assign",Schedule!H15))</f>
-        <v/>
-      </c>
-      <c r="B14" s="19" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="C14" s="31" t="str">
-        <f>IF(ISBLANK(Schedule!H15),"",CONCATENATE("&lt;h1 style="&amp;CHAR(34)&amp;"font-family: Verdana, Geneva, sans-serif; text-align:center"&amp;CHAR(34)&amp;"&gt;Assignment ",Schedule!H15,"&lt;/h1&gt;
----"))</f>
-        <v/>
-      </c>
-      <c r="D14" s="11" t="str">
-        <f>IF(ISBLANK(Schedule!H15),"",CONCATENATE("
-### Description
-",IF(ISBLANK(Schedule!I15),"*None*",Schedule!I15),"
-### Instructions
-",IF(ISBLANK(Schedule!J15),"*None*",Schedule!J15),"
-### Link
-",IF(ISBLANK(Schedule!K20),"*None*",Schedule!R20)))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="15" spans="1:6" ht="15" customHeight="1">
-      <c r="A15" s="30" t="str">
-        <f>IF(ISBLANK(Schedule!H16),"",CONCATENATE("assign",Schedule!H16))</f>
-        <v/>
-      </c>
-      <c r="B15" s="19" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="C15" s="31" t="str">
-        <f>IF(ISBLANK(Schedule!H16),"",CONCATENATE("&lt;h1 style="&amp;CHAR(34)&amp;"font-family: Verdana, Geneva, sans-serif; text-align:center"&amp;CHAR(34)&amp;"&gt;Assignment ",Schedule!H16,"&lt;/h1&gt;
----"))</f>
-        <v/>
-      </c>
-      <c r="D15" s="11" t="str">
-        <f>IF(ISBLANK(Schedule!H16),"",CONCATENATE("
-### Description
-",IF(ISBLANK(Schedule!I16),"*None*",Schedule!I16),"
-### Instructions
-",IF(ISBLANK(Schedule!J16),"*None*",Schedule!J16),"
-### Link
-",IF(ISBLANK(Schedule!K21),"*None*",Schedule!R21)))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="16" spans="1:6" ht="15" customHeight="1">
-      <c r="A16" s="30" t="str">
-        <f>IF(ISBLANK(Schedule!H17),"",CONCATENATE("assign",Schedule!H17))</f>
-        <v/>
-      </c>
-      <c r="B16" s="19" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="C16" s="31" t="str">
-        <f>IF(ISBLANK(Schedule!H17),"",CONCATENATE("&lt;h1 style="&amp;CHAR(34)&amp;"font-family: Verdana, Geneva, sans-serif; text-align:center"&amp;CHAR(34)&amp;"&gt;Assignment ",Schedule!H17,"&lt;/h1&gt;
----"))</f>
-        <v/>
-      </c>
-      <c r="D16" s="11" t="str">
-        <f>IF(ISBLANK(Schedule!H17),"",CONCATENATE("
-### Description
-",IF(ISBLANK(Schedule!I17),"*None*",Schedule!I17),"
-### Instructions
-",IF(ISBLANK(Schedule!J17),"*None*",Schedule!J17),"
-### Link
-",IF(ISBLANK(Schedule!K22),"*None*",Schedule!R22)))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="17" spans="1:4" ht="15" customHeight="1">
-      <c r="A17" s="30" t="str">
-        <f>IF(ISBLANK(Schedule!H18),"",CONCATENATE("assign",Schedule!H18))</f>
-        <v/>
-      </c>
-      <c r="B17" s="19" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="C17" s="31" t="str">
-        <f>IF(ISBLANK(Schedule!H18),"",CONCATENATE("&lt;h1 style="&amp;CHAR(34)&amp;"font-family: Verdana, Geneva, sans-serif; text-align:center"&amp;CHAR(34)&amp;"&gt;Assignment ",Schedule!H18,"&lt;/h1&gt;
----"))</f>
-        <v/>
-      </c>
-      <c r="D17" s="11" t="str">
-        <f>IF(ISBLANK(Schedule!H18),"",CONCATENATE("
-### Description
-",IF(ISBLANK(Schedule!I18),"*None*",Schedule!I18),"
-### Instructions
-",IF(ISBLANK(Schedule!J18),"*None*",Schedule!J18),"
-### Link
-",IF(ISBLANK(Schedule!K23),"*None*",Schedule!R23)))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="18" spans="1:4" ht="15" customHeight="1">
-      <c r="A18" s="30" t="str">
-        <f>IF(ISBLANK(Schedule!H19),"",CONCATENATE("assign",Schedule!H19))</f>
-        <v/>
-      </c>
-      <c r="B18" s="19" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="C18" s="31" t="str">
-        <f>IF(ISBLANK(Schedule!H19),"",CONCATENATE("&lt;h1 style="&amp;CHAR(34)&amp;"font-family: Verdana, Geneva, sans-serif; text-align:center"&amp;CHAR(34)&amp;"&gt;Assignment ",Schedule!H19,"&lt;/h1&gt;
----"))</f>
-        <v/>
-      </c>
-      <c r="D18" s="11" t="str">
-        <f>IF(ISBLANK(Schedule!H19),"",CONCATENATE("
-### Description
-",IF(ISBLANK(Schedule!I19),"*None*",Schedule!I19),"
-### Instructions
-",IF(ISBLANK(Schedule!J19),"*None*",Schedule!J19),"
-### Link
-",IF(ISBLANK(Schedule!K24),"*None*",Schedule!R24)))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="19" spans="1:4" ht="15" customHeight="1">
-      <c r="A19" s="30" t="str">
-        <f>IF(ISBLANK(Schedule!H20),"",CONCATENATE("assign",Schedule!H20))</f>
-        <v/>
-      </c>
-      <c r="B19" s="19" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="C19" s="31" t="str">
-        <f>IF(ISBLANK(Schedule!H20),"",CONCATENATE("&lt;h1 style="&amp;CHAR(34)&amp;"font-family: Verdana, Geneva, sans-serif; text-align:center"&amp;CHAR(34)&amp;"&gt;Assignment ",Schedule!H20,"&lt;/h1&gt;
----"))</f>
-        <v/>
-      </c>
-      <c r="D19" s="11" t="str">
-        <f>IF(ISBLANK(Schedule!H20),"",CONCATENATE("
-### Description
-",IF(ISBLANK(Schedule!I20),"*None*",Schedule!I20),"
-### Instructions
-",IF(ISBLANK(Schedule!J20),"*None*",Schedule!J20),"
-### Link
-",IF(ISBLANK(Schedule!K25),"*None*",Schedule!R25)))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="20" spans="1:4" ht="15" customHeight="1">
-      <c r="A20" s="30" t="str">
-        <f>IF(ISBLANK(Schedule!H21),"",CONCATENATE("assign",Schedule!H21))</f>
-        <v/>
-      </c>
-      <c r="B20" s="19" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="C20" s="31" t="str">
-        <f>IF(ISBLANK(Schedule!H21),"",CONCATENATE("&lt;h1 style="&amp;CHAR(34)&amp;"font-family: Verdana, Geneva, sans-serif; text-align:center"&amp;CHAR(34)&amp;"&gt;Assignment ",Schedule!H21,"&lt;/h1&gt;
----"))</f>
-        <v/>
-      </c>
-      <c r="D20" s="11" t="str">
-        <f>IF(ISBLANK(Schedule!H21),"",CONCATENATE("
-### Description
-",IF(ISBLANK(Schedule!I21),"*None*",Schedule!I21),"
-### Instructions
-",IF(ISBLANK(Schedule!J21),"*None*",Schedule!J21),"
-### Link
-",IF(ISBLANK(Schedule!K26),"*None*",Schedule!R26)))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="21" spans="1:4" ht="15" customHeight="1">
-      <c r="A21" s="30" t="str">
-        <f>IF(ISBLANK(Schedule!H22),"",CONCATENATE("assign",Schedule!H22))</f>
-        <v/>
-      </c>
-      <c r="B21" s="19" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="C21" s="31" t="str">
-        <f>IF(ISBLANK(Schedule!H22),"",CONCATENATE("&lt;h1 style="&amp;CHAR(34)&amp;"font-family: Verdana, Geneva, sans-serif; text-align:center"&amp;CHAR(34)&amp;"&gt;Assignment ",Schedule!H22,"&lt;/h1&gt;
----"))</f>
-        <v/>
-      </c>
-      <c r="D21" s="11" t="str">
-        <f>IF(ISBLANK(Schedule!H22),"",CONCATENATE("
-### Description
-",IF(ISBLANK(Schedule!I22),"*None*",Schedule!I22),"
-### Instructions
-",IF(ISBLANK(Schedule!J22),"*None*",Schedule!J22),"
-### Link
-",IF(ISBLANK(Schedule!K27),"*None*",Schedule!R27)))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="22" spans="1:4" ht="15" customHeight="1">
-      <c r="A22" s="30" t="str">
-        <f>IF(ISBLANK(Schedule!H23),"",CONCATENATE("assign",Schedule!H23))</f>
-        <v/>
-      </c>
-      <c r="B22" s="19" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="C22" s="31" t="str">
-        <f>IF(ISBLANK(Schedule!H23),"",CONCATENATE("&lt;h1 style="&amp;CHAR(34)&amp;"font-family: Verdana, Geneva, sans-serif; text-align:center"&amp;CHAR(34)&amp;"&gt;Assignment ",Schedule!H23,"&lt;/h1&gt;
----"))</f>
-        <v/>
-      </c>
-      <c r="D22" s="11" t="str">
-        <f>IF(ISBLANK(Schedule!H23),"",CONCATENATE("
-### Description
-",IF(ISBLANK(Schedule!I23),"*None*",Schedule!I23),"
-### Instructions
-",IF(ISBLANK(Schedule!J23),"*None*",Schedule!J23),"
-### Link
-",IF(ISBLANK(Schedule!K28),"*None*",Schedule!R28)))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="23" spans="1:4" ht="15" customHeight="1">
-      <c r="A23" s="30" t="str">
-        <f>IF(ISBLANK(Schedule!H24),"",CONCATENATE("assign",Schedule!H24))</f>
-        <v/>
-      </c>
-      <c r="B23" s="19" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="C23" s="31" t="str">
-        <f>IF(ISBLANK(Schedule!H24),"",CONCATENATE("&lt;h1 style="&amp;CHAR(34)&amp;"font-family: Verdana, Geneva, sans-serif; text-align:center"&amp;CHAR(34)&amp;"&gt;Assignment ",Schedule!H24,"&lt;/h1&gt;
----"))</f>
-        <v/>
-      </c>
-      <c r="D23" s="11" t="str">
-        <f>IF(ISBLANK(Schedule!H24),"",CONCATENATE("
-### Description
-",IF(ISBLANK(Schedule!I24),"*None*",Schedule!I24),"
-### Instructions
-",IF(ISBLANK(Schedule!J24),"*None*",Schedule!J24),"
-### Link
-",IF(ISBLANK(Schedule!K29),"*None*",Schedule!R29)))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="24" spans="1:4" ht="15" customHeight="1">
-      <c r="A24" s="30" t="str">
-        <f>IF(ISBLANK(Schedule!H25),"",CONCATENATE("assign",Schedule!H25))</f>
-        <v/>
-      </c>
-      <c r="B24" s="19" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="C24" s="31" t="str">
-        <f>IF(ISBLANK(Schedule!H25),"",CONCATENATE("&lt;h1 style="&amp;CHAR(34)&amp;"font-family: Verdana, Geneva, sans-serif; text-align:center"&amp;CHAR(34)&amp;"&gt;Assignment ",Schedule!H25,"&lt;/h1&gt;
----"))</f>
-        <v/>
-      </c>
-      <c r="D24" s="11" t="str">
-        <f>IF(ISBLANK(Schedule!H25),"",CONCATENATE("
-### Description
-",IF(ISBLANK(Schedule!I25),"*None*",Schedule!I25),"
-### Instructions
-",IF(ISBLANK(Schedule!J25),"*None*",Schedule!J25),"
-### Link
-",IF(ISBLANK(Schedule!K30),"*None*",Schedule!R30)))</f>
-        <v/>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <dimension ref="A1:A20"/>
   <sheetViews>
@@ -7819,7 +7189,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
   <dimension ref="A2:L929"/>
   <sheetViews>
@@ -29130,71 +28500,71 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:22" s="32" customFormat="1" ht="18.3" customHeight="1" thickBot="1">
-      <c r="A1" s="111" t="s">
+      <c r="A1" s="114" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="109" t="s">
+      <c r="B1" s="112" t="s">
         <v>707</v>
       </c>
-      <c r="C1" s="109" t="s">
+      <c r="C1" s="112" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="100" t="s">
+      <c r="D1" s="103" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="98" t="s">
+      <c r="E1" s="101" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="102" t="s">
-        <v>849</v>
-      </c>
-      <c r="G1" s="103"/>
-      <c r="H1" s="104" t="s">
-        <v>859</v>
-      </c>
-      <c r="I1" s="105"/>
-      <c r="J1" s="105"/>
-      <c r="K1" s="106"/>
-      <c r="L1" s="107" t="s">
-        <v>857</v>
-      </c>
-      <c r="M1" s="107" t="s">
-        <v>858</v>
-      </c>
-      <c r="N1" s="113" t="s">
+      <c r="F1" s="105" t="s">
+        <v>846</v>
+      </c>
+      <c r="G1" s="106"/>
+      <c r="H1" s="107" t="s">
+        <v>856</v>
+      </c>
+      <c r="I1" s="108"/>
+      <c r="J1" s="108"/>
+      <c r="K1" s="109"/>
+      <c r="L1" s="110" t="s">
+        <v>854</v>
+      </c>
+      <c r="M1" s="110" t="s">
+        <v>855</v>
+      </c>
+      <c r="N1" s="116" t="s">
+        <v>886</v>
+      </c>
+      <c r="O1" s="117" t="s">
+        <v>887</v>
+      </c>
+      <c r="P1" s="100" t="s">
+        <v>888</v>
+      </c>
+      <c r="Q1" s="100" t="s">
         <v>889</v>
       </c>
-      <c r="O1" s="114" t="s">
+      <c r="R1" s="100" t="s">
         <v>890</v>
       </c>
-      <c r="P1" s="97" t="s">
+      <c r="S1" s="100" t="s">
+        <v>884</v>
+      </c>
+      <c r="T1" s="100" t="s">
+        <v>885</v>
+      </c>
+      <c r="U1" s="100" t="s">
         <v>891</v>
       </c>
-      <c r="Q1" s="97" t="s">
+      <c r="V1" s="100" t="s">
         <v>892</v>
       </c>
-      <c r="R1" s="97" t="s">
-        <v>893</v>
-      </c>
-      <c r="S1" s="97" t="s">
-        <v>887</v>
-      </c>
-      <c r="T1" s="97" t="s">
-        <v>888</v>
-      </c>
-      <c r="U1" s="97" t="s">
-        <v>894</v>
-      </c>
-      <c r="V1" s="97" t="s">
-        <v>895</v>
-      </c>
     </row>
     <row r="2" spans="1:22" s="32" customFormat="1" ht="18.899999999999999" thickTop="1" thickBot="1">
-      <c r="A2" s="112"/>
-      <c r="B2" s="110"/>
-      <c r="C2" s="110"/>
-      <c r="D2" s="101"/>
-      <c r="E2" s="99"/>
+      <c r="A2" s="115"/>
+      <c r="B2" s="113"/>
+      <c r="C2" s="113"/>
+      <c r="D2" s="104"/>
+      <c r="E2" s="102"/>
       <c r="F2" s="72" t="s">
         <v>4</v>
       </c>
@@ -29208,22 +28578,22 @@
         <v>7</v>
       </c>
       <c r="J2" s="76" t="s">
-        <v>856</v>
+        <v>853</v>
       </c>
       <c r="K2" s="77" t="s">
-        <v>860</v>
-      </c>
-      <c r="L2" s="108"/>
-      <c r="M2" s="108"/>
-      <c r="N2" s="113"/>
-      <c r="O2" s="114"/>
-      <c r="P2" s="97"/>
-      <c r="Q2" s="97"/>
-      <c r="R2" s="97"/>
-      <c r="S2" s="97"/>
-      <c r="T2" s="97"/>
-      <c r="U2" s="97"/>
-      <c r="V2" s="97"/>
+        <v>857</v>
+      </c>
+      <c r="L2" s="111"/>
+      <c r="M2" s="111"/>
+      <c r="N2" s="116"/>
+      <c r="O2" s="117"/>
+      <c r="P2" s="100"/>
+      <c r="Q2" s="100"/>
+      <c r="R2" s="100"/>
+      <c r="S2" s="100"/>
+      <c r="T2" s="100"/>
+      <c r="U2" s="100"/>
+      <c r="V2" s="100"/>
     </row>
     <row r="3" spans="1:22" ht="62.4">
       <c r="A3" s="42">
@@ -29403,7 +28773,7 @@
       </c>
       <c r="J5" s="47"/>
       <c r="K5" s="67" t="s">
-        <v>747</v>
+        <v>745</v>
       </c>
       <c r="L5" s="60" t="b">
         <v>1</v>
@@ -29652,7 +29022,7 @@
         <v>2</v>
       </c>
       <c r="K8" s="67" t="s">
-        <v>812</v>
+        <v>809</v>
       </c>
       <c r="L8" s="39" t="b">
         <v>0</v>
@@ -29839,7 +29209,7 @@
       </c>
       <c r="G10" s="46"/>
       <c r="K10" s="67" t="s">
-        <v>824</v>
+        <v>821</v>
       </c>
       <c r="L10" s="39" t="b">
         <v>0</v>
@@ -47177,13 +46547,13 @@
         <v>9</v>
       </c>
       <c r="D1" s="55" t="s">
-        <v>884</v>
+        <v>881</v>
       </c>
       <c r="E1" s="55" t="s">
-        <v>885</v>
+        <v>882</v>
       </c>
       <c r="F1" s="55" t="s">
-        <v>886</v>
+        <v>883</v>
       </c>
     </row>
     <row r="2" spans="1:7">
@@ -47191,10 +46561,10 @@
         <v>2</v>
       </c>
       <c r="B2" s="21" t="s">
-        <v>851</v>
+        <v>848</v>
       </c>
       <c r="C2" s="27" t="s">
-        <v>752</v>
+        <v>750</v>
       </c>
       <c r="D2" s="56" t="str">
         <f t="shared" ref="D2:D4" si="0">CONCATENATE("[",B2,"](",C2,")")</f>
@@ -47218,10 +46588,10 @@
         <v>2</v>
       </c>
       <c r="B3" s="21" t="s">
-        <v>852</v>
+        <v>849</v>
       </c>
       <c r="C3" s="28" t="s">
-        <v>753</v>
+        <v>751</v>
       </c>
       <c r="D3" s="56" t="str">
         <f t="shared" si="0"/>
@@ -47245,10 +46615,10 @@
         <v>2</v>
       </c>
       <c r="B4" s="21" t="s">
-        <v>754</v>
+        <v>752</v>
       </c>
       <c r="C4" s="28" t="s">
-        <v>757</v>
+        <v>755</v>
       </c>
       <c r="D4" s="56" t="str">
         <f t="shared" si="0"/>
@@ -47272,10 +46642,10 @@
         <v>2</v>
       </c>
       <c r="B5" s="21" t="s">
-        <v>755</v>
+        <v>753</v>
       </c>
       <c r="C5" s="28" t="s">
-        <v>758</v>
+        <v>756</v>
       </c>
       <c r="D5" s="56" t="str">
         <f>CONCATENATE("[",B5,"](",C5,")")</f>
@@ -47295,10 +46665,10 @@
         <v>2</v>
       </c>
       <c r="B6" s="21" t="s">
-        <v>756</v>
+        <v>754</v>
       </c>
       <c r="C6" s="28" t="s">
-        <v>759</v>
+        <v>757</v>
       </c>
       <c r="D6" s="56" t="str">
         <f t="shared" ref="D6:D27" si="3">CONCATENATE("[",B6,"](",C6,")")</f>
@@ -47318,10 +46688,10 @@
         <v>4</v>
       </c>
       <c r="B7" s="35" t="s">
-        <v>853</v>
+        <v>850</v>
       </c>
       <c r="C7" s="36" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="D7" s="56" t="str">
         <f t="shared" si="3"/>
@@ -47341,10 +46711,10 @@
         <v>6</v>
       </c>
       <c r="B8" s="35" t="s">
-        <v>854</v>
+        <v>851</v>
       </c>
       <c r="C8" s="36" t="s">
-        <v>761</v>
+        <v>759</v>
       </c>
       <c r="D8" s="56" t="str">
         <f t="shared" si="3"/>
@@ -47364,10 +46734,10 @@
         <v>8</v>
       </c>
       <c r="B9" s="35" t="s">
-        <v>762</v>
+        <v>760</v>
       </c>
       <c r="C9" s="29" t="s">
-        <v>765</v>
+        <v>763</v>
       </c>
       <c r="D9" s="56" t="str">
         <f t="shared" si="3"/>
@@ -47387,10 +46757,10 @@
         <v>8</v>
       </c>
       <c r="B10" s="35" t="s">
-        <v>763</v>
+        <v>761</v>
       </c>
       <c r="C10" s="29" t="s">
-        <v>764</v>
+        <v>762</v>
       </c>
       <c r="D10" s="56" t="str">
         <f t="shared" si="3"/>
@@ -47410,10 +46780,10 @@
         <v>8</v>
       </c>
       <c r="B11" s="35" t="s">
-        <v>766</v>
+        <v>764</v>
       </c>
       <c r="C11" s="29" t="s">
-        <v>767</v>
+        <v>765</v>
       </c>
       <c r="D11" s="56" t="str">
         <f t="shared" si="3"/>
@@ -47433,10 +46803,10 @@
         <v>8</v>
       </c>
       <c r="B12" s="35" t="s">
-        <v>769</v>
+        <v>767</v>
       </c>
       <c r="C12" s="29" t="s">
-        <v>768</v>
+        <v>766</v>
       </c>
       <c r="D12" s="56" t="str">
         <f t="shared" si="3"/>
@@ -47456,10 +46826,10 @@
         <v>8</v>
       </c>
       <c r="B13" s="35" t="s">
-        <v>770</v>
+        <v>768</v>
       </c>
       <c r="C13" s="29" t="s">
-        <v>771</v>
+        <v>769</v>
       </c>
       <c r="D13" s="56" t="str">
         <f t="shared" si="3"/>
@@ -47479,10 +46849,10 @@
         <v>10</v>
       </c>
       <c r="B14" s="9" t="s">
-        <v>773</v>
+        <v>771</v>
       </c>
       <c r="C14" s="37" t="s">
-        <v>772</v>
+        <v>770</v>
       </c>
       <c r="D14" s="56" t="str">
         <f t="shared" si="3"/>
@@ -47502,10 +46872,10 @@
         <v>10</v>
       </c>
       <c r="B15" s="9" t="s">
-        <v>775</v>
+        <v>773</v>
       </c>
       <c r="C15" s="29" t="s">
-        <v>774</v>
+        <v>772</v>
       </c>
       <c r="D15" s="56" t="str">
         <f t="shared" si="3"/>
@@ -47525,10 +46895,10 @@
         <v>12</v>
       </c>
       <c r="B16" s="35" t="s">
-        <v>776</v>
+        <v>774</v>
       </c>
       <c r="C16" s="29" t="s">
-        <v>781</v>
+        <v>779</v>
       </c>
       <c r="D16" s="56" t="str">
         <f t="shared" si="3"/>
@@ -47548,10 +46918,10 @@
         <v>12</v>
       </c>
       <c r="B17" s="35" t="s">
-        <v>777</v>
+        <v>775</v>
       </c>
       <c r="C17" s="29" t="s">
-        <v>782</v>
+        <v>780</v>
       </c>
       <c r="D17" s="56" t="str">
         <f t="shared" si="3"/>
@@ -47571,10 +46941,10 @@
         <v>12</v>
       </c>
       <c r="B18" s="29" t="s">
-        <v>778</v>
+        <v>776</v>
       </c>
       <c r="C18" s="29" t="s">
-        <v>783</v>
+        <v>781</v>
       </c>
       <c r="D18" s="56" t="str">
         <f t="shared" si="3"/>
@@ -47594,10 +46964,10 @@
         <v>12</v>
       </c>
       <c r="B19" s="29" t="s">
-        <v>779</v>
+        <v>777</v>
       </c>
       <c r="C19" s="29" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
       <c r="D19" s="56" t="str">
         <f t="shared" si="3"/>
@@ -47617,10 +46987,10 @@
         <v>12</v>
       </c>
       <c r="B20" s="9" t="s">
-        <v>780</v>
+        <v>778</v>
       </c>
       <c r="C20" s="29" t="s">
-        <v>785</v>
+        <v>783</v>
       </c>
       <c r="D20" s="56" t="str">
         <f t="shared" si="3"/>
@@ -47640,10 +47010,10 @@
         <v>20</v>
       </c>
       <c r="B21" s="9" t="s">
-        <v>793</v>
+        <v>791</v>
       </c>
       <c r="C21" s="29" t="s">
-        <v>786</v>
+        <v>784</v>
       </c>
       <c r="D21" s="56" t="str">
         <f t="shared" si="3"/>
@@ -47663,10 +47033,10 @@
         <v>20</v>
       </c>
       <c r="B22" s="29" t="s">
-        <v>792</v>
+        <v>790</v>
       </c>
       <c r="C22" s="29" t="s">
-        <v>787</v>
+        <v>785</v>
       </c>
       <c r="D22" s="56" t="str">
         <f t="shared" si="3"/>
@@ -47686,10 +47056,10 @@
         <v>20</v>
       </c>
       <c r="B23" s="29" t="s">
-        <v>791</v>
+        <v>789</v>
       </c>
       <c r="C23" s="29" t="s">
-        <v>788</v>
+        <v>786</v>
       </c>
       <c r="D23" s="56" t="str">
         <f t="shared" si="3"/>
@@ -47709,10 +47079,10 @@
         <v>20</v>
       </c>
       <c r="B24" s="9" t="s">
-        <v>790</v>
+        <v>788</v>
       </c>
       <c r="C24" s="29" t="s">
-        <v>789</v>
+        <v>787</v>
       </c>
       <c r="D24" s="56" t="str">
         <f t="shared" si="3"/>
@@ -47732,10 +47102,10 @@
         <v>23</v>
       </c>
       <c r="B25" s="29" t="s">
-        <v>797</v>
+        <v>795</v>
       </c>
       <c r="C25" s="29" t="s">
-        <v>796</v>
+        <v>794</v>
       </c>
       <c r="D25" s="56" t="str">
         <f t="shared" si="3"/>
@@ -47755,10 +47125,10 @@
         <v>23</v>
       </c>
       <c r="B26" s="29" t="s">
-        <v>798</v>
+        <v>796</v>
       </c>
       <c r="C26" s="29" t="s">
-        <v>795</v>
+        <v>793</v>
       </c>
       <c r="D26" s="56" t="str">
         <f t="shared" si="3"/>
@@ -47778,10 +47148,10 @@
         <v>23</v>
       </c>
       <c r="B27" s="29" t="s">
-        <v>799</v>
+        <v>797</v>
       </c>
       <c r="C27" s="29" t="s">
-        <v>794</v>
+        <v>792</v>
       </c>
       <c r="D27" s="56" t="str">
         <f t="shared" si="3"/>
@@ -47809,11 +47179,11 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:I37"/>
+  <dimension ref="A1:L35"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C23" sqref="C23"/>
+      <selection pane="bottomLeft" activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6"/>
@@ -47822,14 +47192,17 @@
     <col min="2" max="2" width="36" customWidth="1"/>
     <col min="3" max="3" width="30.3984375" style="29" customWidth="1"/>
     <col min="4" max="4" width="36" customWidth="1"/>
-    <col min="5" max="5" width="17.046875" style="56" hidden="1" customWidth="1"/>
-    <col min="6" max="6" width="27.25" style="56" hidden="1" customWidth="1"/>
-    <col min="7" max="7" width="30.84765625" style="56" hidden="1" customWidth="1"/>
-    <col min="8" max="8" width="13.1484375" style="56" hidden="1" customWidth="1"/>
-    <col min="9" max="9" width="22.796875" style="56" hidden="1" customWidth="1"/>
+    <col min="5" max="5" width="17.046875" style="56" customWidth="1"/>
+    <col min="6" max="6" width="27.25" style="56" customWidth="1"/>
+    <col min="7" max="7" width="30.84765625" style="56" customWidth="1"/>
+    <col min="8" max="8" width="13.1484375" style="56" customWidth="1"/>
+    <col min="9" max="9" width="17.046875" style="56" customWidth="1"/>
+    <col min="10" max="10" width="15.8984375" customWidth="1"/>
+    <col min="11" max="11" width="25.69921875" style="56" customWidth="1"/>
+    <col min="12" max="12" width="28.19921875" style="56" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="32" customFormat="1" ht="18.3">
+    <row r="1" spans="1:12" s="32" customFormat="1" ht="18.3">
       <c r="A1" s="33" t="s">
         <v>731</v>
       </c>
@@ -47837,28 +47210,35 @@
         <v>732</v>
       </c>
       <c r="C1" s="32" t="s">
-        <v>866</v>
+        <v>863</v>
       </c>
       <c r="D1" s="32" t="s">
-        <v>867</v>
+        <v>864</v>
       </c>
       <c r="E1" s="55" t="s">
+        <v>881</v>
+      </c>
+      <c r="F1" s="55" t="s">
+        <v>882</v>
+      </c>
+      <c r="G1" s="55" t="s">
+        <v>883</v>
+      </c>
+      <c r="H1" s="55" t="s">
         <v>884</v>
       </c>
-      <c r="F1" s="55" t="s">
-        <v>885</v>
-      </c>
-      <c r="G1" s="55" t="s">
-        <v>886</v>
-      </c>
-      <c r="H1" s="55" t="s">
-        <v>887</v>
-      </c>
-      <c r="I1" s="55" t="s">
-        <v>888</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9">
+      <c r="I1" s="55"/>
+      <c r="J1" s="90" t="s">
+        <v>903</v>
+      </c>
+      <c r="K1" s="90" t="s">
+        <v>904</v>
+      </c>
+      <c r="L1" s="90" t="s">
+        <v>905</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12">
       <c r="A2" s="34">
         <v>1</v>
       </c>
@@ -47866,7 +47246,7 @@
         <v>723</v>
       </c>
       <c r="C2" s="21" t="s">
-        <v>873</v>
+        <v>870</v>
       </c>
       <c r="D2" s="27" t="s">
         <v>726</v>
@@ -47894,13 +47274,25 @@
       <c r="I2" s="56" t="str">
         <f>I1&amp;"
 "&amp;H2</f>
-        <v>TOC entries (grouped)
+        <v xml:space="preserve">
   - title: What is Jupyter?
     url: /notebooks/01-what-is-jupyter
     not_numbered: true</v>
       </c>
-    </row>
-    <row r="3" spans="1:9">
+      <c r="J2" s="56" t="str">
+        <f>IF(ISBLANK(C2),"",CONCATENATE("[",B2,"](",Configuration!B$29,Configuration!B$28,"/notebooks/",C2,".html)"))</f>
+        <v>[What is Jupyter?](https://rpi-data.github.io/course-intro-ml-app/notebooks/01-what-is-jupyter.html)</v>
+      </c>
+      <c r="K2" s="56" t="str">
+        <f>IF(A2=A1,K1&amp;"&lt;br&gt;"&amp;J2,J2)</f>
+        <v>[What is Jupyter?](https://rpi-data.github.io/course-intro-ml-app/notebooks/01-what-is-jupyter.html)</v>
+      </c>
+      <c r="L2" s="56" t="str">
+        <f>IF(A2&lt;&gt;A3,K2,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="3" spans="1:12">
       <c r="A3" s="34">
         <v>1</v>
       </c>
@@ -47908,7 +47300,7 @@
         <v>724</v>
       </c>
       <c r="C3" s="21" t="s">
-        <v>876</v>
+        <v>873</v>
       </c>
       <c r="D3" s="28" t="s">
         <v>727</v>
@@ -47918,7 +47310,7 @@
         <v>Notebook Basics - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/01-overview/01-notebook-basics/02-notebook-basics.ipynb)</v>
       </c>
       <c r="F3" s="56" t="str">
-        <f t="shared" ref="F3:F11" si="1">IF(A3=A2,F2&amp;"&lt;br&gt;"&amp;E3,E3)</f>
+        <f t="shared" ref="F3:F33" si="1">IF(A3=A2,F2&amp;"&lt;br&gt;"&amp;E3,E3)</f>
         <v>What is Jupyter? - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/01-overview/01-notebook-basics/01-what-is-jupyter.ipynb#scrollTo=mdFTkIqGwgOJ)&lt;br&gt;Notebook Basics - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/01-overview/01-notebook-basics/02-notebook-basics.ipynb)</v>
       </c>
       <c r="G3" s="56" t="str">
@@ -47926,7 +47318,7 @@
         <v/>
       </c>
       <c r="H3" s="56" t="str">
-        <f t="shared" ref="H3:H35" si="3">IF(ISBLANK(C3),"",CONCATENATE("  - title: ",B3,"
+        <f t="shared" ref="H3:H33" si="3">IF(ISBLANK(C3),"",CONCATENATE("  - title: ",B3,"
     url: /notebooks/",C3,"
     not_numbered: true"))</f>
         <v xml:space="preserve">  - title: Notebook Basics
@@ -47934,9 +47326,9 @@
     not_numbered: true</v>
       </c>
       <c r="I3" s="56" t="str">
-        <f t="shared" ref="I3:I13" si="4">I2&amp;"
+        <f t="shared" ref="I3:I33" si="4">I2&amp;"
 "&amp;H3</f>
-        <v>TOC entries (grouped)
+        <v xml:space="preserve">
   - title: What is Jupyter?
     url: /notebooks/01-what-is-jupyter
     not_numbered: true
@@ -47944,8 +47336,20 @@
     url: /notebooks/02-notebook-basics
     not_numbered: true</v>
       </c>
-    </row>
-    <row r="4" spans="1:9">
+      <c r="J3" s="56" t="str">
+        <f>IF(ISBLANK(C3),"",CONCATENATE("[",B3,"](",Configuration!B$29,Configuration!B$28,"/notebooks/",C3,".html)"))</f>
+        <v>[Notebook Basics](https://rpi-data.github.io/course-intro-ml-app/notebooks/02-notebook-basics.html)</v>
+      </c>
+      <c r="K3" s="56" t="str">
+        <f t="shared" ref="K3:K33" si="5">IF(A3=A2,K2&amp;"&lt;br&gt;"&amp;J3,J3)</f>
+        <v>[What is Jupyter?](https://rpi-data.github.io/course-intro-ml-app/notebooks/01-what-is-jupyter.html)&lt;br&gt;[Notebook Basics](https://rpi-data.github.io/course-intro-ml-app/notebooks/02-notebook-basics.html)</v>
+      </c>
+      <c r="L3" s="56" t="str">
+        <f t="shared" ref="L3:L33" si="6">IF(A3&lt;&gt;A4,K3,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="4" spans="1:12">
       <c r="A4" s="34">
         <v>1</v>
       </c>
@@ -47953,7 +47357,7 @@
         <v>725</v>
       </c>
       <c r="C4" s="21" t="s">
-        <v>874</v>
+        <v>871</v>
       </c>
       <c r="D4" s="28" t="s">
         <v>728</v>
@@ -47978,7 +47382,7 @@
       </c>
       <c r="I4" s="56" t="str">
         <f t="shared" si="4"/>
-        <v>TOC entries (grouped)
+        <v xml:space="preserve">
   - title: What is Jupyter?
     url: /notebooks/01-what-is-jupyter
     not_numbered: true
@@ -47989,8 +47393,20 @@
     url: /notebooks/03-running-code
     not_numbered: true</v>
       </c>
-    </row>
-    <row r="5" spans="1:9">
+      <c r="J4" s="56" t="str">
+        <f>IF(ISBLANK(C4),"",CONCATENATE("[",B4,"](",Configuration!B$29,Configuration!B$28,"/notebooks/",C4,".html)"))</f>
+        <v>[Running Code](https://rpi-data.github.io/course-intro-ml-app/notebooks/03-running-code.html)</v>
+      </c>
+      <c r="K4" s="56" t="str">
+        <f t="shared" si="5"/>
+        <v>[What is Jupyter?](https://rpi-data.github.io/course-intro-ml-app/notebooks/01-what-is-jupyter.html)&lt;br&gt;[Notebook Basics](https://rpi-data.github.io/course-intro-ml-app/notebooks/02-notebook-basics.html)&lt;br&gt;[Running Code](https://rpi-data.github.io/course-intro-ml-app/notebooks/03-running-code.html)</v>
+      </c>
+      <c r="L4" s="56" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+    </row>
+    <row r="5" spans="1:12">
       <c r="A5" s="34">
         <v>1</v>
       </c>
@@ -47998,7 +47414,7 @@
         <v>13</v>
       </c>
       <c r="C5" s="21" t="s">
-        <v>875</v>
+        <v>872</v>
       </c>
       <c r="D5" s="28" t="s">
         <v>729</v>
@@ -48012,7 +47428,7 @@
         <v>What is Jupyter? - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/01-overview/01-notebook-basics/01-what-is-jupyter.ipynb#scrollTo=mdFTkIqGwgOJ)&lt;br&gt;Notebook Basics - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/01-overview/01-notebook-basics/02-notebook-basics.ipynb)&lt;br&gt;Running Code - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/01-overview/01-notebook-basics/03-running-code.ipynb)&lt;br&gt;Markdown - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/01-overview/01-notebook-basics/04-markdown.ipynb)</v>
       </c>
       <c r="G5" s="56" t="str">
-        <f t="shared" ref="G5:G34" si="5">IF(A5&lt;&gt;A6,F5,"")</f>
+        <f t="shared" ref="G5:G33" si="7">IF(A5&lt;&gt;A6,F5,"")</f>
         <v>What is Jupyter? - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/01-overview/01-notebook-basics/01-what-is-jupyter.ipynb#scrollTo=mdFTkIqGwgOJ)&lt;br&gt;Notebook Basics - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/01-overview/01-notebook-basics/02-notebook-basics.ipynb)&lt;br&gt;Running Code - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/01-overview/01-notebook-basics/03-running-code.ipynb)&lt;br&gt;Markdown - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/01-overview/01-notebook-basics/04-markdown.ipynb)</v>
       </c>
       <c r="H5" s="56" t="str">
@@ -48023,7 +47439,7 @@
       </c>
       <c r="I5" s="56" t="str">
         <f t="shared" si="4"/>
-        <v>TOC entries (grouped)
+        <v xml:space="preserve">
   - title: What is Jupyter?
     url: /notebooks/01-what-is-jupyter
     not_numbered: true
@@ -48037,8 +47453,20 @@
     url: /notebooks/04-markdown
     not_numbered: true</v>
       </c>
-    </row>
-    <row r="6" spans="1:9">
+      <c r="J5" s="56" t="str">
+        <f>IF(ISBLANK(C5),"",CONCATENATE("[",B5,"](",Configuration!B$29,Configuration!B$28,"/notebooks/",C5,".html)"))</f>
+        <v>[Markdown](https://rpi-data.github.io/course-intro-ml-app/notebooks/04-markdown.html)</v>
+      </c>
+      <c r="K5" s="56" t="str">
+        <f t="shared" si="5"/>
+        <v>[What is Jupyter?](https://rpi-data.github.io/course-intro-ml-app/notebooks/01-what-is-jupyter.html)&lt;br&gt;[Notebook Basics](https://rpi-data.github.io/course-intro-ml-app/notebooks/02-notebook-basics.html)&lt;br&gt;[Running Code](https://rpi-data.github.io/course-intro-ml-app/notebooks/03-running-code.html)&lt;br&gt;[Markdown](https://rpi-data.github.io/course-intro-ml-app/notebooks/04-markdown.html)</v>
+      </c>
+      <c r="L5" s="56" t="str">
+        <f t="shared" si="6"/>
+        <v>[What is Jupyter?](https://rpi-data.github.io/course-intro-ml-app/notebooks/01-what-is-jupyter.html)&lt;br&gt;[Notebook Basics](https://rpi-data.github.io/course-intro-ml-app/notebooks/02-notebook-basics.html)&lt;br&gt;[Running Code](https://rpi-data.github.io/course-intro-ml-app/notebooks/03-running-code.html)&lt;br&gt;[Markdown](https://rpi-data.github.io/course-intro-ml-app/notebooks/04-markdown.html)</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12">
       <c r="A6" s="34">
         <v>2</v>
       </c>
@@ -48046,13 +47474,13 @@
         <v>738</v>
       </c>
       <c r="C6" s="21" t="s">
-        <v>877</v>
+        <v>874</v>
       </c>
       <c r="D6" t="s">
-        <v>743</v>
+        <v>742</v>
       </c>
       <c r="E6" s="56" t="str">
-        <f t="shared" ref="E6:E35" si="6">CONCATENATE(B6," - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](",D6,")")</f>
+        <f t="shared" ref="E6:E33" si="8">CONCATENATE(B6," - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](",D6,")")</f>
         <v>Python Overview - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/02-intro-python/01-intro-python-overview.ipynb)</v>
       </c>
       <c r="F6" s="56" t="str">
@@ -48060,7 +47488,7 @@
         <v>Python Overview - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/02-intro-python/01-intro-python-overview.ipynb)</v>
       </c>
       <c r="G6" s="56" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="H6" s="56" t="str">
@@ -48071,7 +47499,7 @@
       </c>
       <c r="I6" s="56" t="str">
         <f t="shared" si="4"/>
-        <v>TOC entries (grouped)
+        <v xml:space="preserve">
   - title: What is Jupyter?
     url: /notebooks/01-what-is-jupyter
     not_numbered: true
@@ -48088,8 +47516,20 @@
     url: /notebooks/05-intro-python-overview
     not_numbered: true</v>
       </c>
-    </row>
-    <row r="7" spans="1:9">
+      <c r="J6" s="56" t="str">
+        <f>IF(ISBLANK(C6),"",CONCATENATE("[",B6,"](",Configuration!B$29,Configuration!B$28,"/notebooks/",C6,".html)"))</f>
+        <v>[Python Overview](https://rpi-data.github.io/course-intro-ml-app/notebooks/05-intro-python-overview.html)</v>
+      </c>
+      <c r="K6" s="56" t="str">
+        <f t="shared" si="5"/>
+        <v>[Python Overview](https://rpi-data.github.io/course-intro-ml-app/notebooks/05-intro-python-overview.html)</v>
+      </c>
+      <c r="L6" s="56" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+    </row>
+    <row r="7" spans="1:12">
       <c r="A7" s="34">
         <v>2</v>
       </c>
@@ -48097,13 +47537,13 @@
         <v>739</v>
       </c>
       <c r="C7" s="35" t="s">
-        <v>878</v>
+        <v>875</v>
       </c>
       <c r="D7" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="E7" s="56" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>Basic Data Structures - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/02-intro-python/02-intro-python-datastructures.ipynbhttps://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/02-intro-python/03-intro-python-numpy.ipynb)</v>
       </c>
       <c r="F7" s="56" t="str">
@@ -48111,7 +47551,7 @@
         <v>Python Overview - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/02-intro-python/01-intro-python-overview.ipynb)&lt;br&gt;Basic Data Structures - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/02-intro-python/02-intro-python-datastructures.ipynbhttps://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/02-intro-python/03-intro-python-numpy.ipynb)</v>
       </c>
       <c r="G7" s="56" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="H7" s="56" t="str">
@@ -48122,7 +47562,7 @@
       </c>
       <c r="I7" s="56" t="str">
         <f t="shared" si="4"/>
-        <v>TOC entries (grouped)
+        <v xml:space="preserve">
   - title: What is Jupyter?
     url: /notebooks/01-what-is-jupyter
     not_numbered: true
@@ -48142,8 +47582,20 @@
     url: /notebooks/06-intro-python-datastructures
     not_numbered: true</v>
       </c>
-    </row>
-    <row r="8" spans="1:9">
+      <c r="J7" s="56" t="str">
+        <f>IF(ISBLANK(C7),"",CONCATENATE("[",B7,"](",Configuration!B$29,Configuration!B$28,"/notebooks/",C7,".html)"))</f>
+        <v>[Basic Data Structures](https://rpi-data.github.io/course-intro-ml-app/notebooks/06-intro-python-datastructures.html)</v>
+      </c>
+      <c r="K7" s="56" t="str">
+        <f t="shared" si="5"/>
+        <v>[Python Overview](https://rpi-data.github.io/course-intro-ml-app/notebooks/05-intro-python-overview.html)&lt;br&gt;[Basic Data Structures](https://rpi-data.github.io/course-intro-ml-app/notebooks/06-intro-python-datastructures.html)</v>
+      </c>
+      <c r="L7" s="56" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+    </row>
+    <row r="8" spans="1:12">
       <c r="A8" s="34">
         <v>2</v>
       </c>
@@ -48151,13 +47603,13 @@
         <v>740</v>
       </c>
       <c r="C8" s="35" t="s">
-        <v>879</v>
+        <v>876</v>
       </c>
       <c r="D8" t="s">
-        <v>745</v>
+        <v>744</v>
       </c>
       <c r="E8" s="56" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>Numpy - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/02-intro-python/04-intro-python-pandas.ipynb)</v>
       </c>
       <c r="F8" s="56" t="str">
@@ -48165,7 +47617,7 @@
         <v>Python Overview - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/02-intro-python/01-intro-python-overview.ipynb)&lt;br&gt;Basic Data Structures - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/02-intro-python/02-intro-python-datastructures.ipynbhttps://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/02-intro-python/03-intro-python-numpy.ipynb)&lt;br&gt;Numpy - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/02-intro-python/04-intro-python-pandas.ipynb)</v>
       </c>
       <c r="G8" s="56" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="H8" s="56" t="str">
@@ -48176,7 +47628,7 @@
       </c>
       <c r="I8" s="56" t="str">
         <f t="shared" si="4"/>
-        <v>TOC entries (grouped)
+        <v xml:space="preserve">
   - title: What is Jupyter?
     url: /notebooks/01-what-is-jupyter
     not_numbered: true
@@ -48199,8 +47651,20 @@
     url: /notebooks/07-intro-python-numpy
     not_numbered: true</v>
       </c>
-    </row>
-    <row r="9" spans="1:9">
+      <c r="J8" s="56" t="str">
+        <f>IF(ISBLANK(C8),"",CONCATENATE("[",B8,"](",Configuration!B$29,Configuration!B$28,"/notebooks/",C8,".html)"))</f>
+        <v>[Numpy](https://rpi-data.github.io/course-intro-ml-app/notebooks/07-intro-python-numpy.html)</v>
+      </c>
+      <c r="K8" s="56" t="str">
+        <f t="shared" si="5"/>
+        <v>[Python Overview](https://rpi-data.github.io/course-intro-ml-app/notebooks/05-intro-python-overview.html)&lt;br&gt;[Basic Data Structures](https://rpi-data.github.io/course-intro-ml-app/notebooks/06-intro-python-datastructures.html)&lt;br&gt;[Numpy](https://rpi-data.github.io/course-intro-ml-app/notebooks/07-intro-python-numpy.html)</v>
+      </c>
+      <c r="L8" s="56" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+    </row>
+    <row r="9" spans="1:12">
       <c r="A9" s="34">
         <v>2</v>
       </c>
@@ -48208,13 +47672,13 @@
         <v>741</v>
       </c>
       <c r="C9" s="35" t="s">
-        <v>880</v>
+        <v>877</v>
       </c>
       <c r="D9" t="s">
-        <v>745</v>
+        <v>744</v>
       </c>
       <c r="E9" s="56" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>Pandas - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/02-intro-python/04-intro-python-pandas.ipynb)</v>
       </c>
       <c r="F9" s="56" t="str">
@@ -48222,8 +47686,8 @@
         <v>Python Overview - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/02-intro-python/01-intro-python-overview.ipynb)&lt;br&gt;Basic Data Structures - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/02-intro-python/02-intro-python-datastructures.ipynbhttps://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/02-intro-python/03-intro-python-numpy.ipynb)&lt;br&gt;Numpy - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/02-intro-python/04-intro-python-pandas.ipynb)&lt;br&gt;Pandas - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/02-intro-python/04-intro-python-pandas.ipynb)</v>
       </c>
       <c r="G9" s="56" t="str">
-        <f t="shared" si="5"/>
-        <v/>
+        <f t="shared" si="7"/>
+        <v>Python Overview - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/02-intro-python/01-intro-python-overview.ipynb)&lt;br&gt;Basic Data Structures - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/02-intro-python/02-intro-python-datastructures.ipynbhttps://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/02-intro-python/03-intro-python-numpy.ipynb)&lt;br&gt;Numpy - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/02-intro-python/04-intro-python-pandas.ipynb)&lt;br&gt;Pandas - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/02-intro-python/04-intro-python-pandas.ipynb)</v>
       </c>
       <c r="H9" s="56" t="str">
         <f t="shared" si="3"/>
@@ -48233,7 +47697,7 @@
       </c>
       <c r="I9" s="56" t="str">
         <f t="shared" si="4"/>
-        <v>TOC entries (grouped)
+        <v xml:space="preserve">
   - title: What is Jupyter?
     url: /notebooks/01-what-is-jupyter
     not_numbered: true
@@ -48259,28 +47723,39 @@
     url: /notebooks/08-intro-python-pandas
     not_numbered: true</v>
       </c>
-    </row>
-    <row r="10" spans="1:9">
+      <c r="J9" s="56" t="str">
+        <f>IF(ISBLANK(C9),"",CONCATENATE("[",B9,"](",Configuration!B$29,Configuration!B$28,"/notebooks/",C9,".html)"))</f>
+        <v>[Pandas](https://rpi-data.github.io/course-intro-ml-app/notebooks/08-intro-python-pandas.html)</v>
+      </c>
+      <c r="K9" s="56" t="str">
+        <f t="shared" si="5"/>
+        <v>[Python Overview](https://rpi-data.github.io/course-intro-ml-app/notebooks/05-intro-python-overview.html)&lt;br&gt;[Basic Data Structures](https://rpi-data.github.io/course-intro-ml-app/notebooks/06-intro-python-datastructures.html)&lt;br&gt;[Numpy](https://rpi-data.github.io/course-intro-ml-app/notebooks/07-intro-python-numpy.html)&lt;br&gt;[Pandas](https://rpi-data.github.io/course-intro-ml-app/notebooks/08-intro-python-pandas.html)</v>
+      </c>
+      <c r="L9" s="56" t="str">
+        <f t="shared" si="6"/>
+        <v>[Python Overview](https://rpi-data.github.io/course-intro-ml-app/notebooks/05-intro-python-overview.html)&lt;br&gt;[Basic Data Structures](https://rpi-data.github.io/course-intro-ml-app/notebooks/06-intro-python-datastructures.html)&lt;br&gt;[Numpy](https://rpi-data.github.io/course-intro-ml-app/notebooks/07-intro-python-numpy.html)&lt;br&gt;[Pandas](https://rpi-data.github.io/course-intro-ml-app/notebooks/08-intro-python-pandas.html)</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12">
       <c r="A10" s="34">
-        <v>2</v>
-      </c>
-      <c r="B10" s="35" t="s">
-        <v>742</v>
-      </c>
-      <c r="C10" s="35"/>
+        <v>4</v>
+      </c>
+      <c r="B10" t="s">
+        <v>798</v>
+      </c>
       <c r="D10" t="s">
-        <v>746</v>
+        <v>799</v>
       </c>
       <c r="E10" s="56" t="str">
-        <f t="shared" si="6"/>
-        <v>Lab - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/02-intro-python/lab/lab.ipynb)</v>
+        <f t="shared" si="8"/>
+        <v>Conditional-Loops - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/03-python/01-intro-python-conditionals-loops.ipynb)</v>
       </c>
       <c r="F10" s="56" t="str">
         <f t="shared" si="1"/>
-        <v>Python Overview - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/02-intro-python/01-intro-python-overview.ipynb)&lt;br&gt;Basic Data Structures - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/02-intro-python/02-intro-python-datastructures.ipynbhttps://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/02-intro-python/03-intro-python-numpy.ipynb)&lt;br&gt;Numpy - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/02-intro-python/04-intro-python-pandas.ipynb)&lt;br&gt;Pandas - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/02-intro-python/04-intro-python-pandas.ipynb)&lt;br&gt;Lab - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/02-intro-python/lab/lab.ipynb)</v>
+        <v>Conditional-Loops - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/03-python/01-intro-python-conditionals-loops.ipynb)</v>
       </c>
       <c r="G10" s="56" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="H10" s="56" t="str">
@@ -48289,7 +47764,7 @@
       </c>
       <c r="I10" s="56" t="str">
         <f t="shared" si="4"/>
-        <v xml:space="preserve">TOC entries (grouped)
+        <v xml:space="preserve">
   - title: What is Jupyter?
     url: /notebooks/01-what-is-jupyter
     not_numbered: true
@@ -48316,29 +47791,40 @@
     not_numbered: true
 </v>
       </c>
-    </row>
-    <row r="11" spans="1:9">
+      <c r="J10" s="56" t="str">
+        <f>IF(ISBLANK(C10),"",CONCATENATE("[",B10,"](",Configuration!B$29,Configuration!B$28,"/notebooks/",C10,".html)"))</f>
+        <v/>
+      </c>
+      <c r="K10" s="56" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="L10" s="56" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+    </row>
+    <row r="11" spans="1:12">
       <c r="A11" s="34">
-        <v>2</v>
-      </c>
-      <c r="B11" s="35" t="s">
-        <v>809</v>
-      </c>
-      <c r="C11" s="35"/>
+        <v>4</v>
+      </c>
+      <c r="B11" t="s">
+        <v>800</v>
+      </c>
       <c r="D11" t="s">
-        <v>747</v>
+        <v>801</v>
       </c>
       <c r="E11" s="56" t="str">
-        <f t="shared" si="6"/>
-        <v>Assignment 1 - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/02-intro-python/hm-01/hm01.ipynb)</v>
+        <f t="shared" si="8"/>
+        <v>Functions - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/03-python/02-intro-python-functions.ipynb)</v>
       </c>
       <c r="F11" s="56" t="str">
         <f t="shared" si="1"/>
-        <v>Python Overview - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/02-intro-python/01-intro-python-overview.ipynb)&lt;br&gt;Basic Data Structures - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/02-intro-python/02-intro-python-datastructures.ipynbhttps://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/02-intro-python/03-intro-python-numpy.ipynb)&lt;br&gt;Numpy - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/02-intro-python/04-intro-python-pandas.ipynb)&lt;br&gt;Pandas - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/02-intro-python/04-intro-python-pandas.ipynb)&lt;br&gt;Lab - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/02-intro-python/lab/lab.ipynb)&lt;br&gt;Assignment 1 - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/02-intro-python/hm-01/hm01.ipynb)</v>
+        <v>Conditional-Loops - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/03-python/01-intro-python-conditionals-loops.ipynb)&lt;br&gt;Functions - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/03-python/02-intro-python-functions.ipynb)</v>
       </c>
       <c r="G11" s="56" t="str">
-        <f t="shared" si="5"/>
-        <v>Python Overview - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/02-intro-python/01-intro-python-overview.ipynb)&lt;br&gt;Basic Data Structures - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/02-intro-python/02-intro-python-datastructures.ipynbhttps://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/02-intro-python/03-intro-python-numpy.ipynb)&lt;br&gt;Numpy - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/02-intro-python/04-intro-python-pandas.ipynb)&lt;br&gt;Pandas - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/02-intro-python/04-intro-python-pandas.ipynb)&lt;br&gt;Lab - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/02-intro-python/lab/lab.ipynb)&lt;br&gt;Assignment 1 - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/02-intro-python/hm-01/hm01.ipynb)</v>
+        <f t="shared" si="7"/>
+        <v/>
       </c>
       <c r="H11" s="56" t="str">
         <f t="shared" si="3"/>
@@ -48346,7 +47832,7 @@
       </c>
       <c r="I11" s="56" t="str">
         <f t="shared" si="4"/>
-        <v xml:space="preserve">TOC entries (grouped)
+        <v xml:space="preserve">
   - title: What is Jupyter?
     url: /notebooks/01-what-is-jupyter
     not_numbered: true
@@ -48373,27 +47859,39 @@
     not_numbered: true
 </v>
       </c>
-    </row>
-    <row r="12" spans="1:9">
+      <c r="J11" s="56" t="str">
+        <f>IF(ISBLANK(C11),"",CONCATENATE("[",B11,"](",Configuration!B$29,Configuration!B$28,"/notebooks/",C11,".html)"))</f>
+        <v/>
+      </c>
+      <c r="K11" s="56" t="str">
+        <f t="shared" si="5"/>
+        <v>&lt;br&gt;</v>
+      </c>
+      <c r="L11" s="56" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+    </row>
+    <row r="12" spans="1:12">
       <c r="A12" s="34">
         <v>4</v>
       </c>
       <c r="B12" t="s">
-        <v>800</v>
+        <v>802</v>
       </c>
       <c r="D12" t="s">
-        <v>801</v>
+        <v>803</v>
       </c>
       <c r="E12" s="56" t="str">
-        <f t="shared" si="6"/>
-        <v>Conditional-Loops - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/03-python/01-intro-python-conditionals-loops.ipynb)</v>
+        <f t="shared" si="8"/>
+        <v>Null Values - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/03-python/03-intro-python-null-values.ipynb)</v>
       </c>
       <c r="F12" s="56" t="str">
-        <f t="shared" ref="F12:F35" si="7">IF(A12=A11,F11&amp;"&lt;br&gt;"&amp;E12,E12)</f>
-        <v>Conditional-Loops - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/03-python/01-intro-python-conditionals-loops.ipynb)</v>
+        <f t="shared" si="1"/>
+        <v>Conditional-Loops - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/03-python/01-intro-python-conditionals-loops.ipynb)&lt;br&gt;Functions - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/03-python/02-intro-python-functions.ipynb)&lt;br&gt;Null Values - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/03-python/03-intro-python-null-values.ipynb)</v>
       </c>
       <c r="G12" s="56" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="H12" s="56" t="str">
@@ -48402,7 +47900,7 @@
       </c>
       <c r="I12" s="56" t="str">
         <f t="shared" si="4"/>
-        <v xml:space="preserve">TOC entries (grouped)
+        <v xml:space="preserve">
   - title: What is Jupyter?
     url: /notebooks/01-what-is-jupyter
     not_numbered: true
@@ -48429,27 +47927,39 @@
     not_numbered: true
 </v>
       </c>
-    </row>
-    <row r="13" spans="1:9">
+      <c r="J12" s="56" t="str">
+        <f>IF(ISBLANK(C12),"",CONCATENATE("[",B12,"](",Configuration!B$29,Configuration!B$28,"/notebooks/",C12,".html)"))</f>
+        <v/>
+      </c>
+      <c r="K12" s="56" t="str">
+        <f t="shared" si="5"/>
+        <v>&lt;br&gt;&lt;br&gt;</v>
+      </c>
+      <c r="L12" s="56" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+    </row>
+    <row r="13" spans="1:12">
       <c r="A13" s="34">
         <v>4</v>
       </c>
       <c r="B13" t="s">
-        <v>802</v>
+        <v>804</v>
       </c>
       <c r="D13" t="s">
-        <v>803</v>
+        <v>807</v>
       </c>
       <c r="E13" s="56" t="str">
-        <f t="shared" si="6"/>
-        <v>Functions - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/03-python/02-intro-python-functions.ipynb)</v>
+        <f t="shared" si="8"/>
+        <v>Groupby - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/03-python/04-intro-python-groupby.ipynb)</v>
       </c>
       <c r="F13" s="56" t="str">
+        <f t="shared" si="1"/>
+        <v>Conditional-Loops - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/03-python/01-intro-python-conditionals-loops.ipynb)&lt;br&gt;Functions - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/03-python/02-intro-python-functions.ipynb)&lt;br&gt;Null Values - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/03-python/03-intro-python-null-values.ipynb)&lt;br&gt;Groupby - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/03-python/04-intro-python-groupby.ipynb)</v>
+      </c>
+      <c r="G13" s="56" t="str">
         <f t="shared" si="7"/>
-        <v>Conditional-Loops - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/03-python/01-intro-python-conditionals-loops.ipynb)&lt;br&gt;Functions - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/03-python/02-intro-python-functions.ipynb)</v>
-      </c>
-      <c r="G13" s="56" t="str">
-        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="H13" s="56" t="str">
@@ -48458,7 +47968,7 @@
       </c>
       <c r="I13" s="56" t="str">
         <f t="shared" si="4"/>
-        <v xml:space="preserve">TOC entries (grouped)
+        <v xml:space="preserve">
   - title: What is Jupyter?
     url: /notebooks/01-what-is-jupyter
     not_numbered: true
@@ -48485,27 +47995,39 @@
     not_numbered: true
 </v>
       </c>
-    </row>
-    <row r="14" spans="1:9">
+      <c r="J13" s="56" t="str">
+        <f>IF(ISBLANK(C13),"",CONCATENATE("[",B13,"](",Configuration!B$29,Configuration!B$28,"/notebooks/",C13,".html)"))</f>
+        <v/>
+      </c>
+      <c r="K13" s="56" t="str">
+        <f t="shared" si="5"/>
+        <v>&lt;br&gt;&lt;br&gt;&lt;br&gt;</v>
+      </c>
+      <c r="L13" s="56" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+    </row>
+    <row r="14" spans="1:12">
       <c r="A14" s="34">
         <v>4</v>
       </c>
       <c r="B14" t="s">
-        <v>804</v>
+        <v>805</v>
       </c>
       <c r="D14" t="s">
-        <v>805</v>
+        <v>808</v>
       </c>
       <c r="E14" s="56" t="str">
-        <f t="shared" si="6"/>
-        <v>Null Values - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/03-python/03-intro-python-null-values.ipynb)</v>
+        <f t="shared" si="8"/>
+        <v>Kaggle Baseline - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/03-python/05-intro-kaggle-baseline.ipynb)</v>
       </c>
       <c r="F14" s="56" t="str">
+        <f t="shared" si="1"/>
+        <v>Conditional-Loops - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/03-python/01-intro-python-conditionals-loops.ipynb)&lt;br&gt;Functions - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/03-python/02-intro-python-functions.ipynb)&lt;br&gt;Null Values - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/03-python/03-intro-python-null-values.ipynb)&lt;br&gt;Groupby - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/03-python/04-intro-python-groupby.ipynb)&lt;br&gt;Kaggle Baseline - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/03-python/05-intro-kaggle-baseline.ipynb)</v>
+      </c>
+      <c r="G14" s="56" t="str">
         <f t="shared" si="7"/>
-        <v>Conditional-Loops - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/03-python/01-intro-python-conditionals-loops.ipynb)&lt;br&gt;Functions - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/03-python/02-intro-python-functions.ipynb)&lt;br&gt;Null Values - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/03-python/03-intro-python-null-values.ipynb)</v>
-      </c>
-      <c r="G14" s="56" t="str">
-        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="H14" s="56" t="str">
@@ -48513,9 +48035,8 @@
         <v/>
       </c>
       <c r="I14" s="56" t="str">
-        <f>I13&amp;"
-"&amp;H14</f>
-        <v xml:space="preserve">TOC entries (grouped)
+        <f t="shared" si="4"/>
+        <v xml:space="preserve">
   - title: What is Jupyter?
     url: /notebooks/01-what-is-jupyter
     not_numbered: true
@@ -48542,8 +48063,20 @@
     not_numbered: true
 </v>
       </c>
-    </row>
-    <row r="15" spans="1:9">
+      <c r="J14" s="56" t="str">
+        <f>IF(ISBLANK(C14),"",CONCATENATE("[",B14,"](",Configuration!B$29,Configuration!B$28,"/notebooks/",C14,".html)"))</f>
+        <v/>
+      </c>
+      <c r="K14" s="56" t="str">
+        <f t="shared" si="5"/>
+        <v>&lt;br&gt;&lt;br&gt;&lt;br&gt;&lt;br&gt;</v>
+      </c>
+      <c r="L14" s="56" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+    </row>
+    <row r="15" spans="1:12">
       <c r="A15" s="34">
         <v>4</v>
       </c>
@@ -48551,28 +48084,27 @@
         <v>806</v>
       </c>
       <c r="D15" t="s">
-        <v>810</v>
+        <v>809</v>
       </c>
       <c r="E15" s="56" t="str">
-        <f t="shared" si="6"/>
-        <v>Groupby - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/03-python/04-intro-python-groupby.ipynb)</v>
+        <f t="shared" si="8"/>
+        <v>Assignment 2 - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/03-python/hm-02/hm02.ipynb)</v>
       </c>
       <c r="F15" s="56" t="str">
+        <f t="shared" si="1"/>
+        <v>Conditional-Loops - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/03-python/01-intro-python-conditionals-loops.ipynb)&lt;br&gt;Functions - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/03-python/02-intro-python-functions.ipynb)&lt;br&gt;Null Values - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/03-python/03-intro-python-null-values.ipynb)&lt;br&gt;Groupby - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/03-python/04-intro-python-groupby.ipynb)&lt;br&gt;Kaggle Baseline - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/03-python/05-intro-kaggle-baseline.ipynb)&lt;br&gt;Assignment 2 - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/03-python/hm-02/hm02.ipynb)</v>
+      </c>
+      <c r="G15" s="56" t="str">
         <f t="shared" si="7"/>
-        <v>Conditional-Loops - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/03-python/01-intro-python-conditionals-loops.ipynb)&lt;br&gt;Functions - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/03-python/02-intro-python-functions.ipynb)&lt;br&gt;Null Values - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/03-python/03-intro-python-null-values.ipynb)&lt;br&gt;Groupby - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/03-python/04-intro-python-groupby.ipynb)</v>
-      </c>
-      <c r="G15" s="56" t="str">
-        <f t="shared" si="5"/>
-        <v/>
+        <v>Conditional-Loops - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/03-python/01-intro-python-conditionals-loops.ipynb)&lt;br&gt;Functions - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/03-python/02-intro-python-functions.ipynb)&lt;br&gt;Null Values - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/03-python/03-intro-python-null-values.ipynb)&lt;br&gt;Groupby - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/03-python/04-intro-python-groupby.ipynb)&lt;br&gt;Kaggle Baseline - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/03-python/05-intro-kaggle-baseline.ipynb)&lt;br&gt;Assignment 2 - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/03-python/hm-02/hm02.ipynb)</v>
       </c>
       <c r="H15" s="56" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="I15" s="56" t="str">
-        <f t="shared" ref="I15:I35" si="8">I14&amp;"
-"&amp;H15</f>
-        <v xml:space="preserve">TOC entries (grouped)
+        <f t="shared" si="4"/>
+        <v xml:space="preserve">
   - title: What is Jupyter?
     url: /notebooks/01-what-is-jupyter
     not_numbered: true
@@ -48599,27 +48131,39 @@
     not_numbered: true
 </v>
       </c>
-    </row>
-    <row r="16" spans="1:9">
+      <c r="J15" s="56" t="str">
+        <f>IF(ISBLANK(C15),"",CONCATENATE("[",B15,"](",Configuration!B$29,Configuration!B$28,"/notebooks/",C15,".html)"))</f>
+        <v/>
+      </c>
+      <c r="K15" s="56" t="str">
+        <f t="shared" si="5"/>
+        <v>&lt;br&gt;&lt;br&gt;&lt;br&gt;&lt;br&gt;&lt;br&gt;</v>
+      </c>
+      <c r="L15" s="56" t="str">
+        <f t="shared" si="6"/>
+        <v>&lt;br&gt;&lt;br&gt;&lt;br&gt;&lt;br&gt;&lt;br&gt;</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12">
       <c r="A16" s="34">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B16" t="s">
-        <v>807</v>
+        <v>810</v>
       </c>
       <c r="D16" t="s">
-        <v>811</v>
+        <v>816</v>
       </c>
       <c r="E16" s="56" t="str">
-        <f t="shared" si="6"/>
-        <v>Kaggle Baseline - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/03-python/05-intro-kaggle-baseline.ipynb)</v>
+        <f t="shared" si="8"/>
+        <v>Twitter - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/04-viz-api-scraper/01_intro_api_twitter.ipynb)</v>
       </c>
       <c r="F16" s="56" t="str">
+        <f t="shared" si="1"/>
+        <v>Twitter - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/04-viz-api-scraper/01_intro_api_twitter.ipynb)</v>
+      </c>
+      <c r="G16" s="56" t="str">
         <f t="shared" si="7"/>
-        <v>Conditional-Loops - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/03-python/01-intro-python-conditionals-loops.ipynb)&lt;br&gt;Functions - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/03-python/02-intro-python-functions.ipynb)&lt;br&gt;Null Values - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/03-python/03-intro-python-null-values.ipynb)&lt;br&gt;Groupby - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/03-python/04-intro-python-groupby.ipynb)&lt;br&gt;Kaggle Baseline - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/03-python/05-intro-kaggle-baseline.ipynb)</v>
-      </c>
-      <c r="G16" s="56" t="str">
-        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="H16" s="56" t="str">
@@ -48627,8 +48171,8 @@
         <v/>
       </c>
       <c r="I16" s="56" t="str">
-        <f t="shared" si="8"/>
-        <v xml:space="preserve">TOC entries (grouped)
+        <f t="shared" si="4"/>
+        <v xml:space="preserve">
   - title: What is Jupyter?
     url: /notebooks/01-what-is-jupyter
     not_numbered: true
@@ -48655,36 +48199,48 @@
     not_numbered: true
 </v>
       </c>
-    </row>
-    <row r="17" spans="1:9">
+      <c r="J16" s="56" t="str">
+        <f>IF(ISBLANK(C16),"",CONCATENATE("[",B16,"](",Configuration!B$29,Configuration!B$28,"/notebooks/",C16,".html)"))</f>
+        <v/>
+      </c>
+      <c r="K16" s="56" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="L16" s="56" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+    </row>
+    <row r="17" spans="1:12">
       <c r="A17" s="34">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B17" t="s">
-        <v>808</v>
+        <v>811</v>
       </c>
       <c r="D17" t="s">
-        <v>812</v>
+        <v>817</v>
       </c>
       <c r="E17" s="56" t="str">
-        <f t="shared" si="6"/>
-        <v>Assignment 2 - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/03-python/hm-02/hm02.ipynb)</v>
+        <f t="shared" si="8"/>
+        <v>Web Mining - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/04-viz-api-scraper/02_intro_python_webmining.ipynb)</v>
       </c>
       <c r="F17" s="56" t="str">
+        <f t="shared" si="1"/>
+        <v>Twitter - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/04-viz-api-scraper/01_intro_api_twitter.ipynb)&lt;br&gt;Web Mining - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/04-viz-api-scraper/02_intro_python_webmining.ipynb)</v>
+      </c>
+      <c r="G17" s="56" t="str">
         <f t="shared" si="7"/>
-        <v>Conditional-Loops - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/03-python/01-intro-python-conditionals-loops.ipynb)&lt;br&gt;Functions - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/03-python/02-intro-python-functions.ipynb)&lt;br&gt;Null Values - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/03-python/03-intro-python-null-values.ipynb)&lt;br&gt;Groupby - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/03-python/04-intro-python-groupby.ipynb)&lt;br&gt;Kaggle Baseline - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/03-python/05-intro-kaggle-baseline.ipynb)&lt;br&gt;Assignment 2 - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/03-python/hm-02/hm02.ipynb)</v>
-      </c>
-      <c r="G17" s="56" t="str">
-        <f t="shared" si="5"/>
-        <v>Conditional-Loops - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/03-python/01-intro-python-conditionals-loops.ipynb)&lt;br&gt;Functions - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/03-python/02-intro-python-functions.ipynb)&lt;br&gt;Null Values - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/03-python/03-intro-python-null-values.ipynb)&lt;br&gt;Groupby - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/03-python/04-intro-python-groupby.ipynb)&lt;br&gt;Kaggle Baseline - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/03-python/05-intro-kaggle-baseline.ipynb)&lt;br&gt;Assignment 2 - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/03-python/hm-02/hm02.ipynb)</v>
+        <v/>
       </c>
       <c r="H17" s="56" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="I17" s="56" t="str">
-        <f t="shared" si="8"/>
-        <v xml:space="preserve">TOC entries (grouped)
+        <f t="shared" si="4"/>
+        <v xml:space="preserve">
   - title: What is Jupyter?
     url: /notebooks/01-what-is-jupyter
     not_numbered: true
@@ -48711,27 +48267,39 @@
     not_numbered: true
 </v>
       </c>
-    </row>
-    <row r="18" spans="1:9">
+      <c r="J17" s="56" t="str">
+        <f>IF(ISBLANK(C17),"",CONCATENATE("[",B17,"](",Configuration!B$29,Configuration!B$28,"/notebooks/",C17,".html)"))</f>
+        <v/>
+      </c>
+      <c r="K17" s="56" t="str">
+        <f t="shared" si="5"/>
+        <v>&lt;br&gt;</v>
+      </c>
+      <c r="L17" s="56" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+    </row>
+    <row r="18" spans="1:12">
       <c r="A18" s="34">
         <v>6</v>
       </c>
       <c r="B18" t="s">
-        <v>813</v>
+        <v>812</v>
       </c>
       <c r="D18" t="s">
-        <v>819</v>
+        <v>818</v>
       </c>
       <c r="E18" s="56" t="str">
-        <f t="shared" si="6"/>
-        <v>Twitter - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/04-viz-api-scraper/01_intro_api_twitter.ipynb)</v>
+        <f t="shared" si="8"/>
+        <v>Visualizations - Seaborn - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/04-viz-api-scraper/03_visualization_python_seaborn.ipynb)</v>
       </c>
       <c r="F18" s="56" t="str">
+        <f t="shared" si="1"/>
+        <v>Twitter - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/04-viz-api-scraper/01_intro_api_twitter.ipynb)&lt;br&gt;Web Mining - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/04-viz-api-scraper/02_intro_python_webmining.ipynb)&lt;br&gt;Visualizations - Seaborn - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/04-viz-api-scraper/03_visualization_python_seaborn.ipynb)</v>
+      </c>
+      <c r="G18" s="56" t="str">
         <f t="shared" si="7"/>
-        <v>Twitter - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/04-viz-api-scraper/01_intro_api_twitter.ipynb)</v>
-      </c>
-      <c r="G18" s="56" t="str">
-        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="H18" s="56" t="str">
@@ -48739,8 +48307,8 @@
         <v/>
       </c>
       <c r="I18" s="56" t="str">
-        <f t="shared" si="8"/>
-        <v xml:space="preserve">TOC entries (grouped)
+        <f t="shared" si="4"/>
+        <v xml:space="preserve">
   - title: What is Jupyter?
     url: /notebooks/01-what-is-jupyter
     not_numbered: true
@@ -48767,27 +48335,39 @@
     not_numbered: true
 </v>
       </c>
-    </row>
-    <row r="19" spans="1:9">
+      <c r="J18" s="56" t="str">
+        <f>IF(ISBLANK(C18),"",CONCATENATE("[",B18,"](",Configuration!B$29,Configuration!B$28,"/notebooks/",C18,".html)"))</f>
+        <v/>
+      </c>
+      <c r="K18" s="56" t="str">
+        <f t="shared" si="5"/>
+        <v>&lt;br&gt;&lt;br&gt;</v>
+      </c>
+      <c r="L18" s="56" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+    </row>
+    <row r="19" spans="1:12">
       <c r="A19" s="34">
         <v>6</v>
       </c>
       <c r="B19" t="s">
-        <v>814</v>
+        <v>813</v>
       </c>
       <c r="D19" t="s">
-        <v>820</v>
+        <v>819</v>
       </c>
       <c r="E19" s="56" t="str">
-        <f t="shared" si="6"/>
-        <v>Web Mining - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/04-viz-api-scraper/02_intro_python_webmining.ipynb)</v>
+        <f t="shared" si="8"/>
+        <v>Strings - Regular Expressions - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/04-viz-api-scraper/04_strings_and_regular_expressions.ipynb)</v>
       </c>
       <c r="F19" s="56" t="str">
+        <f t="shared" si="1"/>
+        <v>Twitter - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/04-viz-api-scraper/01_intro_api_twitter.ipynb)&lt;br&gt;Web Mining - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/04-viz-api-scraper/02_intro_python_webmining.ipynb)&lt;br&gt;Visualizations - Seaborn - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/04-viz-api-scraper/03_visualization_python_seaborn.ipynb)&lt;br&gt;Strings - Regular Expressions - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/04-viz-api-scraper/04_strings_and_regular_expressions.ipynb)</v>
+      </c>
+      <c r="G19" s="56" t="str">
         <f t="shared" si="7"/>
-        <v>Twitter - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/04-viz-api-scraper/01_intro_api_twitter.ipynb)&lt;br&gt;Web Mining - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/04-viz-api-scraper/02_intro_python_webmining.ipynb)</v>
-      </c>
-      <c r="G19" s="56" t="str">
-        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="H19" s="56" t="str">
@@ -48795,8 +48375,8 @@
         <v/>
       </c>
       <c r="I19" s="56" t="str">
-        <f t="shared" si="8"/>
-        <v xml:space="preserve">TOC entries (grouped)
+        <f t="shared" si="4"/>
+        <v xml:space="preserve">
   - title: What is Jupyter?
     url: /notebooks/01-what-is-jupyter
     not_numbered: true
@@ -48823,27 +48403,39 @@
     not_numbered: true
 </v>
       </c>
-    </row>
-    <row r="20" spans="1:9">
+      <c r="J19" s="56" t="str">
+        <f>IF(ISBLANK(C19),"",CONCATENATE("[",B19,"](",Configuration!B$29,Configuration!B$28,"/notebooks/",C19,".html)"))</f>
+        <v/>
+      </c>
+      <c r="K19" s="56" t="str">
+        <f t="shared" si="5"/>
+        <v>&lt;br&gt;&lt;br&gt;&lt;br&gt;</v>
+      </c>
+      <c r="L19" s="56" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+    </row>
+    <row r="20" spans="1:12">
       <c r="A20" s="34">
         <v>6</v>
       </c>
       <c r="B20" t="s">
-        <v>815</v>
+        <v>814</v>
       </c>
       <c r="D20" t="s">
-        <v>821</v>
+        <v>820</v>
       </c>
       <c r="E20" s="56" t="str">
-        <f t="shared" si="6"/>
-        <v>Visualizations - Seaborn - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/04-viz-api-scraper/03_visualization_python_seaborn.ipynb)</v>
+        <f t="shared" si="8"/>
+        <v>Feature Dummies - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/04-viz-api-scraper/05_features_dummies.ipynb)</v>
       </c>
       <c r="F20" s="56" t="str">
+        <f t="shared" si="1"/>
+        <v>Twitter - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/04-viz-api-scraper/01_intro_api_twitter.ipynb)&lt;br&gt;Web Mining - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/04-viz-api-scraper/02_intro_python_webmining.ipynb)&lt;br&gt;Visualizations - Seaborn - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/04-viz-api-scraper/03_visualization_python_seaborn.ipynb)&lt;br&gt;Strings - Regular Expressions - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/04-viz-api-scraper/04_strings_and_regular_expressions.ipynb)&lt;br&gt;Feature Dummies - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/04-viz-api-scraper/05_features_dummies.ipynb)</v>
+      </c>
+      <c r="G20" s="56" t="str">
         <f t="shared" si="7"/>
-        <v>Twitter - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/04-viz-api-scraper/01_intro_api_twitter.ipynb)&lt;br&gt;Web Mining - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/04-viz-api-scraper/02_intro_python_webmining.ipynb)&lt;br&gt;Visualizations - Seaborn - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/04-viz-api-scraper/03_visualization_python_seaborn.ipynb)</v>
-      </c>
-      <c r="G20" s="56" t="str">
-        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="H20" s="56" t="str">
@@ -48851,8 +48443,8 @@
         <v/>
       </c>
       <c r="I20" s="56" t="str">
-        <f t="shared" si="8"/>
-        <v xml:space="preserve">TOC entries (grouped)
+        <f t="shared" si="4"/>
+        <v xml:space="preserve">
   - title: What is Jupyter?
     url: /notebooks/01-what-is-jupyter
     not_numbered: true
@@ -48879,36 +48471,48 @@
     not_numbered: true
 </v>
       </c>
-    </row>
-    <row r="21" spans="1:9">
+      <c r="J20" s="56" t="str">
+        <f>IF(ISBLANK(C20),"",CONCATENATE("[",B20,"](",Configuration!B$29,Configuration!B$28,"/notebooks/",C20,".html)"))</f>
+        <v/>
+      </c>
+      <c r="K20" s="56" t="str">
+        <f t="shared" si="5"/>
+        <v>&lt;br&gt;&lt;br&gt;&lt;br&gt;&lt;br&gt;</v>
+      </c>
+      <c r="L20" s="56" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+    </row>
+    <row r="21" spans="1:12">
       <c r="A21" s="34">
         <v>6</v>
       </c>
       <c r="B21" t="s">
-        <v>816</v>
+        <v>815</v>
       </c>
       <c r="D21" t="s">
-        <v>822</v>
+        <v>821</v>
       </c>
       <c r="E21" s="56" t="str">
-        <f t="shared" si="6"/>
-        <v>Strings - Regular Expressions - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/04-viz-api-scraper/04_strings_and_regular_expressions.ipynb)</v>
+        <f t="shared" si="8"/>
+        <v>Assignment 3 - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/04-viz-api-scraper/hm-03/hm03.ipynb)</v>
       </c>
       <c r="F21" s="56" t="str">
+        <f t="shared" si="1"/>
+        <v>Twitter - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/04-viz-api-scraper/01_intro_api_twitter.ipynb)&lt;br&gt;Web Mining - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/04-viz-api-scraper/02_intro_python_webmining.ipynb)&lt;br&gt;Visualizations - Seaborn - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/04-viz-api-scraper/03_visualization_python_seaborn.ipynb)&lt;br&gt;Strings - Regular Expressions - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/04-viz-api-scraper/04_strings_and_regular_expressions.ipynb)&lt;br&gt;Feature Dummies - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/04-viz-api-scraper/05_features_dummies.ipynb)&lt;br&gt;Assignment 3 - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/04-viz-api-scraper/hm-03/hm03.ipynb)</v>
+      </c>
+      <c r="G21" s="56" t="str">
         <f t="shared" si="7"/>
-        <v>Twitter - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/04-viz-api-scraper/01_intro_api_twitter.ipynb)&lt;br&gt;Web Mining - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/04-viz-api-scraper/02_intro_python_webmining.ipynb)&lt;br&gt;Visualizations - Seaborn - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/04-viz-api-scraper/03_visualization_python_seaborn.ipynb)&lt;br&gt;Strings - Regular Expressions - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/04-viz-api-scraper/04_strings_and_regular_expressions.ipynb)</v>
-      </c>
-      <c r="G21" s="56" t="str">
-        <f t="shared" si="5"/>
-        <v/>
+        <v>Twitter - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/04-viz-api-scraper/01_intro_api_twitter.ipynb)&lt;br&gt;Web Mining - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/04-viz-api-scraper/02_intro_python_webmining.ipynb)&lt;br&gt;Visualizations - Seaborn - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/04-viz-api-scraper/03_visualization_python_seaborn.ipynb)&lt;br&gt;Strings - Regular Expressions - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/04-viz-api-scraper/04_strings_and_regular_expressions.ipynb)&lt;br&gt;Feature Dummies - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/04-viz-api-scraper/05_features_dummies.ipynb)&lt;br&gt;Assignment 3 - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/04-viz-api-scraper/hm-03/hm03.ipynb)</v>
       </c>
       <c r="H21" s="56" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="I21" s="56" t="str">
-        <f t="shared" si="8"/>
-        <v xml:space="preserve">TOC entries (grouped)
+        <f t="shared" si="4"/>
+        <v xml:space="preserve">
   - title: What is Jupyter?
     url: /notebooks/01-what-is-jupyter
     not_numbered: true
@@ -48935,27 +48539,39 @@
     not_numbered: true
 </v>
       </c>
-    </row>
-    <row r="22" spans="1:9">
+      <c r="J21" s="56" t="str">
+        <f>IF(ISBLANK(C21),"",CONCATENATE("[",B21,"](",Configuration!B$29,Configuration!B$28,"/notebooks/",C21,".html)"))</f>
+        <v/>
+      </c>
+      <c r="K21" s="56" t="str">
+        <f t="shared" si="5"/>
+        <v>&lt;br&gt;&lt;br&gt;&lt;br&gt;&lt;br&gt;&lt;br&gt;</v>
+      </c>
+      <c r="L21" s="56" t="str">
+        <f t="shared" si="6"/>
+        <v>&lt;br&gt;&lt;br&gt;&lt;br&gt;&lt;br&gt;&lt;br&gt;</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12">
       <c r="A22" s="34">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B22" t="s">
-        <v>817</v>
+        <v>822</v>
       </c>
       <c r="D22" t="s">
-        <v>823</v>
+        <v>835</v>
       </c>
       <c r="E22" s="56" t="str">
-        <f t="shared" si="6"/>
-        <v>Feature Dummies - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/04-viz-api-scraper/05_features_dummies.ipynb)</v>
+        <f t="shared" si="8"/>
+        <v>The Simplest Neural Network with Numpy - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/05-intro-modeling/01-Neural-Networks.ipynb)</v>
       </c>
       <c r="F22" s="56" t="str">
+        <f t="shared" si="1"/>
+        <v>The Simplest Neural Network with Numpy - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/05-intro-modeling/01-Neural-Networks.ipynb)</v>
+      </c>
+      <c r="G22" s="56" t="str">
         <f t="shared" si="7"/>
-        <v>Twitter - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/04-viz-api-scraper/01_intro_api_twitter.ipynb)&lt;br&gt;Web Mining - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/04-viz-api-scraper/02_intro_python_webmining.ipynb)&lt;br&gt;Visualizations - Seaborn - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/04-viz-api-scraper/03_visualization_python_seaborn.ipynb)&lt;br&gt;Strings - Regular Expressions - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/04-viz-api-scraper/04_strings_and_regular_expressions.ipynb)&lt;br&gt;Feature Dummies - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/04-viz-api-scraper/05_features_dummies.ipynb)</v>
-      </c>
-      <c r="G22" s="56" t="str">
-        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="H22" s="56" t="str">
@@ -48963,8 +48579,8 @@
         <v/>
       </c>
       <c r="I22" s="56" t="str">
-        <f t="shared" si="8"/>
-        <v xml:space="preserve">TOC entries (grouped)
+        <f t="shared" si="4"/>
+        <v xml:space="preserve">
   - title: What is Jupyter?
     url: /notebooks/01-what-is-jupyter
     not_numbered: true
@@ -48991,36 +48607,48 @@
     not_numbered: true
 </v>
       </c>
-    </row>
-    <row r="23" spans="1:9">
+      <c r="J22" s="56" t="str">
+        <f>IF(ISBLANK(C22),"",CONCATENATE("[",B22,"](",Configuration!B$29,Configuration!B$28,"/notebooks/",C22,".html)"))</f>
+        <v/>
+      </c>
+      <c r="K22" s="56" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="L22" s="56" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+    </row>
+    <row r="23" spans="1:12">
       <c r="A23" s="34">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B23" t="s">
-        <v>818</v>
+        <v>823</v>
       </c>
       <c r="D23" t="s">
-        <v>824</v>
+        <v>834</v>
       </c>
       <c r="E23" s="56" t="str">
-        <f t="shared" si="6"/>
-        <v>Assignment 3 - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/04-viz-api-scraper/hm-03/hm03.ipynb)</v>
+        <f t="shared" si="8"/>
+        <v>Train Test Split - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/05-intro-modeling/01-training-test-split.ipynb)</v>
       </c>
       <c r="F23" s="56" t="str">
+        <f t="shared" si="1"/>
+        <v>The Simplest Neural Network with Numpy - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/05-intro-modeling/01-Neural-Networks.ipynb)&lt;br&gt;Train Test Split - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/05-intro-modeling/01-training-test-split.ipynb)</v>
+      </c>
+      <c r="G23" s="56" t="str">
         <f t="shared" si="7"/>
-        <v>Twitter - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/04-viz-api-scraper/01_intro_api_twitter.ipynb)&lt;br&gt;Web Mining - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/04-viz-api-scraper/02_intro_python_webmining.ipynb)&lt;br&gt;Visualizations - Seaborn - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/04-viz-api-scraper/03_visualization_python_seaborn.ipynb)&lt;br&gt;Strings - Regular Expressions - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/04-viz-api-scraper/04_strings_and_regular_expressions.ipynb)&lt;br&gt;Feature Dummies - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/04-viz-api-scraper/05_features_dummies.ipynb)&lt;br&gt;Assignment 3 - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/04-viz-api-scraper/hm-03/hm03.ipynb)</v>
-      </c>
-      <c r="G23" s="56" t="str">
-        <f t="shared" si="5"/>
-        <v>Twitter - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/04-viz-api-scraper/01_intro_api_twitter.ipynb)&lt;br&gt;Web Mining - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/04-viz-api-scraper/02_intro_python_webmining.ipynb)&lt;br&gt;Visualizations - Seaborn - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/04-viz-api-scraper/03_visualization_python_seaborn.ipynb)&lt;br&gt;Strings - Regular Expressions - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/04-viz-api-scraper/04_strings_and_regular_expressions.ipynb)&lt;br&gt;Feature Dummies - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/04-viz-api-scraper/05_features_dummies.ipynb)&lt;br&gt;Assignment 3 - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/04-viz-api-scraper/hm-03/hm03.ipynb)</v>
+        <v/>
       </c>
       <c r="H23" s="56" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="I23" s="56" t="str">
-        <f t="shared" si="8"/>
-        <v xml:space="preserve">TOC entries (grouped)
+        <f t="shared" si="4"/>
+        <v xml:space="preserve">
   - title: What is Jupyter?
     url: /notebooks/01-what-is-jupyter
     not_numbered: true
@@ -49047,27 +48675,39 @@
     not_numbered: true
 </v>
       </c>
-    </row>
-    <row r="24" spans="1:9">
+      <c r="J23" s="56" t="str">
+        <f>IF(ISBLANK(C23),"",CONCATENATE("[",B23,"](",Configuration!B$29,Configuration!B$28,"/notebooks/",C23,".html)"))</f>
+        <v/>
+      </c>
+      <c r="K23" s="56" t="str">
+        <f t="shared" si="5"/>
+        <v>&lt;br&gt;</v>
+      </c>
+      <c r="L23" s="56" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+    </row>
+    <row r="24" spans="1:12">
       <c r="A24" s="34">
         <v>9</v>
       </c>
       <c r="B24" t="s">
-        <v>825</v>
+        <v>824</v>
       </c>
       <c r="D24" t="s">
-        <v>838</v>
+        <v>833</v>
       </c>
       <c r="E24" s="56" t="str">
-        <f t="shared" si="6"/>
-        <v>The Simplest Neural Network with Numpy - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/05-intro-modeling/01-Neural-Networks.ipynb)</v>
+        <f t="shared" si="8"/>
+        <v>Introduction to Logistic Regression - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/05-intro-modeling/02-intro-logistic-knn.ipynb)</v>
       </c>
       <c r="F24" s="56" t="str">
+        <f t="shared" si="1"/>
+        <v>The Simplest Neural Network with Numpy - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/05-intro-modeling/01-Neural-Networks.ipynb)&lt;br&gt;Train Test Split - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/05-intro-modeling/01-training-test-split.ipynb)&lt;br&gt;Introduction to Logistic Regression - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/05-intro-modeling/02-intro-logistic-knn.ipynb)</v>
+      </c>
+      <c r="G24" s="56" t="str">
         <f t="shared" si="7"/>
-        <v>The Simplest Neural Network with Numpy - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/05-intro-modeling/01-Neural-Networks.ipynb)</v>
-      </c>
-      <c r="G24" s="56" t="str">
-        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="H24" s="56" t="str">
@@ -49075,8 +48715,8 @@
         <v/>
       </c>
       <c r="I24" s="56" t="str">
-        <f t="shared" si="8"/>
-        <v xml:space="preserve">TOC entries (grouped)
+        <f t="shared" si="4"/>
+        <v xml:space="preserve">
   - title: What is Jupyter?
     url: /notebooks/01-what-is-jupyter
     not_numbered: true
@@ -49103,27 +48743,39 @@
     not_numbered: true
 </v>
       </c>
-    </row>
-    <row r="25" spans="1:9">
+      <c r="J24" s="56" t="str">
+        <f>IF(ISBLANK(C24),"",CONCATENATE("[",B24,"](",Configuration!B$29,Configuration!B$28,"/notebooks/",C24,".html)"))</f>
+        <v/>
+      </c>
+      <c r="K24" s="56" t="str">
+        <f t="shared" si="5"/>
+        <v>&lt;br&gt;&lt;br&gt;</v>
+      </c>
+      <c r="L24" s="56" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+    </row>
+    <row r="25" spans="1:12">
       <c r="A25" s="34">
         <v>9</v>
       </c>
       <c r="B25" t="s">
-        <v>826</v>
+        <v>825</v>
       </c>
       <c r="D25" t="s">
-        <v>837</v>
+        <v>832</v>
       </c>
       <c r="E25" s="56" t="str">
-        <f t="shared" si="6"/>
-        <v>Train Test Split - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/05-intro-modeling/01-training-test-split.ipynb)</v>
+        <f t="shared" si="8"/>
+        <v>K Nearest Neighbor - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/05-intro-modeling/03-knn.ipynb)</v>
       </c>
       <c r="F25" s="56" t="str">
+        <f t="shared" si="1"/>
+        <v>The Simplest Neural Network with Numpy - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/05-intro-modeling/01-Neural-Networks.ipynb)&lt;br&gt;Train Test Split - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/05-intro-modeling/01-training-test-split.ipynb)&lt;br&gt;Introduction to Logistic Regression - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/05-intro-modeling/02-intro-logistic-knn.ipynb)&lt;br&gt;K Nearest Neighbor - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/05-intro-modeling/03-knn.ipynb)</v>
+      </c>
+      <c r="G25" s="56" t="str">
         <f t="shared" si="7"/>
-        <v>The Simplest Neural Network with Numpy - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/05-intro-modeling/01-Neural-Networks.ipynb)&lt;br&gt;Train Test Split - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/05-intro-modeling/01-training-test-split.ipynb)</v>
-      </c>
-      <c r="G25" s="56" t="str">
-        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="H25" s="56" t="str">
@@ -49131,8 +48783,8 @@
         <v/>
       </c>
       <c r="I25" s="56" t="str">
-        <f t="shared" si="8"/>
-        <v xml:space="preserve">TOC entries (grouped)
+        <f t="shared" si="4"/>
+        <v xml:space="preserve">
   - title: What is Jupyter?
     url: /notebooks/01-what-is-jupyter
     not_numbered: true
@@ -49159,27 +48811,39 @@
     not_numbered: true
 </v>
       </c>
-    </row>
-    <row r="26" spans="1:9">
+      <c r="J25" s="56" t="str">
+        <f>IF(ISBLANK(C25),"",CONCATENATE("[",B25,"](",Configuration!B$29,Configuration!B$28,"/notebooks/",C25,".html)"))</f>
+        <v/>
+      </c>
+      <c r="K25" s="56" t="str">
+        <f t="shared" si="5"/>
+        <v>&lt;br&gt;&lt;br&gt;&lt;br&gt;</v>
+      </c>
+      <c r="L25" s="56" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+    </row>
+    <row r="26" spans="1:12">
       <c r="A26" s="34">
         <v>9</v>
       </c>
       <c r="B26" t="s">
-        <v>827</v>
+        <v>826</v>
       </c>
       <c r="D26" t="s">
-        <v>836</v>
+        <v>831</v>
       </c>
       <c r="E26" s="56" t="str">
-        <f t="shared" si="6"/>
-        <v>Introduction to Logistic Regression - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/05-intro-modeling/02-intro-logistic-knn.ipynb)</v>
+        <f t="shared" si="8"/>
+        <v>ROC and SVM - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/05-intro-modeling/04-svm-roc.ipynb)</v>
       </c>
       <c r="F26" s="56" t="str">
+        <f t="shared" si="1"/>
+        <v>The Simplest Neural Network with Numpy - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/05-intro-modeling/01-Neural-Networks.ipynb)&lt;br&gt;Train Test Split - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/05-intro-modeling/01-training-test-split.ipynb)&lt;br&gt;Introduction to Logistic Regression - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/05-intro-modeling/02-intro-logistic-knn.ipynb)&lt;br&gt;K Nearest Neighbor - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/05-intro-modeling/03-knn.ipynb)&lt;br&gt;ROC and SVM - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/05-intro-modeling/04-svm-roc.ipynb)</v>
+      </c>
+      <c r="G26" s="56" t="str">
         <f t="shared" si="7"/>
-        <v>The Simplest Neural Network with Numpy - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/05-intro-modeling/01-Neural-Networks.ipynb)&lt;br&gt;Train Test Split - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/05-intro-modeling/01-training-test-split.ipynb)&lt;br&gt;Introduction to Logistic Regression - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/05-intro-modeling/02-intro-logistic-knn.ipynb)</v>
-      </c>
-      <c r="G26" s="56" t="str">
-        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="H26" s="56" t="str">
@@ -49187,8 +48851,8 @@
         <v/>
       </c>
       <c r="I26" s="56" t="str">
-        <f t="shared" si="8"/>
-        <v xml:space="preserve">TOC entries (grouped)
+        <f t="shared" si="4"/>
+        <v xml:space="preserve">
   - title: What is Jupyter?
     url: /notebooks/01-what-is-jupyter
     not_numbered: true
@@ -49215,27 +48879,39 @@
     not_numbered: true
 </v>
       </c>
-    </row>
-    <row r="27" spans="1:9">
+      <c r="J26" s="56" t="str">
+        <f>IF(ISBLANK(C26),"",CONCATENATE("[",B26,"](",Configuration!B$29,Configuration!B$28,"/notebooks/",C26,".html)"))</f>
+        <v/>
+      </c>
+      <c r="K26" s="56" t="str">
+        <f t="shared" si="5"/>
+        <v>&lt;br&gt;&lt;br&gt;&lt;br&gt;&lt;br&gt;</v>
+      </c>
+      <c r="L26" s="56" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+    </row>
+    <row r="27" spans="1:12">
       <c r="A27" s="34">
         <v>9</v>
       </c>
       <c r="B27" t="s">
-        <v>828</v>
+        <v>827</v>
       </c>
       <c r="D27" t="s">
-        <v>835</v>
+        <v>830</v>
       </c>
       <c r="E27" s="56" t="str">
-        <f t="shared" si="6"/>
-        <v>K Nearest Neighbor - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/05-intro-modeling/03-knn.ipynb)</v>
+        <f t="shared" si="8"/>
+        <v>HM5A Visualization &amp; Screen Scraping - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/05-intro-modeling/hm5/homework_05A.ipynb)</v>
       </c>
       <c r="F27" s="56" t="str">
+        <f t="shared" si="1"/>
+        <v>The Simplest Neural Network with Numpy - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/05-intro-modeling/01-Neural-Networks.ipynb)&lt;br&gt;Train Test Split - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/05-intro-modeling/01-training-test-split.ipynb)&lt;br&gt;Introduction to Logistic Regression - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/05-intro-modeling/02-intro-logistic-knn.ipynb)&lt;br&gt;K Nearest Neighbor - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/05-intro-modeling/03-knn.ipynb)&lt;br&gt;ROC and SVM - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/05-intro-modeling/04-svm-roc.ipynb)&lt;br&gt;HM5A Visualization &amp; Screen Scraping - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/05-intro-modeling/hm5/homework_05A.ipynb)</v>
+      </c>
+      <c r="G27" s="56" t="str">
         <f t="shared" si="7"/>
-        <v>The Simplest Neural Network with Numpy - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/05-intro-modeling/01-Neural-Networks.ipynb)&lt;br&gt;Train Test Split - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/05-intro-modeling/01-training-test-split.ipynb)&lt;br&gt;Introduction to Logistic Regression - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/05-intro-modeling/02-intro-logistic-knn.ipynb)&lt;br&gt;K Nearest Neighbor - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/05-intro-modeling/03-knn.ipynb)</v>
-      </c>
-      <c r="G27" s="56" t="str">
-        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="H27" s="56" t="str">
@@ -49243,8 +48919,8 @@
         <v/>
       </c>
       <c r="I27" s="56" t="str">
-        <f t="shared" si="8"/>
-        <v xml:space="preserve">TOC entries (grouped)
+        <f t="shared" si="4"/>
+        <v xml:space="preserve">
   - title: What is Jupyter?
     url: /notebooks/01-what-is-jupyter
     not_numbered: true
@@ -49271,36 +48947,48 @@
     not_numbered: true
 </v>
       </c>
-    </row>
-    <row r="28" spans="1:9">
+      <c r="J27" s="56" t="str">
+        <f>IF(ISBLANK(C27),"",CONCATENATE("[",B27,"](",Configuration!B$29,Configuration!B$28,"/notebooks/",C27,".html)"))</f>
+        <v/>
+      </c>
+      <c r="K27" s="56" t="str">
+        <f t="shared" si="5"/>
+        <v>&lt;br&gt;&lt;br&gt;&lt;br&gt;&lt;br&gt;&lt;br&gt;</v>
+      </c>
+      <c r="L27" s="56" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+    </row>
+    <row r="28" spans="1:12">
       <c r="A28" s="34">
         <v>9</v>
       </c>
       <c r="B28" t="s">
+        <v>828</v>
+      </c>
+      <c r="D28" t="s">
         <v>829</v>
       </c>
-      <c r="D28" t="s">
-        <v>834</v>
-      </c>
       <c r="E28" s="56" t="str">
-        <f t="shared" si="6"/>
-        <v>ROC and SVM - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/05-intro-modeling/04-svm-roc.ipynb)</v>
+        <f t="shared" si="8"/>
+        <v>HM5B Intro Modeling - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/05-intro-modeling/hm5/homework_05B.ipynb)</v>
       </c>
       <c r="F28" s="56" t="str">
+        <f t="shared" si="1"/>
+        <v>The Simplest Neural Network with Numpy - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/05-intro-modeling/01-Neural-Networks.ipynb)&lt;br&gt;Train Test Split - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/05-intro-modeling/01-training-test-split.ipynb)&lt;br&gt;Introduction to Logistic Regression - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/05-intro-modeling/02-intro-logistic-knn.ipynb)&lt;br&gt;K Nearest Neighbor - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/05-intro-modeling/03-knn.ipynb)&lt;br&gt;ROC and SVM - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/05-intro-modeling/04-svm-roc.ipynb)&lt;br&gt;HM5A Visualization &amp; Screen Scraping - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/05-intro-modeling/hm5/homework_05A.ipynb)&lt;br&gt;HM5B Intro Modeling - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/05-intro-modeling/hm5/homework_05B.ipynb)</v>
+      </c>
+      <c r="G28" s="56" t="str">
         <f t="shared" si="7"/>
-        <v>The Simplest Neural Network with Numpy - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/05-intro-modeling/01-Neural-Networks.ipynb)&lt;br&gt;Train Test Split - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/05-intro-modeling/01-training-test-split.ipynb)&lt;br&gt;Introduction to Logistic Regression - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/05-intro-modeling/02-intro-logistic-knn.ipynb)&lt;br&gt;K Nearest Neighbor - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/05-intro-modeling/03-knn.ipynb)&lt;br&gt;ROC and SVM - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/05-intro-modeling/04-svm-roc.ipynb)</v>
-      </c>
-      <c r="G28" s="56" t="str">
-        <f t="shared" si="5"/>
-        <v/>
+        <v>The Simplest Neural Network with Numpy - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/05-intro-modeling/01-Neural-Networks.ipynb)&lt;br&gt;Train Test Split - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/05-intro-modeling/01-training-test-split.ipynb)&lt;br&gt;Introduction to Logistic Regression - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/05-intro-modeling/02-intro-logistic-knn.ipynb)&lt;br&gt;K Nearest Neighbor - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/05-intro-modeling/03-knn.ipynb)&lt;br&gt;ROC and SVM - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/05-intro-modeling/04-svm-roc.ipynb)&lt;br&gt;HM5A Visualization &amp; Screen Scraping - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/05-intro-modeling/hm5/homework_05A.ipynb)&lt;br&gt;HM5B Intro Modeling - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/05-intro-modeling/hm5/homework_05B.ipynb)</v>
       </c>
       <c r="H28" s="56" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="I28" s="56" t="str">
-        <f t="shared" si="8"/>
-        <v xml:space="preserve">TOC entries (grouped)
+        <f t="shared" si="4"/>
+        <v xml:space="preserve">
   - title: What is Jupyter?
     url: /notebooks/01-what-is-jupyter
     not_numbered: true
@@ -49327,27 +49015,39 @@
     not_numbered: true
 </v>
       </c>
-    </row>
-    <row r="29" spans="1:9">
+      <c r="J28" s="56" t="str">
+        <f>IF(ISBLANK(C28),"",CONCATENATE("[",B28,"](",Configuration!B$29,Configuration!B$28,"/notebooks/",C28,".html)"))</f>
+        <v/>
+      </c>
+      <c r="K28" s="56" t="str">
+        <f t="shared" si="5"/>
+        <v>&lt;br&gt;&lt;br&gt;&lt;br&gt;&lt;br&gt;&lt;br&gt;&lt;br&gt;</v>
+      </c>
+      <c r="L28" s="56" t="str">
+        <f t="shared" si="6"/>
+        <v>&lt;br&gt;&lt;br&gt;&lt;br&gt;&lt;br&gt;&lt;br&gt;&lt;br&gt;</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12">
       <c r="A29" s="34">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="B29" t="s">
-        <v>830</v>
+        <v>836</v>
       </c>
       <c r="D29" t="s">
-        <v>833</v>
+        <v>839</v>
       </c>
       <c r="E29" s="56" t="str">
-        <f t="shared" si="6"/>
-        <v>HM5A Visualization &amp; Screen Scraping - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/05-intro-modeling/hm5/homework_05A.ipynb)</v>
+        <f t="shared" si="8"/>
+        <v>Matrix Regression - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/07-intro-modeling2/Python/01-matrix-regression-gradient-decent-python.ipynb)</v>
       </c>
       <c r="F29" s="56" t="str">
+        <f t="shared" si="1"/>
+        <v>Matrix Regression - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/07-intro-modeling2/Python/01-matrix-regression-gradient-decent-python.ipynb)</v>
+      </c>
+      <c r="G29" s="56" t="str">
         <f t="shared" si="7"/>
-        <v>The Simplest Neural Network with Numpy - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/05-intro-modeling/01-Neural-Networks.ipynb)&lt;br&gt;Train Test Split - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/05-intro-modeling/01-training-test-split.ipynb)&lt;br&gt;Introduction to Logistic Regression - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/05-intro-modeling/02-intro-logistic-knn.ipynb)&lt;br&gt;K Nearest Neighbor - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/05-intro-modeling/03-knn.ipynb)&lt;br&gt;ROC and SVM - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/05-intro-modeling/04-svm-roc.ipynb)&lt;br&gt;HM5A Visualization &amp; Screen Scraping - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/05-intro-modeling/hm5/homework_05A.ipynb)</v>
-      </c>
-      <c r="G29" s="56" t="str">
-        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="H29" s="56" t="str">
@@ -49355,8 +49055,8 @@
         <v/>
       </c>
       <c r="I29" s="56" t="str">
-        <f t="shared" si="8"/>
-        <v xml:space="preserve">TOC entries (grouped)
+        <f t="shared" si="4"/>
+        <v xml:space="preserve">
   - title: What is Jupyter?
     url: /notebooks/01-what-is-jupyter
     not_numbered: true
@@ -49383,36 +49083,48 @@
     not_numbered: true
 </v>
       </c>
-    </row>
-    <row r="30" spans="1:9">
+      <c r="J29" s="56" t="str">
+        <f>IF(ISBLANK(C29),"",CONCATENATE("[",B29,"](",Configuration!B$29,Configuration!B$28,"/notebooks/",C29,".html)"))</f>
+        <v/>
+      </c>
+      <c r="K29" s="56" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="L29" s="56" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+    </row>
+    <row r="30" spans="1:12">
       <c r="A30" s="34">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="B30" t="s">
-        <v>831</v>
+        <v>837</v>
       </c>
       <c r="D30" t="s">
-        <v>832</v>
+        <v>840</v>
       </c>
       <c r="E30" s="56" t="str">
-        <f t="shared" si="6"/>
-        <v>HM5B Intro Modeling - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/05-intro-modeling/hm5/homework_05B.ipynb)</v>
+        <f t="shared" si="8"/>
+        <v>Regression Basics - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/07-intro-modeling2/Python/02-regression-boston-housing-python.ipynb)</v>
       </c>
       <c r="F30" s="56" t="str">
+        <f t="shared" si="1"/>
+        <v>Matrix Regression - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/07-intro-modeling2/Python/01-matrix-regression-gradient-decent-python.ipynb)&lt;br&gt;Regression Basics - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/07-intro-modeling2/Python/02-regression-boston-housing-python.ipynb)</v>
+      </c>
+      <c r="G30" s="56" t="str">
         <f t="shared" si="7"/>
-        <v>The Simplest Neural Network with Numpy - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/05-intro-modeling/01-Neural-Networks.ipynb)&lt;br&gt;Train Test Split - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/05-intro-modeling/01-training-test-split.ipynb)&lt;br&gt;Introduction to Logistic Regression - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/05-intro-modeling/02-intro-logistic-knn.ipynb)&lt;br&gt;K Nearest Neighbor - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/05-intro-modeling/03-knn.ipynb)&lt;br&gt;ROC and SVM - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/05-intro-modeling/04-svm-roc.ipynb)&lt;br&gt;HM5A Visualization &amp; Screen Scraping - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/05-intro-modeling/hm5/homework_05A.ipynb)&lt;br&gt;HM5B Intro Modeling - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/05-intro-modeling/hm5/homework_05B.ipynb)</v>
-      </c>
-      <c r="G30" s="56" t="str">
-        <f t="shared" si="5"/>
-        <v>The Simplest Neural Network with Numpy - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/05-intro-modeling/01-Neural-Networks.ipynb)&lt;br&gt;Train Test Split - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/05-intro-modeling/01-training-test-split.ipynb)&lt;br&gt;Introduction to Logistic Regression - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/05-intro-modeling/02-intro-logistic-knn.ipynb)&lt;br&gt;K Nearest Neighbor - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/05-intro-modeling/03-knn.ipynb)&lt;br&gt;ROC and SVM - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/05-intro-modeling/04-svm-roc.ipynb)&lt;br&gt;HM5A Visualization &amp; Screen Scraping - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/05-intro-modeling/hm5/homework_05A.ipynb)&lt;br&gt;HM5B Intro Modeling - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/05-intro-modeling/hm5/homework_05B.ipynb)</v>
+        <v/>
       </c>
       <c r="H30" s="56" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="I30" s="56" t="str">
-        <f t="shared" si="8"/>
-        <v xml:space="preserve">TOC entries (grouped)
+        <f t="shared" si="4"/>
+        <v xml:space="preserve">
   - title: What is Jupyter?
     url: /notebooks/01-what-is-jupyter
     not_numbered: true
@@ -49439,36 +49151,48 @@
     not_numbered: true
 </v>
       </c>
-    </row>
-    <row r="31" spans="1:9">
+      <c r="J30" s="56" t="str">
+        <f>IF(ISBLANK(C30),"",CONCATENATE("[",B30,"](",Configuration!B$29,Configuration!B$28,"/notebooks/",C30,".html)"))</f>
+        <v/>
+      </c>
+      <c r="K30" s="56" t="str">
+        <f t="shared" si="5"/>
+        <v>&lt;br&gt;</v>
+      </c>
+      <c r="L30" s="56" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+    </row>
+    <row r="31" spans="1:12">
       <c r="A31" s="34">
         <v>13</v>
       </c>
       <c r="B31" t="s">
-        <v>839</v>
+        <v>838</v>
       </c>
       <c r="D31" t="s">
-        <v>842</v>
+        <v>841</v>
       </c>
       <c r="E31" s="56" t="str">
-        <f t="shared" si="6"/>
-        <v>Matrix Regression - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/07-intro-modeling2/Python/01-matrix-regression-gradient-decent-python.ipynb)</v>
+        <f t="shared" si="8"/>
+        <v>Ridge and Lasso Regression - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/07-intro-modeling2/Python/03-ridge-lasso-python.ipynb)</v>
       </c>
       <c r="F31" s="56" t="str">
+        <f t="shared" si="1"/>
+        <v>Matrix Regression - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/07-intro-modeling2/Python/01-matrix-regression-gradient-decent-python.ipynb)&lt;br&gt;Regression Basics - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/07-intro-modeling2/Python/02-regression-boston-housing-python.ipynb)&lt;br&gt;Ridge and Lasso Regression - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/07-intro-modeling2/Python/03-ridge-lasso-python.ipynb)</v>
+      </c>
+      <c r="G31" s="56" t="str">
         <f t="shared" si="7"/>
-        <v>Matrix Regression - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/07-intro-modeling2/Python/01-matrix-regression-gradient-decent-python.ipynb)</v>
-      </c>
-      <c r="G31" s="56" t="str">
-        <f t="shared" si="5"/>
-        <v/>
+        <v>Matrix Regression - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/07-intro-modeling2/Python/01-matrix-regression-gradient-decent-python.ipynb)&lt;br&gt;Regression Basics - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/07-intro-modeling2/Python/02-regression-boston-housing-python.ipynb)&lt;br&gt;Ridge and Lasso Regression - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/07-intro-modeling2/Python/03-ridge-lasso-python.ipynb)</v>
       </c>
       <c r="H31" s="56" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="I31" s="56" t="str">
-        <f t="shared" si="8"/>
-        <v xml:space="preserve">TOC entries (grouped)
+        <f t="shared" si="4"/>
+        <v xml:space="preserve">
   - title: What is Jupyter?
     url: /notebooks/01-what-is-jupyter
     not_numbered: true
@@ -49495,27 +49219,39 @@
     not_numbered: true
 </v>
       </c>
-    </row>
-    <row r="32" spans="1:9">
+      <c r="J31" s="56" t="str">
+        <f>IF(ISBLANK(C31),"",CONCATENATE("[",B31,"](",Configuration!B$29,Configuration!B$28,"/notebooks/",C31,".html)"))</f>
+        <v/>
+      </c>
+      <c r="K31" s="56" t="str">
+        <f t="shared" si="5"/>
+        <v>&lt;br&gt;&lt;br&gt;</v>
+      </c>
+      <c r="L31" s="56" t="str">
+        <f t="shared" si="6"/>
+        <v>&lt;br&gt;&lt;br&gt;</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12">
       <c r="A32" s="34">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B32" t="s">
-        <v>840</v>
+        <v>838</v>
       </c>
       <c r="D32" t="s">
-        <v>843</v>
+        <v>841</v>
       </c>
       <c r="E32" s="56" t="str">
-        <f t="shared" si="6"/>
-        <v>Regression Basics - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/07-intro-modeling2/Python/02-regression-boston-housing-python.ipynb)</v>
+        <f t="shared" si="8"/>
+        <v>Ridge and Lasso Regression - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/07-intro-modeling2/Python/03-ridge-lasso-python.ipynb)</v>
       </c>
       <c r="F32" s="56" t="str">
+        <f t="shared" si="1"/>
+        <v>Ridge and Lasso Regression - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/07-intro-modeling2/Python/03-ridge-lasso-python.ipynb)</v>
+      </c>
+      <c r="G32" s="56" t="str">
         <f t="shared" si="7"/>
-        <v>Matrix Regression - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/07-intro-modeling2/Python/01-matrix-regression-gradient-decent-python.ipynb)&lt;br&gt;Regression Basics - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/07-intro-modeling2/Python/02-regression-boston-housing-python.ipynb)</v>
-      </c>
-      <c r="G32" s="56" t="str">
-        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="H32" s="56" t="str">
@@ -49523,8 +49259,8 @@
         <v/>
       </c>
       <c r="I32" s="56" t="str">
-        <f t="shared" si="8"/>
-        <v xml:space="preserve">TOC entries (grouped)
+        <f t="shared" si="4"/>
+        <v xml:space="preserve">
   - title: What is Jupyter?
     url: /notebooks/01-what-is-jupyter
     not_numbered: true
@@ -49551,36 +49287,48 @@
     not_numbered: true
 </v>
       </c>
-    </row>
-    <row r="33" spans="1:9">
+      <c r="J32" s="56" t="str">
+        <f>IF(ISBLANK(C32),"",CONCATENATE("[",B32,"](",Configuration!B$29,Configuration!B$28,"/notebooks/",C32,".html)"))</f>
+        <v/>
+      </c>
+      <c r="K32" s="56" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="L32" s="56" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+    </row>
+    <row r="33" spans="1:12">
       <c r="A33" s="34">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B33" t="s">
-        <v>841</v>
+        <v>842</v>
       </c>
       <c r="D33" t="s">
-        <v>844</v>
+        <v>843</v>
       </c>
       <c r="E33" s="56" t="str">
-        <f t="shared" si="6"/>
-        <v>Ridge and Lasso Regression - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/07-intro-modeling2/Python/03-ridge-lasso-python.ipynb)</v>
+        <f t="shared" si="8"/>
+        <v>PCA - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/07-intro-modeling2/Python/04_introduction_pca.ipynb)</v>
       </c>
       <c r="F33" s="56" t="str">
+        <f t="shared" si="1"/>
+        <v>Ridge and Lasso Regression - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/07-intro-modeling2/Python/03-ridge-lasso-python.ipynb)&lt;br&gt;PCA - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/07-intro-modeling2/Python/04_introduction_pca.ipynb)</v>
+      </c>
+      <c r="G33" s="56" t="str">
         <f t="shared" si="7"/>
-        <v>Matrix Regression - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/07-intro-modeling2/Python/01-matrix-regression-gradient-decent-python.ipynb)&lt;br&gt;Regression Basics - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/07-intro-modeling2/Python/02-regression-boston-housing-python.ipynb)&lt;br&gt;Ridge and Lasso Regression - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/07-intro-modeling2/Python/03-ridge-lasso-python.ipynb)</v>
-      </c>
-      <c r="G33" s="56" t="str">
-        <f t="shared" si="5"/>
-        <v>Matrix Regression - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/07-intro-modeling2/Python/01-matrix-regression-gradient-decent-python.ipynb)&lt;br&gt;Regression Basics - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/07-intro-modeling2/Python/02-regression-boston-housing-python.ipynb)&lt;br&gt;Ridge and Lasso Regression - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/07-intro-modeling2/Python/03-ridge-lasso-python.ipynb)</v>
+        <v>Ridge and Lasso Regression - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/07-intro-modeling2/Python/03-ridge-lasso-python.ipynb)&lt;br&gt;PCA - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/07-intro-modeling2/Python/04_introduction_pca.ipynb)</v>
       </c>
       <c r="H33" s="56" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="I33" s="56" t="str">
-        <f t="shared" si="8"/>
-        <v xml:space="preserve">TOC entries (grouped)
+        <f t="shared" si="4"/>
+        <v xml:space="preserve">
   - title: What is Jupyter?
     url: /notebooks/01-what-is-jupyter
     not_numbered: true
@@ -49607,123 +49355,23 @@
     not_numbered: true
 </v>
       </c>
-    </row>
-    <row r="34" spans="1:9">
-      <c r="A34" s="34">
-        <v>15</v>
-      </c>
-      <c r="B34" t="s">
-        <v>841</v>
-      </c>
-      <c r="D34" t="s">
-        <v>844</v>
-      </c>
-      <c r="E34" s="56" t="str">
+      <c r="J33" s="56" t="str">
+        <f>IF(ISBLANK(C33),"",CONCATENATE("[",B33,"](",Configuration!B$29,Configuration!B$28,"/notebooks/",C33,".html)"))</f>
+        <v/>
+      </c>
+      <c r="K33" s="56" t="str">
+        <f t="shared" si="5"/>
+        <v>&lt;br&gt;</v>
+      </c>
+      <c r="L33" s="56" t="str">
         <f t="shared" si="6"/>
-        <v>Ridge and Lasso Regression - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/07-intro-modeling2/Python/03-ridge-lasso-python.ipynb)</v>
-      </c>
-      <c r="F34" s="56" t="str">
-        <f t="shared" si="7"/>
-        <v>Ridge and Lasso Regression - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/07-intro-modeling2/Python/03-ridge-lasso-python.ipynb)</v>
-      </c>
-      <c r="G34" s="56" t="str">
-        <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="H34" s="56" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="I34" s="56" t="str">
-        <f t="shared" si="8"/>
-        <v xml:space="preserve">TOC entries (grouped)
-  - title: What is Jupyter?
-    url: /notebooks/01-what-is-jupyter
-    not_numbered: true
-  - title: Notebook Basics
-    url: /notebooks/02-notebook-basics
-    not_numbered: true
-  - title: Running Code
-    url: /notebooks/03-running-code
-    not_numbered: true
-  - title: Markdown
-    url: /notebooks/04-markdown
-    not_numbered: true
-  - title: Python Overview
-    url: /notebooks/05-intro-python-overview
-    not_numbered: true
-  - title: Basic Data Structures
-    url: /notebooks/06-intro-python-datastructures
-    not_numbered: true
-  - title: Numpy
-    url: /notebooks/07-intro-python-numpy
-    not_numbered: true
-  - title: Pandas
-    url: /notebooks/08-intro-python-pandas
-    not_numbered: true
-</v>
-      </c>
-    </row>
-    <row r="35" spans="1:9">
-      <c r="A35" s="34">
-        <v>15</v>
-      </c>
-      <c r="B35" t="s">
-        <v>845</v>
-      </c>
-      <c r="D35" t="s">
-        <v>846</v>
-      </c>
-      <c r="E35" s="56" t="str">
-        <f t="shared" si="6"/>
-        <v>PCA - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/07-intro-modeling2/Python/04_introduction_pca.ipynb)</v>
-      </c>
-      <c r="F35" s="56" t="str">
-        <f t="shared" si="7"/>
-        <v>Ridge and Lasso Regression - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/07-intro-modeling2/Python/03-ridge-lasso-python.ipynb)&lt;br&gt;PCA - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/07-intro-modeling2/Python/04_introduction_pca.ipynb)</v>
-      </c>
-      <c r="G35" s="56" t="str">
-        <f>IF(A35&lt;&gt;A37,F35,"")</f>
-        <v>Ridge and Lasso Regression - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/07-intro-modeling2/Python/03-ridge-lasso-python.ipynb)&lt;br&gt;PCA - [![Open In Colab](https://colab.research.google.com/assets/colab-badge.svg)](https://colab.research.google.com/github/rpi-techfundamentals/spring2019-materials/blob/master/07-intro-modeling2/Python/04_introduction_pca.ipynb)</v>
-      </c>
-      <c r="H35" s="56" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="I35" s="56" t="str">
-        <f t="shared" si="8"/>
-        <v xml:space="preserve">TOC entries (grouped)
-  - title: What is Jupyter?
-    url: /notebooks/01-what-is-jupyter
-    not_numbered: true
-  - title: Notebook Basics
-    url: /notebooks/02-notebook-basics
-    not_numbered: true
-  - title: Running Code
-    url: /notebooks/03-running-code
-    not_numbered: true
-  - title: Markdown
-    url: /notebooks/04-markdown
-    not_numbered: true
-  - title: Python Overview
-    url: /notebooks/05-intro-python-overview
-    not_numbered: true
-  - title: Basic Data Structures
-    url: /notebooks/06-intro-python-datastructures
-    not_numbered: true
-  - title: Numpy
-    url: /notebooks/07-intro-python-numpy
-    not_numbered: true
-  - title: Pandas
-    url: /notebooks/08-intro-python-pandas
-    not_numbered: true
-</v>
-      </c>
-    </row>
-    <row r="37" spans="1:9">
-      <c r="B37" s="9"/>
-      <c r="C37" s="9"/>
-      <c r="D37" s="9"/>
+        <v>&lt;br&gt;</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12">
+      <c r="B35" s="9"/>
+      <c r="C35" s="9"/>
+      <c r="D35" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -49852,10 +49500,10 @@
       </c>
     </row>
     <row r="5" spans="1:2" ht="15.75" customHeight="1">
-      <c r="A5" s="115">
+      <c r="A5" s="118">
         <v>43709</v>
       </c>
-      <c r="B5" s="116"/>
+      <c r="B5" s="119"/>
     </row>
     <row r="6" spans="1:2" ht="15.75" customHeight="1">
       <c r="A6" s="6">
@@ -49898,10 +49546,10 @@
       </c>
     </row>
     <row r="11" spans="1:2" ht="15.75" customHeight="1">
-      <c r="A11" s="115">
+      <c r="A11" s="118">
         <v>43739</v>
       </c>
-      <c r="B11" s="116"/>
+      <c r="B11" s="119"/>
     </row>
     <row r="12" spans="1:2" ht="15.75" customHeight="1">
       <c r="A12" s="6">
@@ -49952,10 +49600,10 @@
       </c>
     </row>
     <row r="18" spans="1:2" ht="15.75" customHeight="1">
-      <c r="A18" s="115">
+      <c r="A18" s="118">
         <v>43770</v>
       </c>
-      <c r="B18" s="116"/>
+      <c r="B18" s="119"/>
     </row>
     <row r="19" spans="1:2" ht="15.75" customHeight="1">
       <c r="A19" s="8" t="s">
@@ -50022,10 +49670,10 @@
       </c>
     </row>
     <row r="27" spans="1:2" ht="15.75" customHeight="1">
-      <c r="A27" s="115">
+      <c r="A27" s="118">
         <v>43800</v>
       </c>
-      <c r="B27" s="116"/>
+      <c r="B27" s="119"/>
     </row>
     <row r="28" spans="1:2" ht="15.75" customHeight="1">
       <c r="A28" s="6">
@@ -50108,10 +49756,10 @@
       </c>
     </row>
     <row r="38" spans="1:2" ht="15.75" customHeight="1">
-      <c r="A38" s="115">
+      <c r="A38" s="118">
         <v>43831</v>
       </c>
-      <c r="B38" s="116"/>
+      <c r="B38" s="119"/>
     </row>
     <row r="39" spans="1:2" ht="15.75" customHeight="1">
       <c r="A39" s="8" t="s">
@@ -50162,10 +49810,10 @@
       </c>
     </row>
     <row r="45" spans="1:2" ht="15.75" customHeight="1">
-      <c r="A45" s="115">
+      <c r="A45" s="118">
         <v>43862</v>
       </c>
-      <c r="B45" s="116"/>
+      <c r="B45" s="119"/>
     </row>
     <row r="46" spans="1:2" ht="15.75" customHeight="1">
       <c r="A46" s="6">
@@ -50192,10 +49840,10 @@
       </c>
     </row>
     <row r="49" spans="1:2" ht="15.75" customHeight="1">
-      <c r="A49" s="115">
+      <c r="A49" s="118">
         <v>43891</v>
       </c>
-      <c r="B49" s="116"/>
+      <c r="B49" s="119"/>
     </row>
     <row r="50" spans="1:2" ht="15.75" customHeight="1">
       <c r="A50" s="6">
@@ -50270,10 +49918,10 @@
       </c>
     </row>
     <row r="59" spans="1:2" ht="15.75" customHeight="1">
-      <c r="A59" s="115">
+      <c r="A59" s="118">
         <v>43922</v>
       </c>
-      <c r="B59" s="116"/>
+      <c r="B59" s="119"/>
     </row>
     <row r="60" spans="1:2" ht="15.75" customHeight="1">
       <c r="A60" s="6">
@@ -50316,10 +49964,10 @@
       </c>
     </row>
     <row r="65" spans="1:2" ht="15.75" customHeight="1">
-      <c r="A65" s="115">
+      <c r="A65" s="118">
         <v>43952</v>
       </c>
-      <c r="B65" s="116"/>
+      <c r="B65" s="119"/>
     </row>
     <row r="66" spans="1:2" ht="15.75" customHeight="1">
       <c r="A66" s="8" t="s">
@@ -51408,7 +51056,7 @@
   <dimension ref="A1:A9"/>
   <sheetViews>
     <sheetView zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+      <selection activeCell="M4" sqref="M4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6"/>
@@ -51418,17 +51066,17 @@
   <sheetData>
     <row r="1" spans="1:1" ht="358.8">
       <c r="A1" s="30" t="s">
-        <v>868</v>
+        <v>865</v>
       </c>
     </row>
     <row r="2" spans="1:1" ht="187.2">
       <c r="A2" s="30" t="s">
-        <v>870</v>
+        <v>867</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="124.8">
       <c r="A3" s="26" t="s">
-        <v>882</v>
+        <v>879</v>
       </c>
     </row>
     <row r="4" spans="1:1" s="29" customFormat="1" ht="409.5">
@@ -51527,13 +51175,13 @@
     </row>
     <row r="5" spans="1:1" ht="78">
       <c r="A5" s="30" t="s">
-        <v>883</v>
+        <v>880</v>
       </c>
     </row>
     <row r="6" spans="1:1" s="29" customFormat="1" ht="392.7" customHeight="1">
       <c r="A6" s="71" t="str">
         <f>LOOKUP(2,1/(Notebooks!I:I&lt;&gt;""),Notebooks!I:I)</f>
-        <v xml:space="preserve">TOC entries (grouped)
+        <v xml:space="preserve">
   - title: What is Jupyter?
     url: /notebooks/01-what-is-jupyter
     not_numbered: true
@@ -51563,7 +51211,7 @@
     </row>
     <row r="7" spans="1:1" ht="78">
       <c r="A7" s="30" t="s">
-        <v>881</v>
+        <v>878</v>
       </c>
     </row>
     <row r="8" spans="1:1" s="29" customFormat="1" ht="409.5">
@@ -51581,7 +51229,7 @@
     </row>
     <row r="9" spans="1:1" ht="390">
       <c r="A9" s="31" t="s">
-        <v>871</v>
+        <v>868</v>
       </c>
     </row>
   </sheetData>
@@ -51616,16 +51264,16 @@
         <v>703</v>
       </c>
       <c r="D1" s="29" t="s">
-        <v>872</v>
+        <v>869</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="68"/>
       <c r="B2" s="68" t="s">
-        <v>898</v>
+        <v>895</v>
       </c>
       <c r="C2" s="79" t="s">
-        <v>899</v>
+        <v>896</v>
       </c>
       <c r="D2" s="29" t="b">
         <v>1</v>
@@ -52144,7 +51792,7 @@
   <sheetData>
     <row r="1" spans="1:1" ht="46.8">
       <c r="A1" s="20" t="s">
-        <v>897</v>
+        <v>894</v>
       </c>
     </row>
     <row r="2" spans="1:1" ht="409.5">

</xml_diff>

<commit_message>
Fix cells in excel sheet
</commit_message>
<xml_diff>
--- a/book.xlsx
+++ b/book.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sjgar\Documents\GitHub\course-intro-ml-app\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C3F436B-A0BC-41F4-ABE9-55730686E879}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70A3EA53-1230-4E43-9B35-DD6EC137D560}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="12504" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12696" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Configuration" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4137" uniqueCount="906">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4136" uniqueCount="906">
   <si>
     <t>Wk</t>
   </si>
@@ -3516,9 +3516,6 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
@@ -3531,29 +3528,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="5" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="27" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="27" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
     <xf numFmtId="49" fontId="5" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -3564,6 +3543,37 @@
       <alignment horizontal="center" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="27" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="27" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="164" fontId="9" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment wrapText="1"/>
@@ -3600,26 +3610,12 @@
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="166" fontId="4" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -3941,7 +3937,7 @@
   <dimension ref="A1:F55"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="B42" sqref="B42:E42"/>
+      <selection activeCell="B2" sqref="B2:E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.09765625" defaultRowHeight="15" customHeight="1"/>
@@ -3961,12 +3957,12 @@
       <c r="A2" s="29" t="s">
         <v>656</v>
       </c>
-      <c r="B2" s="97" t="s">
+      <c r="B2" s="96" t="s">
         <v>860</v>
       </c>
-      <c r="C2" s="97"/>
-      <c r="D2" s="97"/>
-      <c r="E2" s="97"/>
+      <c r="C2" s="96"/>
+      <c r="D2" s="96"/>
+      <c r="E2" s="96"/>
     </row>
     <row r="3" spans="1:5" s="4" customFormat="1" ht="15" customHeight="1">
       <c r="A3" s="9" t="s">
@@ -4005,12 +4001,12 @@
       <c r="A6" s="1" t="s">
         <v>696</v>
       </c>
-      <c r="B6" s="96">
+      <c r="B6" s="93">
         <v>14</v>
       </c>
-      <c r="C6" s="96"/>
-      <c r="D6" s="96"/>
-      <c r="E6" s="96"/>
+      <c r="C6" s="93"/>
+      <c r="D6" s="93"/>
+      <c r="E6" s="93"/>
     </row>
     <row r="7" spans="1:5" s="29" customFormat="1" ht="15" customHeight="1">
       <c r="A7" s="1"/>
@@ -4042,32 +4038,32 @@
       <c r="A10" s="1" t="s">
         <v>680</v>
       </c>
-      <c r="B10" s="96" t="s">
+      <c r="B10" s="93" t="s">
         <v>683</v>
       </c>
-      <c r="C10" s="96"/>
-      <c r="D10" s="96"/>
-      <c r="E10" s="96"/>
+      <c r="C10" s="93"/>
+      <c r="D10" s="93"/>
+      <c r="E10" s="93"/>
     </row>
     <row r="11" spans="1:5" s="29" customFormat="1" ht="15" customHeight="1">
       <c r="A11" s="1" t="s">
         <v>862</v>
       </c>
-      <c r="B11" s="96"/>
-      <c r="C11" s="96"/>
-      <c r="D11" s="96"/>
-      <c r="E11" s="96"/>
+      <c r="B11" s="93"/>
+      <c r="C11" s="93"/>
+      <c r="D11" s="93"/>
+      <c r="E11" s="93"/>
     </row>
     <row r="12" spans="1:5" s="4" customFormat="1" ht="15" customHeight="1">
       <c r="A12" s="1" t="s">
         <v>681</v>
       </c>
-      <c r="B12" s="96" t="s">
+      <c r="B12" s="93" t="s">
         <v>684</v>
       </c>
-      <c r="C12" s="96"/>
-      <c r="D12" s="96"/>
-      <c r="E12" s="96"/>
+      <c r="C12" s="93"/>
+      <c r="D12" s="93"/>
+      <c r="E12" s="93"/>
     </row>
     <row r="13" spans="1:5" s="29" customFormat="1" ht="15" customHeight="1">
       <c r="A13" s="1"/>
@@ -4077,12 +4073,12 @@
       <c r="A14" s="1" t="s">
         <v>682</v>
       </c>
-      <c r="B14" s="96" t="s">
+      <c r="B14" s="93" t="s">
         <v>685</v>
       </c>
-      <c r="C14" s="96"/>
-      <c r="D14" s="96"/>
-      <c r="E14" s="96"/>
+      <c r="C14" s="93"/>
+      <c r="D14" s="93"/>
+      <c r="E14" s="93"/>
     </row>
     <row r="15" spans="1:5" s="4" customFormat="1" ht="15" customHeight="1">
       <c r="A15" s="1" t="s">
@@ -4099,30 +4095,30 @@
       <c r="A16" s="1" t="s">
         <v>680</v>
       </c>
-      <c r="B16" s="96" t="s">
+      <c r="B16" s="93" t="s">
         <v>687</v>
       </c>
-      <c r="C16" s="96"/>
-      <c r="D16" s="96"/>
-      <c r="E16" s="96"/>
+      <c r="C16" s="93"/>
+      <c r="D16" s="93"/>
+      <c r="E16" s="93"/>
     </row>
     <row r="17" spans="1:6" s="29" customFormat="1" ht="15" customHeight="1">
       <c r="A17" s="1" t="s">
         <v>862</v>
       </c>
-      <c r="B17" s="96"/>
-      <c r="C17" s="96"/>
-      <c r="D17" s="96"/>
-      <c r="E17" s="96"/>
+      <c r="B17" s="93"/>
+      <c r="C17" s="93"/>
+      <c r="D17" s="93"/>
+      <c r="E17" s="93"/>
     </row>
     <row r="18" spans="1:6" s="29" customFormat="1" ht="15" customHeight="1">
       <c r="A18" s="1" t="s">
         <v>681</v>
       </c>
-      <c r="B18" s="96"/>
-      <c r="C18" s="96"/>
-      <c r="D18" s="96"/>
-      <c r="E18" s="96"/>
+      <c r="B18" s="93"/>
+      <c r="C18" s="93"/>
+      <c r="D18" s="93"/>
+      <c r="E18" s="93"/>
     </row>
     <row r="19" spans="1:6" s="29" customFormat="1" ht="15" customHeight="1">
       <c r="A19" s="1"/>
@@ -4132,12 +4128,12 @@
       <c r="A20" s="22" t="s">
         <v>688</v>
       </c>
-      <c r="B20" s="98" t="s">
+      <c r="B20" s="91" t="s">
         <v>689</v>
       </c>
-      <c r="C20" s="98"/>
-      <c r="D20" s="98"/>
-      <c r="E20" s="98"/>
+      <c r="C20" s="91"/>
+      <c r="D20" s="91"/>
+      <c r="E20" s="91"/>
     </row>
     <row r="21" spans="1:6" s="29" customFormat="1" ht="14.7" customHeight="1">
       <c r="A21" s="22"/>
@@ -4150,30 +4146,30 @@
       <c r="A22" s="22" t="s">
         <v>858</v>
       </c>
-      <c r="B22" s="98" t="s">
+      <c r="B22" s="91" t="s">
         <v>697</v>
       </c>
-      <c r="C22" s="98"/>
-      <c r="D22" s="98"/>
-      <c r="E22" s="98"/>
+      <c r="C22" s="91"/>
+      <c r="D22" s="91"/>
+      <c r="E22" s="91"/>
     </row>
     <row r="23" spans="1:6" s="29" customFormat="1" ht="38.1" customHeight="1">
       <c r="A23" s="22" t="s">
         <v>859</v>
       </c>
-      <c r="B23" s="99"/>
-      <c r="C23" s="99"/>
-      <c r="D23" s="99"/>
-      <c r="E23" s="99"/>
+      <c r="B23" s="92"/>
+      <c r="C23" s="92"/>
+      <c r="D23" s="92"/>
+      <c r="E23" s="92"/>
     </row>
     <row r="24" spans="1:6" s="29" customFormat="1" ht="38.1" customHeight="1">
       <c r="A24" s="22" t="s">
         <v>861</v>
       </c>
-      <c r="B24" s="99"/>
-      <c r="C24" s="99"/>
-      <c r="D24" s="99"/>
-      <c r="E24" s="99"/>
+      <c r="B24" s="92"/>
+      <c r="C24" s="92"/>
+      <c r="D24" s="92"/>
+      <c r="E24" s="92"/>
     </row>
     <row r="25" spans="1:6" s="4" customFormat="1" ht="15" customHeight="1">
       <c r="A25" s="1"/>
@@ -4238,12 +4234,12 @@
       <c r="A32" s="9" t="s">
         <v>722</v>
       </c>
-      <c r="B32" s="93" t="s">
+      <c r="B32" s="97" t="s">
         <v>18</v>
       </c>
-      <c r="C32" s="93"/>
-      <c r="D32" s="93"/>
-      <c r="E32" s="93"/>
+      <c r="C32" s="97"/>
+      <c r="D32" s="97"/>
+      <c r="E32" s="97"/>
       <c r="F32" s="14" t="s">
         <v>899</v>
       </c>
@@ -4252,12 +4248,12 @@
       <c r="A33" s="9" t="s">
         <v>669</v>
       </c>
-      <c r="B33" s="93" t="s">
+      <c r="B33" s="97" t="s">
         <v>676</v>
       </c>
-      <c r="C33" s="93"/>
-      <c r="D33" s="93"/>
-      <c r="E33" s="93"/>
+      <c r="C33" s="97"/>
+      <c r="D33" s="97"/>
+      <c r="E33" s="97"/>
       <c r="F33" s="14" t="s">
         <v>900</v>
       </c>
@@ -4280,12 +4276,12 @@
       <c r="A35" s="9" t="s">
         <v>866</v>
       </c>
-      <c r="B35" s="93" t="s">
+      <c r="B35" s="97" t="s">
         <v>670</v>
       </c>
-      <c r="C35" s="93"/>
-      <c r="D35" s="93"/>
-      <c r="E35" s="93"/>
+      <c r="C35" s="97"/>
+      <c r="D35" s="97"/>
+      <c r="E35" s="97"/>
       <c r="F35" s="14" t="s">
         <v>902</v>
       </c>
@@ -4304,12 +4300,12 @@
       <c r="A38" s="9" t="s">
         <v>709</v>
       </c>
-      <c r="B38" s="96" t="s">
+      <c r="B38" s="93" t="s">
         <v>659</v>
       </c>
-      <c r="C38" s="96"/>
-      <c r="D38" s="96"/>
-      <c r="E38" s="96"/>
+      <c r="C38" s="93"/>
+      <c r="D38" s="93"/>
+      <c r="E38" s="93"/>
     </row>
     <row r="39" spans="1:6" ht="15" customHeight="1">
       <c r="A39" s="9" t="s">
@@ -4326,12 +4322,12 @@
       <c r="A40" s="9" t="s">
         <v>710</v>
       </c>
-      <c r="B40" s="93" t="s">
+      <c r="B40" s="97" t="s">
         <v>660</v>
       </c>
-      <c r="C40" s="93"/>
-      <c r="D40" s="93"/>
-      <c r="E40" s="93"/>
+      <c r="C40" s="97"/>
+      <c r="D40" s="97"/>
+      <c r="E40" s="97"/>
     </row>
     <row r="41" spans="1:6" ht="15" customHeight="1">
       <c r="A41" s="9" t="s">
@@ -4348,12 +4344,12 @@
       <c r="A42" s="9" t="s">
         <v>711</v>
       </c>
-      <c r="B42" s="93" t="s">
+      <c r="B42" s="97" t="s">
         <v>661</v>
       </c>
-      <c r="C42" s="93"/>
-      <c r="D42" s="93"/>
-      <c r="E42" s="93"/>
+      <c r="C42" s="97"/>
+      <c r="D42" s="97"/>
+      <c r="E42" s="97"/>
     </row>
     <row r="43" spans="1:6" ht="15" customHeight="1">
       <c r="A43" s="9" t="s">
@@ -4380,7 +4376,7 @@
       </c>
     </row>
     <row r="47" spans="1:6" ht="15" customHeight="1">
-      <c r="A47" s="85" t="s">
+      <c r="A47" s="84" t="s">
         <v>715</v>
       </c>
       <c r="B47" s="80" t="s">
@@ -4388,7 +4384,7 @@
       </c>
     </row>
     <row r="48" spans="1:6" ht="15" customHeight="1">
-      <c r="A48" s="86" t="s">
+      <c r="A48" s="85" t="s">
         <v>717</v>
       </c>
       <c r="B48" s="81" t="s">
@@ -4396,7 +4392,7 @@
       </c>
     </row>
     <row r="49" spans="1:2" ht="15" customHeight="1">
-      <c r="A49" s="86" t="s">
+      <c r="A49" s="85" t="s">
         <v>718</v>
       </c>
       <c r="B49" s="81" t="s">
@@ -4404,36 +4400,59 @@
       </c>
     </row>
     <row r="50" spans="1:2" ht="15" customHeight="1">
-      <c r="A50" s="86" t="s">
+      <c r="A50" s="85" t="s">
         <v>31</v>
       </c>
-      <c r="B50" s="91" t="s">
+      <c r="B50" s="89" t="s">
         <v>716</v>
       </c>
     </row>
     <row r="51" spans="1:2" ht="15" customHeight="1">
-      <c r="A51" s="87"/>
+      <c r="A51" s="86"/>
       <c r="B51" s="82"/>
     </row>
     <row r="52" spans="1:2" ht="15" customHeight="1">
-      <c r="A52" s="87"/>
-      <c r="B52" s="92"/>
+      <c r="A52" s="86"/>
+      <c r="B52" s="90"/>
     </row>
     <row r="53" spans="1:2" ht="15" customHeight="1">
-      <c r="A53" s="87"/>
-      <c r="B53" s="92"/>
+      <c r="A53" s="86"/>
+      <c r="B53" s="90"/>
     </row>
     <row r="54" spans="1:2" ht="15" customHeight="1">
-      <c r="A54" s="88"/>
+      <c r="A54" s="87"/>
       <c r="B54" s="83"/>
     </row>
     <row r="55" spans="1:2" ht="15" customHeight="1">
-      <c r="A55" s="89"/>
-      <c r="B55" s="84"/>
+      <c r="A55" s="118"/>
+      <c r="B55" s="119"/>
     </row>
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1" insertHyperlinks="0" selectLockedCells="1"/>
   <mergeCells count="32">
+    <mergeCell ref="B40:E40"/>
+    <mergeCell ref="B41:E41"/>
+    <mergeCell ref="B42:E42"/>
+    <mergeCell ref="B43:E43"/>
+    <mergeCell ref="B32:E32"/>
+    <mergeCell ref="B33:E33"/>
+    <mergeCell ref="B34:E34"/>
+    <mergeCell ref="B35:E35"/>
+    <mergeCell ref="B27:E27"/>
+    <mergeCell ref="B28:E28"/>
+    <mergeCell ref="B29:E29"/>
+    <mergeCell ref="B38:E38"/>
+    <mergeCell ref="B39:E39"/>
+    <mergeCell ref="B6:E6"/>
+    <mergeCell ref="B5:E5"/>
+    <mergeCell ref="B4:E4"/>
+    <mergeCell ref="B3:E3"/>
+    <mergeCell ref="B2:E2"/>
+    <mergeCell ref="B12:E12"/>
+    <mergeCell ref="B11:E11"/>
+    <mergeCell ref="B10:E10"/>
+    <mergeCell ref="B9:E9"/>
+    <mergeCell ref="B8:E8"/>
     <mergeCell ref="B20:E20"/>
     <mergeCell ref="B22:E22"/>
     <mergeCell ref="B23:E23"/>
@@ -4443,29 +4462,6 @@
     <mergeCell ref="B16:E16"/>
     <mergeCell ref="B17:E17"/>
     <mergeCell ref="B18:E18"/>
-    <mergeCell ref="B12:E12"/>
-    <mergeCell ref="B11:E11"/>
-    <mergeCell ref="B10:E10"/>
-    <mergeCell ref="B9:E9"/>
-    <mergeCell ref="B8:E8"/>
-    <mergeCell ref="B6:E6"/>
-    <mergeCell ref="B5:E5"/>
-    <mergeCell ref="B4:E4"/>
-    <mergeCell ref="B3:E3"/>
-    <mergeCell ref="B2:E2"/>
-    <mergeCell ref="B27:E27"/>
-    <mergeCell ref="B28:E28"/>
-    <mergeCell ref="B29:E29"/>
-    <mergeCell ref="B38:E38"/>
-    <mergeCell ref="B39:E39"/>
-    <mergeCell ref="B40:E40"/>
-    <mergeCell ref="B41:E41"/>
-    <mergeCell ref="B42:E42"/>
-    <mergeCell ref="B43:E43"/>
-    <mergeCell ref="B32:E32"/>
-    <mergeCell ref="B33:E33"/>
-    <mergeCell ref="B34:E34"/>
-    <mergeCell ref="B35:E35"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B9" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
@@ -28500,71 +28496,71 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:22" s="32" customFormat="1" ht="18.3" customHeight="1" thickBot="1">
-      <c r="A1" s="114" t="s">
+      <c r="A1" s="100" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="112" t="s">
+      <c r="B1" s="98" t="s">
         <v>707</v>
       </c>
-      <c r="C1" s="112" t="s">
+      <c r="C1" s="98" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="103" t="s">
+      <c r="D1" s="107" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="101" t="s">
+      <c r="E1" s="105" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="105" t="s">
+      <c r="F1" s="109" t="s">
         <v>846</v>
       </c>
-      <c r="G1" s="106"/>
-      <c r="H1" s="107" t="s">
+      <c r="G1" s="110"/>
+      <c r="H1" s="111" t="s">
         <v>856</v>
       </c>
-      <c r="I1" s="108"/>
-      <c r="J1" s="108"/>
-      <c r="K1" s="109"/>
-      <c r="L1" s="110" t="s">
+      <c r="I1" s="112"/>
+      <c r="J1" s="112"/>
+      <c r="K1" s="113"/>
+      <c r="L1" s="114" t="s">
         <v>854</v>
       </c>
-      <c r="M1" s="110" t="s">
+      <c r="M1" s="114" t="s">
         <v>855</v>
       </c>
-      <c r="N1" s="116" t="s">
+      <c r="N1" s="102" t="s">
         <v>886</v>
       </c>
-      <c r="O1" s="117" t="s">
+      <c r="O1" s="103" t="s">
         <v>887</v>
       </c>
-      <c r="P1" s="100" t="s">
+      <c r="P1" s="104" t="s">
         <v>888</v>
       </c>
-      <c r="Q1" s="100" t="s">
+      <c r="Q1" s="104" t="s">
         <v>889</v>
       </c>
-      <c r="R1" s="100" t="s">
+      <c r="R1" s="104" t="s">
         <v>890</v>
       </c>
-      <c r="S1" s="100" t="s">
+      <c r="S1" s="104" t="s">
         <v>884</v>
       </c>
-      <c r="T1" s="100" t="s">
+      <c r="T1" s="104" t="s">
         <v>885</v>
       </c>
-      <c r="U1" s="100" t="s">
+      <c r="U1" s="104" t="s">
         <v>891</v>
       </c>
-      <c r="V1" s="100" t="s">
+      <c r="V1" s="104" t="s">
         <v>892</v>
       </c>
     </row>
     <row r="2" spans="1:22" s="32" customFormat="1" ht="18.899999999999999" thickTop="1" thickBot="1">
-      <c r="A2" s="115"/>
-      <c r="B2" s="113"/>
-      <c r="C2" s="113"/>
-      <c r="D2" s="104"/>
-      <c r="E2" s="102"/>
+      <c r="A2" s="101"/>
+      <c r="B2" s="99"/>
+      <c r="C2" s="99"/>
+      <c r="D2" s="108"/>
+      <c r="E2" s="106"/>
       <c r="F2" s="72" t="s">
         <v>4</v>
       </c>
@@ -28583,17 +28579,17 @@
       <c r="K2" s="77" t="s">
         <v>857</v>
       </c>
-      <c r="L2" s="111"/>
-      <c r="M2" s="111"/>
-      <c r="N2" s="116"/>
-      <c r="O2" s="117"/>
-      <c r="P2" s="100"/>
-      <c r="Q2" s="100"/>
-      <c r="R2" s="100"/>
-      <c r="S2" s="100"/>
-      <c r="T2" s="100"/>
-      <c r="U2" s="100"/>
-      <c r="V2" s="100"/>
+      <c r="L2" s="115"/>
+      <c r="M2" s="115"/>
+      <c r="N2" s="102"/>
+      <c r="O2" s="103"/>
+      <c r="P2" s="104"/>
+      <c r="Q2" s="104"/>
+      <c r="R2" s="104"/>
+      <c r="S2" s="104"/>
+      <c r="T2" s="104"/>
+      <c r="U2" s="104"/>
+      <c r="V2" s="104"/>
     </row>
     <row r="3" spans="1:22" ht="62.4">
       <c r="A3" s="42">
@@ -46493,11 +46489,12 @@
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="N1:N2"/>
-    <mergeCell ref="O1:O2"/>
+    <mergeCell ref="V1:V2"/>
+    <mergeCell ref="Q1:Q2"/>
+    <mergeCell ref="R1:R2"/>
+    <mergeCell ref="S1:S2"/>
+    <mergeCell ref="T1:T2"/>
+    <mergeCell ref="U1:U2"/>
     <mergeCell ref="P1:P2"/>
     <mergeCell ref="E1:E2"/>
     <mergeCell ref="D1:D2"/>
@@ -46505,12 +46502,11 @@
     <mergeCell ref="H1:K1"/>
     <mergeCell ref="M1:M2"/>
     <mergeCell ref="L1:L2"/>
-    <mergeCell ref="V1:V2"/>
-    <mergeCell ref="Q1:Q2"/>
-    <mergeCell ref="R1:R2"/>
-    <mergeCell ref="S1:S2"/>
-    <mergeCell ref="T1:T2"/>
-    <mergeCell ref="U1:U2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="N1:N2"/>
+    <mergeCell ref="O1:O2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -47183,7 +47179,7 @@
   <sheetViews>
     <sheetView zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I2" sqref="I2"/>
+      <selection pane="bottomLeft" activeCell="AA21" sqref="AA21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6"/>
@@ -47192,14 +47188,14 @@
     <col min="2" max="2" width="36" customWidth="1"/>
     <col min="3" max="3" width="30.3984375" style="29" customWidth="1"/>
     <col min="4" max="4" width="36" customWidth="1"/>
-    <col min="5" max="5" width="17.046875" style="56" customWidth="1"/>
-    <col min="6" max="6" width="27.25" style="56" customWidth="1"/>
-    <col min="7" max="7" width="30.84765625" style="56" customWidth="1"/>
-    <col min="8" max="8" width="13.1484375" style="56" customWidth="1"/>
-    <col min="9" max="9" width="17.046875" style="56" customWidth="1"/>
-    <col min="10" max="10" width="15.8984375" customWidth="1"/>
-    <col min="11" max="11" width="25.69921875" style="56" customWidth="1"/>
-    <col min="12" max="12" width="28.19921875" style="56" customWidth="1"/>
+    <col min="5" max="5" width="17.046875" style="56" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="27.25" style="56" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="30.84765625" style="56" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="13.1484375" style="56" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="17.046875" style="56" hidden="1" customWidth="1"/>
+    <col min="10" max="10" width="15.8984375" hidden="1" customWidth="1"/>
+    <col min="11" max="11" width="25.69921875" style="56" hidden="1" customWidth="1"/>
+    <col min="12" max="12" width="28.19921875" style="56" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" s="32" customFormat="1" ht="18.3">
@@ -47224,17 +47220,15 @@
       <c r="G1" s="55" t="s">
         <v>883</v>
       </c>
-      <c r="H1" s="55" t="s">
-        <v>884</v>
-      </c>
+      <c r="H1" s="55"/>
       <c r="I1" s="55"/>
-      <c r="J1" s="90" t="s">
+      <c r="J1" s="88" t="s">
         <v>903</v>
       </c>
-      <c r="K1" s="90" t="s">
+      <c r="K1" s="88" t="s">
         <v>904</v>
       </c>
-      <c r="L1" s="90" t="s">
+      <c r="L1" s="88" t="s">
         <v>905</v>
       </c>
     </row>
@@ -49500,10 +49494,10 @@
       </c>
     </row>
     <row r="5" spans="1:2" ht="15.75" customHeight="1">
-      <c r="A5" s="118">
+      <c r="A5" s="116">
         <v>43709</v>
       </c>
-      <c r="B5" s="119"/>
+      <c r="B5" s="117"/>
     </row>
     <row r="6" spans="1:2" ht="15.75" customHeight="1">
       <c r="A6" s="6">
@@ -49546,10 +49540,10 @@
       </c>
     </row>
     <row r="11" spans="1:2" ht="15.75" customHeight="1">
-      <c r="A11" s="118">
+      <c r="A11" s="116">
         <v>43739</v>
       </c>
-      <c r="B11" s="119"/>
+      <c r="B11" s="117"/>
     </row>
     <row r="12" spans="1:2" ht="15.75" customHeight="1">
       <c r="A12" s="6">
@@ -49600,10 +49594,10 @@
       </c>
     </row>
     <row r="18" spans="1:2" ht="15.75" customHeight="1">
-      <c r="A18" s="118">
+      <c r="A18" s="116">
         <v>43770</v>
       </c>
-      <c r="B18" s="119"/>
+      <c r="B18" s="117"/>
     </row>
     <row r="19" spans="1:2" ht="15.75" customHeight="1">
       <c r="A19" s="8" t="s">
@@ -49670,10 +49664,10 @@
       </c>
     </row>
     <row r="27" spans="1:2" ht="15.75" customHeight="1">
-      <c r="A27" s="118">
+      <c r="A27" s="116">
         <v>43800</v>
       </c>
-      <c r="B27" s="119"/>
+      <c r="B27" s="117"/>
     </row>
     <row r="28" spans="1:2" ht="15.75" customHeight="1">
       <c r="A28" s="6">
@@ -49756,10 +49750,10 @@
       </c>
     </row>
     <row r="38" spans="1:2" ht="15.75" customHeight="1">
-      <c r="A38" s="118">
+      <c r="A38" s="116">
         <v>43831</v>
       </c>
-      <c r="B38" s="119"/>
+      <c r="B38" s="117"/>
     </row>
     <row r="39" spans="1:2" ht="15.75" customHeight="1">
       <c r="A39" s="8" t="s">
@@ -49810,10 +49804,10 @@
       </c>
     </row>
     <row r="45" spans="1:2" ht="15.75" customHeight="1">
-      <c r="A45" s="118">
+      <c r="A45" s="116">
         <v>43862</v>
       </c>
-      <c r="B45" s="119"/>
+      <c r="B45" s="117"/>
     </row>
     <row r="46" spans="1:2" ht="15.75" customHeight="1">
       <c r="A46" s="6">
@@ -49840,10 +49834,10 @@
       </c>
     </row>
     <row r="49" spans="1:2" ht="15.75" customHeight="1">
-      <c r="A49" s="118">
+      <c r="A49" s="116">
         <v>43891</v>
       </c>
-      <c r="B49" s="119"/>
+      <c r="B49" s="117"/>
     </row>
     <row r="50" spans="1:2" ht="15.75" customHeight="1">
       <c r="A50" s="6">
@@ -49918,10 +49912,10 @@
       </c>
     </row>
     <row r="59" spans="1:2" ht="15.75" customHeight="1">
-      <c r="A59" s="118">
+      <c r="A59" s="116">
         <v>43922</v>
       </c>
-      <c r="B59" s="119"/>
+      <c r="B59" s="117"/>
     </row>
     <row r="60" spans="1:2" ht="15.75" customHeight="1">
       <c r="A60" s="6">
@@ -49964,10 +49958,10 @@
       </c>
     </row>
     <row r="65" spans="1:2" ht="15.75" customHeight="1">
-      <c r="A65" s="118">
+      <c r="A65" s="116">
         <v>43952</v>
       </c>
-      <c r="B65" s="119"/>
+      <c r="B65" s="117"/>
     </row>
     <row r="66" spans="1:2" ht="15.75" customHeight="1">
       <c r="A66" s="8" t="s">

</xml_diff>